<commit_message>
Auto commit at 2025-09-09 15:29:34.55
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="cdsc" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -523,7 +523,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
Auto commit at 2025-09-11  9:19:07.36
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
   <si>
     <t>电站名称</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>301号直流</t>
+  </si>
+  <si>
+    <t>B04号直流</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="179" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+    <numFmt numFmtId="177" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -217,8 +220,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -523,10 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F64"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -587,117 +591,117 @@
         <v>45906.578356481485</v>
       </c>
       <c r="E3" s="2">
-        <v>45910.311261574076</v>
+        <v>45911.324201388888</v>
       </c>
       <c r="F3">
-        <v>90</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4">
-        <v>45905.534791666665</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45909.203703703701</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>45907.567233796297</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45911.324201388888</v>
+      </c>
       <c r="F4">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4">
-        <v>45902.230208333334</v>
+        <v>45905.534791666665</v>
       </c>
       <c r="D5" s="4">
-        <v>45905.834178240744</v>
+        <v>45909.203703703701</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>45902.056701388887</v>
+        <v>45902.230208333334</v>
       </c>
       <c r="D6" s="4">
-        <v>45905.500868055555</v>
+        <v>45905.834178240744</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4">
-        <v>45905.263715277775</v>
+        <v>45902.056701388887</v>
       </c>
       <c r="D7" s="4">
-        <v>45908.553703703707</v>
+        <v>45905.500868055555</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4">
-        <v>45906.271747685183</v>
+        <v>45905.263715277775</v>
       </c>
       <c r="D8" s="4">
-        <v>45909.218194444446</v>
+        <v>45908.553703703707</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4">
-        <v>45907.567233796297</v>
-      </c>
-      <c r="E9" s="2">
-        <v>45910.311261574076</v>
-      </c>
+        <v>45906.271747685183</v>
+      </c>
+      <c r="D9" s="4">
+        <v>45909.218194444446</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -710,11 +714,12 @@
       <c r="C10" s="4">
         <v>45907.570555555554</v>
       </c>
-      <c r="E10" s="2">
-        <v>45910.311261574076</v>
-      </c>
+      <c r="D10" s="4">
+        <v>45910.500289351854</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="F10">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -722,35 +727,33 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4">
-        <v>45904.095752314817</v>
-      </c>
-      <c r="D11" s="4">
-        <v>45906.629687499997</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>45908.525706018518</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45911.324201388888</v>
+      </c>
       <c r="F11">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4">
-        <v>45906.25440972222</v>
-      </c>
-      <c r="D12" s="4">
-        <v>45908.543657407405</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>45908.550717592596</v>
+      </c>
+      <c r="E12" s="2">
+        <v>45911.324201388888</v>
+      </c>
       <c r="F12">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -758,17 +761,16 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4">
-        <v>45904.238113425927</v>
-      </c>
-      <c r="D13" s="4">
-        <v>45906.537569444445</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>45908.603506944448</v>
+      </c>
+      <c r="E13" s="2">
+        <v>45911.324201388888</v>
+      </c>
       <c r="F13">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -776,35 +778,35 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4">
-        <v>45902.031944444447</v>
+        <v>45904.095752314817</v>
       </c>
       <c r="D14" s="4">
-        <v>45904.216631944444</v>
+        <v>45906.629687499997</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C15" s="4">
-        <v>45907.401435185187</v>
+        <v>45906.25440972222</v>
       </c>
       <c r="D15" s="4">
-        <v>45909.52579861111</v>
+        <v>45908.543657407405</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -812,17 +814,17 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="4">
-        <v>45905.060277777775</v>
+        <v>45904.238113425927</v>
       </c>
       <c r="D16" s="4">
-        <v>45907.134097222224</v>
+        <v>45906.537569444445</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -830,17 +832,16 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4">
-        <v>45903.0937037037</v>
-      </c>
-      <c r="D17" s="4">
-        <v>45905.186064814814</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>45909.053182870368</v>
+      </c>
+      <c r="E17" s="2">
+        <v>45911.324201388888</v>
+      </c>
       <c r="F17">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -848,89 +849,88 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4">
-        <v>45907.522546296299</v>
+        <v>45902.031944444447</v>
       </c>
       <c r="D18" s="4">
-        <v>45909.570775462962</v>
+        <v>45904.216631944444</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4">
-        <v>45902.027557870373</v>
+        <v>45907.401435185187</v>
       </c>
       <c r="D19" s="4">
-        <v>45904.000578703701</v>
+        <v>45909.52579861111</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C20" s="4">
-        <v>45903.038356481484</v>
-      </c>
-      <c r="D20" s="4">
-        <v>45905.020983796298</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>45909.236574074072</v>
+      </c>
+      <c r="E20" s="2">
+        <v>45911.324201388888</v>
+      </c>
       <c r="F20">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4">
-        <v>45903.579016203701</v>
+        <v>45905.060277777775</v>
       </c>
       <c r="D21" s="4">
-        <v>45905.501250000001</v>
+        <v>45907.134097222224</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4">
-        <v>45908.082407407404</v>
+        <v>45908.552488425928</v>
       </c>
       <c r="D22" s="4">
-        <v>45910.006041666667</v>
+        <v>45910.652662037035</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
@@ -938,141 +938,143 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23" s="4">
-        <v>45906.549328703702</v>
+        <v>45903.0937037037</v>
       </c>
       <c r="D23" s="4">
-        <v>45908.533761574072</v>
+        <v>45905.186064814814</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C24" s="4">
-        <v>45905.58865740741</v>
+        <v>45907.522546296299</v>
       </c>
       <c r="D24" s="4">
-        <v>45907.541539351849</v>
+        <v>45909.570775462962</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4">
-        <v>45906.091840277775</v>
+        <v>45908.570474537039</v>
       </c>
       <c r="D25" s="4">
-        <v>45908.0002662037</v>
+        <v>45910.550486111111</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C26" s="4">
-        <v>45903.560266203705</v>
+        <v>45902.027557870373</v>
       </c>
       <c r="D26" s="4">
-        <v>45905.407696759263</v>
+        <v>45904.000578703701</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4">
-        <v>45901.550439814811</v>
+        <v>45903.038356481484</v>
       </c>
       <c r="D27" s="4">
-        <v>45903.3437962963</v>
+        <v>45905.020983796298</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C28" s="4">
-        <v>45904.367662037039</v>
+        <v>45903.579016203701</v>
       </c>
       <c r="D28" s="4">
-        <v>45906.129490740743</v>
+        <v>45905.501250000001</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C29" s="4">
-        <v>45908.525706018518</v>
-      </c>
-      <c r="E29" s="2">
-        <v>45910.311261574076</v>
-      </c>
+        <v>45908.082407407404</v>
+      </c>
+      <c r="D29" s="4">
+        <v>45910.006041666667</v>
+      </c>
+      <c r="E29" s="2"/>
       <c r="F29">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C30" s="4">
-        <v>45908.570474537039</v>
-      </c>
-      <c r="E30" s="2">
-        <v>45910.311261574076</v>
-      </c>
+        <v>45906.549328703702</v>
+      </c>
+      <c r="D30" s="4">
+        <v>45908.533761574072</v>
+      </c>
+      <c r="E30" s="2"/>
       <c r="F30">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -1083,13 +1085,14 @@
         <v>23</v>
       </c>
       <c r="C31" s="4">
-        <v>45908.550717592596</v>
-      </c>
-      <c r="E31" s="2">
-        <v>45910.311261574076</v>
-      </c>
+        <v>45905.58865740741</v>
+      </c>
+      <c r="D31" s="4">
+        <v>45907.541539351849</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="F31">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -1097,123 +1100,124 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C32" s="4">
-        <v>45908.552488425928</v>
-      </c>
-      <c r="E32" s="2">
-        <v>45910.311261574076</v>
-      </c>
+        <v>45906.091840277775</v>
+      </c>
+      <c r="D32" s="4">
+        <v>45908.0002662037</v>
+      </c>
+      <c r="E32" s="2"/>
       <c r="F32">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C33" s="4">
-        <v>45908.603506944448</v>
-      </c>
-      <c r="E33" s="2">
-        <v>45910.311261574076</v>
-      </c>
+        <v>45903.560266203705</v>
+      </c>
+      <c r="D33" s="4">
+        <v>45905.407696759263</v>
+      </c>
+      <c r="E33" s="2"/>
       <c r="F33">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="4">
-        <v>45906.348958333336</v>
+        <v>45904.367662037039</v>
       </c>
       <c r="D34" s="4">
-        <v>45908.012199074074</v>
+        <v>45906.129490740743</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C35" s="4">
-        <v>45903.75744212963</v>
+        <v>45901.550439814811</v>
       </c>
       <c r="D35" s="4">
-        <v>45905.312962962962</v>
+        <v>45903.3437962963</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C36" s="4">
-        <v>45907.705949074072</v>
+        <v>45909.261608796296</v>
       </c>
       <c r="D36" s="4">
-        <v>45909.21980324074</v>
+        <v>45911.001076388886</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C37" s="4">
-        <v>45907.729745370372</v>
-      </c>
-      <c r="D37" s="4">
-        <v>45909.231006944443</v>
-      </c>
-      <c r="E37" s="2"/>
+        <v>45909.602083333331</v>
+      </c>
+      <c r="E37" s="2">
+        <v>45911.324201388888</v>
+      </c>
       <c r="F37">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C38" s="4">
-        <v>45903.548900462964</v>
+        <v>45906.348958333336</v>
       </c>
       <c r="D38" s="4">
-        <v>45905.052442129629</v>
+        <v>45908.012199074074</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -1221,17 +1225,17 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C39" s="4">
-        <v>45903.531446759262</v>
+        <v>45903.75744212963</v>
       </c>
       <c r="D39" s="4">
-        <v>45905.010671296295</v>
+        <v>45905.312962962962</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -1239,17 +1243,17 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C40" s="4">
-        <v>45901.03025462963</v>
+        <v>45907.705949074072</v>
       </c>
       <c r="D40" s="4">
-        <v>45902.500243055554</v>
+        <v>45909.21980324074</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -1257,13 +1261,13 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C41" s="4">
-        <v>45908.210324074076</v>
+        <v>45908.058252314811</v>
       </c>
       <c r="D41" s="4">
-        <v>45909.712118055555</v>
+        <v>45909.559004629627</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41">
@@ -1278,10 +1282,10 @@
         <v>17</v>
       </c>
       <c r="C42" s="4">
-        <v>45908.058252314811</v>
+        <v>45909.579212962963</v>
       </c>
       <c r="D42" s="4">
-        <v>45909.559004629627</v>
+        <v>45911.07608796296</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42">
@@ -1290,56 +1294,56 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C43" s="4">
-        <v>45906.573877314811</v>
+        <v>45903.531446759262</v>
       </c>
       <c r="D43" s="4">
-        <v>45908.008958333332</v>
+        <v>45905.010671296295</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C44" s="4">
-        <v>45902.025509259256</v>
+        <v>45908.210324074076</v>
       </c>
       <c r="D44" s="4">
-        <v>45903.49627314815</v>
+        <v>45909.712118055555</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C45" s="4">
-        <v>45904.063692129632</v>
+        <v>45901.03025462963</v>
       </c>
       <c r="D45" s="4">
-        <v>45905.506157407406</v>
+        <v>45902.500243055554</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
@@ -1347,67 +1351,66 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C46" s="4">
-        <v>45901.560231481482</v>
+        <v>45907.729745370372</v>
       </c>
       <c r="D46" s="4">
-        <v>45903.0312037037</v>
+        <v>45909.231006944443</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C47" s="4">
-        <v>45902.545347222222</v>
+        <v>45903.548900462964</v>
       </c>
       <c r="D47" s="4">
-        <v>45904.018020833333</v>
+        <v>45905.052442129629</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C48" s="4">
-        <v>45908.562800925924</v>
-      </c>
-      <c r="D48" s="4">
-        <v>45910.003263888888</v>
-      </c>
-      <c r="E48" s="2"/>
+        <v>45909.799317129633</v>
+      </c>
+      <c r="E48" s="2">
+        <v>45911.324201388888</v>
+      </c>
       <c r="F48">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C49" s="4">
-        <v>45906.065810185188</v>
+        <v>45902.025509259256</v>
       </c>
       <c r="D49" s="4">
-        <v>45907.50099537037</v>
+        <v>45903.49627314815</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49">
@@ -1437,71 +1440,71 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C51" s="4">
-        <v>45903.062071759261</v>
+        <v>45902.545347222222</v>
       </c>
       <c r="D51" s="4">
-        <v>45904.471817129626</v>
+        <v>45904.018020833333</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C52" s="4">
-        <v>45903.625138888892</v>
+        <v>45908.562800925924</v>
       </c>
       <c r="D52" s="4">
-        <v>45905.008043981485</v>
+        <v>45910.003263888888</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C53" s="4">
-        <v>45906.087141203701</v>
+        <v>45906.065810185188</v>
       </c>
       <c r="D53" s="4">
-        <v>45907.494085648148</v>
+        <v>45907.50099537037</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C54" s="4">
-        <v>45902.767638888887</v>
+        <v>45904.063692129632</v>
       </c>
       <c r="D54" s="4">
-        <v>45904.084664351853</v>
+        <v>45905.506157407406</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -1509,17 +1512,17 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C55" s="4">
-        <v>45907.194444444445</v>
+        <v>45901.560231481482</v>
       </c>
       <c r="D55" s="4">
-        <v>45908.530740740738</v>
+        <v>45903.0312037037</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -1527,16 +1530,17 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C56" s="4">
-        <v>45909.039467592593</v>
-      </c>
-      <c r="E56" s="2">
-        <v>45910.311261574076</v>
-      </c>
+        <v>45906.573877314811</v>
+      </c>
+      <c r="D56" s="4">
+        <v>45908.008958333332</v>
+      </c>
+      <c r="E56" s="2"/>
       <c r="F56">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
@@ -1544,107 +1548,107 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C57" s="4">
-        <v>45906.221956018519</v>
+        <v>45903.062071759261</v>
       </c>
       <c r="D57" s="4">
-        <v>45907.510810185187</v>
+        <v>45904.471817129626</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C58" s="4">
-        <v>45906.810439814813</v>
+        <v>45903.625138888892</v>
       </c>
       <c r="D58" s="4">
-        <v>45908.090266203704</v>
+        <v>45905.008043981485</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C59" s="4">
-        <v>45907.24454861111</v>
+        <v>45906.087141203701</v>
       </c>
       <c r="D59" s="4">
-        <v>45908.508622685185</v>
+        <v>45907.494085648148</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C60" s="4">
-        <v>45905.7655787037</v>
+        <v>45907.194444444445</v>
       </c>
       <c r="D60" s="4">
-        <v>45907.012766203705</v>
+        <v>45908.530740740738</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C61" s="4">
-        <v>45904.257928240739</v>
+        <v>45902.767638888887</v>
       </c>
       <c r="D61" s="4">
-        <v>45905.532916666663</v>
+        <v>45904.084664351853</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C62" s="4">
-        <v>45903.095196759263</v>
+        <v>45909.039467592593</v>
       </c>
       <c r="D62" s="4">
-        <v>45904.33935185185</v>
+        <v>45910.373379629629</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
@@ -1652,17 +1656,17 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C63" s="4">
-        <v>45903.574432870373</v>
+        <v>45906.810439814813</v>
       </c>
       <c r="D63" s="4">
-        <v>45904.814143518517</v>
+        <v>45908.090266203704</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
@@ -1670,15 +1674,172 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C64" s="4">
-        <v>45909.053182870368</v>
-      </c>
-      <c r="E64" s="2">
-        <v>45910.311261574076</v>
-      </c>
+        <v>45906.221956018519</v>
+      </c>
+      <c r="D64" s="4">
+        <v>45907.510810185187</v>
+      </c>
+      <c r="E64" s="2"/>
       <c r="F64">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>46</v>
+      </c>
+      <c r="C65" s="4">
+        <v>45910.021134259259</v>
+      </c>
+      <c r="E65" s="4">
+        <v>45911.324201388888</v>
+      </c>
+      <c r="F65">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="4">
+        <v>45910.029456018521</v>
+      </c>
+      <c r="E66" s="4">
+        <v>45911.324201388888</v>
+      </c>
+      <c r="F66">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="4">
+        <v>45907.24454861111</v>
+      </c>
+      <c r="D67" s="4">
+        <v>45908.508622685185</v>
+      </c>
+      <c r="E67" s="4"/>
+      <c r="F67">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="4">
+        <v>45903.574432870373</v>
+      </c>
+      <c r="D68" s="4">
+        <v>45904.814143518517</v>
+      </c>
+      <c r="E68" s="4"/>
+      <c r="F68">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="4">
+        <v>45904.257928240739</v>
+      </c>
+      <c r="D69" s="4">
+        <v>45905.532916666663</v>
+      </c>
+      <c r="E69" s="4"/>
+      <c r="F69">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" s="4">
+        <v>45910.054398148146</v>
+      </c>
+      <c r="E70" s="4">
+        <v>45911.324201388888</v>
+      </c>
+      <c r="F70">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="4">
+        <v>45903.095196759263</v>
+      </c>
+      <c r="D71" s="4">
+        <v>45904.33935185185</v>
+      </c>
+      <c r="F71">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72" s="4">
+        <v>45909.260914351849</v>
+      </c>
+      <c r="D72" s="4">
+        <v>45910.524594907409</v>
+      </c>
+      <c r="F72">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>43</v>
+      </c>
+      <c r="C73" s="4">
+        <v>45905.7655787037</v>
+      </c>
+      <c r="D73" s="4">
+        <v>45907.012766203705</v>
+      </c>
+      <c r="F73">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-11 10:00:43.91
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$A$1:$F$73</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="69">
   <si>
     <t>电站名称</t>
   </si>
@@ -164,6 +167,63 @@
   </si>
   <si>
     <t>B04号直流</t>
+  </si>
+  <si>
+    <t>905号直流</t>
+  </si>
+  <si>
+    <t>B01号直流</t>
+  </si>
+  <si>
+    <t>307号直流</t>
+  </si>
+  <si>
+    <t>102号直流</t>
+  </si>
+  <si>
+    <t>705号直流</t>
+  </si>
+  <si>
+    <t>404号直流</t>
+  </si>
+  <si>
+    <t>A04号直流</t>
+  </si>
+  <si>
+    <t>704号直流</t>
+  </si>
+  <si>
+    <t>A05号直流</t>
+  </si>
+  <si>
+    <t>108号直流</t>
+  </si>
+  <si>
+    <t>203号直流</t>
+  </si>
+  <si>
+    <t>A01号直流</t>
+  </si>
+  <si>
+    <t>605号直流</t>
+  </si>
+  <si>
+    <t>403号直流</t>
+  </si>
+  <si>
+    <t>A03号直流</t>
+  </si>
+  <si>
+    <t>110号直流</t>
+  </si>
+  <si>
+    <t>111号直流</t>
+  </si>
+  <si>
+    <t>405号直流</t>
+  </si>
+  <si>
+    <t>002B号直流</t>
   </si>
 </sst>
 </file>
@@ -527,10 +587,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1843,6 +1903,1077 @@
         <v>30</v>
       </c>
     </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="4">
+        <v>45910.067824074074</v>
+      </c>
+      <c r="D74" s="4">
+        <v>45911.284560185188</v>
+      </c>
+      <c r="F74">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="4">
+        <v>45901.125694444447</v>
+      </c>
+      <c r="D75" s="4">
+        <v>45902.348506944443</v>
+      </c>
+      <c r="F75">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" s="4">
+        <v>45907.051342592589</v>
+      </c>
+      <c r="D76" s="4">
+        <v>45908.250138888892</v>
+      </c>
+      <c r="F76">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77" s="4">
+        <v>45903.550567129627</v>
+      </c>
+      <c r="D77" s="4">
+        <v>45904.756435185183</v>
+      </c>
+      <c r="F77">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" s="4">
+        <v>45903.346064814818</v>
+      </c>
+      <c r="D78" s="4">
+        <v>45904.573182870372</v>
+      </c>
+      <c r="F78">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="4">
+        <v>45905.566099537034</v>
+      </c>
+      <c r="D79" s="4">
+        <v>45906.734594907408</v>
+      </c>
+      <c r="F79">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80" s="4">
+        <v>45907.048576388886</v>
+      </c>
+      <c r="D80" s="4">
+        <v>45908.228101851855</v>
+      </c>
+      <c r="F80">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" s="4">
+        <v>45901.038946759261</v>
+      </c>
+      <c r="D81" s="4">
+        <v>45902.182835648149</v>
+      </c>
+      <c r="F81">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" s="4">
+        <v>45907.389652777776</v>
+      </c>
+      <c r="D82" s="4">
+        <v>45908.550567129627</v>
+      </c>
+      <c r="F82">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83" t="s">
+        <v>7</v>
+      </c>
+      <c r="B83" t="s">
+        <v>34</v>
+      </c>
+      <c r="C83" s="4">
+        <v>45904.03466435185</v>
+      </c>
+      <c r="D83" s="4">
+        <v>45905.192037037035</v>
+      </c>
+      <c r="F83">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="4">
+        <v>45909.373738425929</v>
+      </c>
+      <c r="D84" s="4">
+        <v>45910.524085648147</v>
+      </c>
+      <c r="F84">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="4">
+        <v>45907.094305555554</v>
+      </c>
+      <c r="D85" s="4">
+        <v>45908.213356481479</v>
+      </c>
+      <c r="F85">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" t="s">
+        <v>56</v>
+      </c>
+      <c r="C86" s="4">
+        <v>45909.091203703705</v>
+      </c>
+      <c r="D86" s="4">
+        <v>45910.220127314817</v>
+      </c>
+      <c r="F86">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A87" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" t="s">
+        <v>57</v>
+      </c>
+      <c r="C87" s="4">
+        <v>45906.042974537035</v>
+      </c>
+      <c r="D87" s="4">
+        <v>45907.169976851852</v>
+      </c>
+      <c r="F87">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88" s="4">
+        <v>45906.575902777775</v>
+      </c>
+      <c r="D88" s="4">
+        <v>45907.67150462963</v>
+      </c>
+      <c r="F88">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89" t="s">
+        <v>9</v>
+      </c>
+      <c r="B89" t="s">
+        <v>39</v>
+      </c>
+      <c r="C89" s="4">
+        <v>45909.514016203706</v>
+      </c>
+      <c r="D89" s="4">
+        <v>45910.611180555556</v>
+      </c>
+      <c r="F89">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B90" t="s">
+        <v>58</v>
+      </c>
+      <c r="C90" s="4">
+        <v>45906.047337962962</v>
+      </c>
+      <c r="D90" s="4">
+        <v>45907.137569444443</v>
+      </c>
+      <c r="F90">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91" t="s">
+        <v>41</v>
+      </c>
+      <c r="C91" s="4">
+        <v>45908.118969907409</v>
+      </c>
+      <c r="D91" s="4">
+        <v>45909.179571759261</v>
+      </c>
+      <c r="F91">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="4">
+        <v>45910.247546296298</v>
+      </c>
+      <c r="E92" s="4">
+        <v>45911.324201388888</v>
+      </c>
+      <c r="F92">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" t="s">
+        <v>45</v>
+      </c>
+      <c r="C93" s="4">
+        <v>45902.027233796296</v>
+      </c>
+      <c r="D93" s="4">
+        <v>45903.087951388887</v>
+      </c>
+      <c r="F93">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A94" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" t="s">
+        <v>53</v>
+      </c>
+      <c r="C94" s="4">
+        <v>45907.134444444448</v>
+      </c>
+      <c r="D94" s="4">
+        <v>45908.224537037036</v>
+      </c>
+      <c r="F94">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A95" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" s="4">
+        <v>45901.259722222225</v>
+      </c>
+      <c r="D95" s="4">
+        <v>45902.373217592591</v>
+      </c>
+      <c r="F95">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A96" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" s="4">
+        <v>45909.039143518516</v>
+      </c>
+      <c r="D96" s="4">
+        <v>45910.102083333331</v>
+      </c>
+      <c r="F96">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" s="4">
+        <v>45901.470590277779</v>
+      </c>
+      <c r="D97" s="4">
+        <v>45902.562650462962</v>
+      </c>
+      <c r="F97">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A98" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98" t="s">
+        <v>14</v>
+      </c>
+      <c r="C98" s="4">
+        <v>45910.196134259262</v>
+      </c>
+      <c r="D98" s="4">
+        <v>45911.248784722222</v>
+      </c>
+      <c r="F98">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="4">
+        <v>45908.19803240741</v>
+      </c>
+      <c r="D99" s="4">
+        <v>45909.213159722225</v>
+      </c>
+      <c r="F99">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A100" t="s">
+        <v>9</v>
+      </c>
+      <c r="B100" t="s">
+        <v>60</v>
+      </c>
+      <c r="C100" s="4">
+        <v>45907.620358796295</v>
+      </c>
+      <c r="D100" s="4">
+        <v>45908.656805555554</v>
+      </c>
+      <c r="F100">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A101" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="4">
+        <v>45908.567731481482</v>
+      </c>
+      <c r="D101" s="4">
+        <v>45909.606053240743</v>
+      </c>
+      <c r="F101">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A102" t="s">
+        <v>9</v>
+      </c>
+      <c r="B102" t="s">
+        <v>35</v>
+      </c>
+      <c r="C102" s="4">
+        <v>45905.577847222223</v>
+      </c>
+      <c r="D102" s="4">
+        <v>45906.623020833336</v>
+      </c>
+      <c r="F102">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" t="s">
+        <v>61</v>
+      </c>
+      <c r="C103" s="4">
+        <v>45901.148784722223</v>
+      </c>
+      <c r="D103" s="4">
+        <v>45902.167685185188</v>
+      </c>
+      <c r="F103">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A104" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" t="s">
+        <v>62</v>
+      </c>
+      <c r="C104" s="4">
+        <v>45901.158136574071</v>
+      </c>
+      <c r="D104" s="4">
+        <v>45902.190081018518</v>
+      </c>
+      <c r="F104">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" t="s">
+        <v>63</v>
+      </c>
+      <c r="C105" s="4">
+        <v>45903.08121527778</v>
+      </c>
+      <c r="D105" s="4">
+        <v>45904.113680555558</v>
+      </c>
+      <c r="F105">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A106" t="s">
+        <v>7</v>
+      </c>
+      <c r="B106" t="s">
+        <v>64</v>
+      </c>
+      <c r="C106" s="4">
+        <v>45903.038553240738</v>
+      </c>
+      <c r="D106" s="4">
+        <v>45904.044745370367</v>
+      </c>
+      <c r="F106">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A107" t="s">
+        <v>7</v>
+      </c>
+      <c r="B107" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" s="4">
+        <v>45908.570671296293</v>
+      </c>
+      <c r="D107" s="4">
+        <v>45909.609884259262</v>
+      </c>
+      <c r="F107">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108" s="4">
+        <v>45901.569282407407</v>
+      </c>
+      <c r="D108" s="4">
+        <v>45902.593414351853</v>
+      </c>
+      <c r="F108">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" t="s">
+        <v>60</v>
+      </c>
+      <c r="C109" s="4">
+        <v>45906.5156712963</v>
+      </c>
+      <c r="D109" s="4">
+        <v>45907.565092592595</v>
+      </c>
+      <c r="F109">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A110" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" t="s">
+        <v>66</v>
+      </c>
+      <c r="C110" s="4">
+        <v>45909.239444444444</v>
+      </c>
+      <c r="D110" s="4">
+        <v>45910.265706018516</v>
+      </c>
+      <c r="F110">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" t="s">
+        <v>47</v>
+      </c>
+      <c r="C111" s="4">
+        <v>45904.531631944446</v>
+      </c>
+      <c r="D111" s="4">
+        <v>45905.530775462961</v>
+      </c>
+      <c r="F111">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112" t="s">
+        <v>47</v>
+      </c>
+      <c r="C112" s="4">
+        <v>45909.029490740744</v>
+      </c>
+      <c r="D112" s="4">
+        <v>45910.00445601852</v>
+      </c>
+      <c r="F112">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A113" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113" t="s">
+        <v>35</v>
+      </c>
+      <c r="C113" s="4">
+        <v>45903.551539351851</v>
+      </c>
+      <c r="D113" s="4">
+        <v>45904.543136574073</v>
+      </c>
+      <c r="F113">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A114" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="4">
+        <v>45910.02920138889</v>
+      </c>
+      <c r="D114" s="4">
+        <v>45911.005185185182</v>
+      </c>
+      <c r="F114">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115" t="s">
+        <v>67</v>
+      </c>
+      <c r="C115" s="4">
+        <v>45907.019560185188</v>
+      </c>
+      <c r="D115" s="4">
+        <v>45908.010844907411</v>
+      </c>
+      <c r="F115">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A116" t="s">
+        <v>9</v>
+      </c>
+      <c r="B116" t="s">
+        <v>11</v>
+      </c>
+      <c r="C116" s="4">
+        <v>45903.531400462962</v>
+      </c>
+      <c r="D116" s="4">
+        <v>45904.523900462962</v>
+      </c>
+      <c r="F116">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A117" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" t="s">
+        <v>58</v>
+      </c>
+      <c r="C117" s="4">
+        <v>45905.028263888889</v>
+      </c>
+      <c r="D117" s="4">
+        <v>45906.015115740738</v>
+      </c>
+      <c r="F117">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>63</v>
+      </c>
+      <c r="C118" s="4">
+        <v>45906.993020833332</v>
+      </c>
+      <c r="D118" s="4">
+        <v>45907.99009259259</v>
+      </c>
+      <c r="F118">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" t="s">
+        <v>32</v>
+      </c>
+      <c r="C119" s="4">
+        <v>45906.572326388887</v>
+      </c>
+      <c r="D119" s="4">
+        <v>45907.549814814818</v>
+      </c>
+      <c r="F119">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" t="s">
+        <v>32</v>
+      </c>
+      <c r="C120" s="4">
+        <v>45910.041087962964</v>
+      </c>
+      <c r="D120" s="4">
+        <v>45911.026550925926</v>
+      </c>
+      <c r="F120">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" t="s">
+        <v>41</v>
+      </c>
+      <c r="C121" s="4">
+        <v>45909.531261574077</v>
+      </c>
+      <c r="D121" s="4">
+        <v>45910.523888888885</v>
+      </c>
+      <c r="F121">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" t="s">
+        <v>39</v>
+      </c>
+      <c r="C122" s="4">
+        <v>45904.038356481484</v>
+      </c>
+      <c r="D122" s="4">
+        <v>45905.000960648147</v>
+      </c>
+      <c r="F122">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A123" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123" t="s">
+        <v>54</v>
+      </c>
+      <c r="C123" s="4">
+        <v>45903.040659722225</v>
+      </c>
+      <c r="D123" s="4">
+        <v>45904.012349537035</v>
+      </c>
+      <c r="F123">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" t="s">
+        <v>54</v>
+      </c>
+      <c r="C124" s="4">
+        <v>45905.033067129632</v>
+      </c>
+      <c r="D124" s="4">
+        <v>45906.00104166667</v>
+      </c>
+      <c r="F124">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A125" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" t="s">
+        <v>20</v>
+      </c>
+      <c r="C125" s="4">
+        <v>45901.038090277776</v>
+      </c>
+      <c r="D125" s="4">
+        <v>45902.001168981478</v>
+      </c>
+      <c r="F125">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A126" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" t="s">
+        <v>20</v>
+      </c>
+      <c r="C126" s="4">
+        <v>45905.558854166666</v>
+      </c>
+      <c r="D126" s="4">
+        <v>45906.555868055555</v>
+      </c>
+      <c r="F126">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A127" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" t="s">
+        <v>18</v>
+      </c>
+      <c r="C127" s="4">
+        <v>45901.116909722223</v>
+      </c>
+      <c r="D127" s="4">
+        <v>45902.102569444447</v>
+      </c>
+      <c r="F127">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A128" t="s">
+        <v>7</v>
+      </c>
+      <c r="B128" t="s">
+        <v>34</v>
+      </c>
+      <c r="C128" s="4">
+        <v>45901.538043981483</v>
+      </c>
+      <c r="D128" s="4">
+        <v>45902.527268518519</v>
+      </c>
+      <c r="F128">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A129" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129" t="s">
+        <v>21</v>
+      </c>
+      <c r="C129" s="4">
+        <v>45908.923564814817</v>
+      </c>
+      <c r="D129" s="4">
+        <v>45909.953576388885</v>
+      </c>
+      <c r="F129">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A130" t="s">
+        <v>12</v>
+      </c>
+      <c r="B130" t="s">
+        <v>33</v>
+      </c>
+      <c r="C130" s="4">
+        <v>45907.041504629633</v>
+      </c>
+      <c r="D130" s="4">
+        <v>45908.003831018519</v>
+      </c>
+      <c r="F130">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A131" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" t="s">
+        <v>53</v>
+      </c>
+      <c r="C131" s="4">
+        <v>45902.031307870369</v>
+      </c>
+      <c r="D131" s="4">
+        <v>45903.015347222223</v>
+      </c>
+      <c r="F131">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A132" t="s">
+        <v>12</v>
+      </c>
+      <c r="B132" t="s">
+        <v>68</v>
+      </c>
+      <c r="C132" s="4">
+        <v>45906.520752314813</v>
+      </c>
+      <c r="D132" s="4">
+        <v>45907.527858796297</v>
+      </c>
+      <c r="F132">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A133" t="s">
+        <v>12</v>
+      </c>
+      <c r="B133" t="s">
+        <v>42</v>
+      </c>
+      <c r="C133" s="4">
+        <v>45909.532372685186</v>
+      </c>
+      <c r="D133" s="4">
+        <v>45910.502280092594</v>
+      </c>
+      <c r="F133">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A134" t="s">
+        <v>5</v>
+      </c>
+      <c r="B134" t="s">
+        <v>31</v>
+      </c>
+      <c r="C134" s="4">
+        <v>45904.702118055553</v>
+      </c>
+      <c r="D134" s="4">
+        <v>45905.667326388888</v>
+      </c>
+      <c r="F134">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A135" t="s">
+        <v>5</v>
+      </c>
+      <c r="B135" t="s">
+        <v>65</v>
+      </c>
+      <c r="C135" s="4">
+        <v>45904.020173611112</v>
+      </c>
+      <c r="D135" s="4">
+        <v>45905.008136574077</v>
+      </c>
+      <c r="F135">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A136" t="s">
+        <v>5</v>
+      </c>
+      <c r="B136" t="s">
+        <v>53</v>
+      </c>
+      <c r="C136" s="4">
+        <v>45902.329155092593</v>
+      </c>
+      <c r="D136" s="4">
+        <v>45903.310069444444</v>
+      </c>
+      <c r="F136">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto commit at 2025-09-14  9:39:00.46
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="66">
   <si>
     <t>电站名称</t>
   </si>
@@ -191,6 +191,30 @@
   </si>
   <si>
     <t>803号直流</t>
+  </si>
+  <si>
+    <t>长沙市开福区高岭香江国际城充电站建设项目</t>
+  </si>
+  <si>
+    <t>107号直流</t>
+  </si>
+  <si>
+    <t>109号直流</t>
+  </si>
+  <si>
+    <t>208号直流</t>
+  </si>
+  <si>
+    <t>302号直流</t>
+  </si>
+  <si>
+    <t>111号直流</t>
+  </si>
+  <si>
+    <t>204号直流</t>
+  </si>
+  <si>
+    <t>206号直流</t>
   </si>
 </sst>
 </file>
@@ -551,19 +575,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="32.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.25" customWidth="1"/>
-    <col min="4" max="4" width="24.375" customWidth="1"/>
-    <col min="5" max="5" width="24.875" customWidth="1"/>
+    <col min="3" max="3" width="29.375" customWidth="1"/>
+    <col min="4" max="4" width="26.375" customWidth="1"/>
+    <col min="5" max="5" width="28.875" customWidth="1"/>
     <col min="6" max="6" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -599,10 +623,10 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>45914.320879629631</v>
+        <v>45914.373865740738</v>
       </c>
       <c r="F2">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -635,10 +659,10 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>45914.320879629631</v>
+        <v>45914.373865740738</v>
       </c>
       <c r="F4">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -769,16 +793,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2">
-        <v>45907.570555555554</v>
+        <v>45906.271747685183</v>
       </c>
       <c r="D12" s="2">
-        <v>45910.500289351854</v>
+        <v>45909.218194444446</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12">
@@ -787,16 +811,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2">
-        <v>45906.271747685183</v>
+        <v>45907.570555555554</v>
       </c>
       <c r="D13" s="2">
-        <v>45909.218194444446</v>
+        <v>45910.500289351854</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13">
@@ -815,10 +839,10 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2">
-        <v>45914.320879629631</v>
+        <v>45914.373865740738</v>
       </c>
       <c r="F14">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -931,16 +955,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2">
-        <v>45907.522546296299</v>
+        <v>45910.355798611112</v>
       </c>
       <c r="D21" s="2">
-        <v>45909.570775462962</v>
+        <v>45912.393368055556</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21">
@@ -952,35 +976,35 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2">
-        <v>45912.328969907408</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2">
-        <v>45914.320879629631</v>
-      </c>
+        <v>45907.522546296299</v>
+      </c>
+      <c r="D22" s="2">
+        <v>45909.570775462962</v>
+      </c>
+      <c r="E22" s="2"/>
       <c r="F22">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C23" s="2">
-        <v>45911.040381944447</v>
-      </c>
-      <c r="D23" s="2">
-        <v>45913.023263888892</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>45912.328969907408</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
+        <v>45914.373865740738</v>
+      </c>
       <c r="F23">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
@@ -988,13 +1012,13 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2">
-        <v>45908.570474537039</v>
+        <v>45911.040381944447</v>
       </c>
       <c r="D24" s="2">
-        <v>45910.550486111111</v>
+        <v>45913.023263888892</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24">
@@ -1003,34 +1027,34 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C25" s="2">
-        <v>45912.060983796298</v>
+        <v>45908.570474537039</v>
       </c>
       <c r="D25" s="2">
-        <v>45914.012141203704</v>
+        <v>45910.550486111111</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C26" s="2">
-        <v>45906.549328703702</v>
+        <v>45910.561724537038</v>
       </c>
       <c r="D26" s="2">
-        <v>45908.533761574072</v>
+        <v>45912.509375000001</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26">
@@ -1078,53 +1102,53 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2">
-        <v>45906.091840277775</v>
+        <v>45912.060983796298</v>
       </c>
       <c r="D29" s="2">
-        <v>45908.0002662037</v>
+        <v>45914.012141203704</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2">
-        <v>45905.58865740741</v>
+        <v>45906.549328703702</v>
       </c>
       <c r="D30" s="2">
-        <v>45907.541539351849</v>
+        <v>45908.533761574072</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C31" s="2">
-        <v>45911.646747685183</v>
+        <v>45905.58865740741</v>
       </c>
       <c r="D31" s="2">
-        <v>45913.523923611108</v>
+        <v>45907.541539351849</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -1132,107 +1156,107 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C32" s="2">
-        <v>45911.562384259261</v>
+        <v>45906.091840277775</v>
       </c>
       <c r="D32" s="2">
-        <v>45913.435532407406</v>
+        <v>45908.0002662037</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C33" s="2">
-        <v>45909.261608796296</v>
+        <v>45911.646747685183</v>
       </c>
       <c r="D33" s="2">
-        <v>45911.001076388886</v>
+        <v>45913.523923611108</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C34" s="2">
-        <v>45909.799317129633</v>
+        <v>45911.562384259261</v>
       </c>
       <c r="D34" s="2">
-        <v>45911.513888888891</v>
+        <v>45913.435532407406</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C35" s="2">
-        <v>45911.531018518515</v>
+        <v>45909.261608796296</v>
       </c>
       <c r="D35" s="2">
-        <v>45913.206875000003</v>
+        <v>45911.001076388886</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="2">
-        <v>45907.705949074072</v>
+        <v>45909.799317129633</v>
       </c>
       <c r="D36" s="2">
-        <v>45909.21980324074</v>
+        <v>45911.513888888891</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C37" s="2">
-        <v>45908.058252314811</v>
+        <v>45906.348958333336</v>
       </c>
       <c r="D37" s="2">
-        <v>45909.559004629627</v>
+        <v>45908.012199074074</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -1240,17 +1264,17 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C38" s="2">
-        <v>45909.579212962963</v>
+        <v>45911.531018518515</v>
       </c>
       <c r="D38" s="2">
-        <v>45911.07608796296</v>
+        <v>45913.206875000003</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -1258,31 +1282,31 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C39" s="2">
-        <v>45908.210324074076</v>
+        <v>45907.705949074072</v>
       </c>
       <c r="D39" s="2">
-        <v>45909.712118055555</v>
+        <v>45909.21980324074</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C40" s="2">
-        <v>45910.534502314818</v>
+        <v>45907.729745370372</v>
       </c>
       <c r="D40" s="2">
-        <v>45912.012048611112</v>
+        <v>45909.231006944443</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40">
@@ -1291,16 +1315,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C41" s="2">
-        <v>45907.729745370372</v>
+        <v>45908.058252314811</v>
       </c>
       <c r="D41" s="2">
-        <v>45909.231006944443</v>
+        <v>45909.559004629627</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41">
@@ -1312,17 +1336,17 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C42" s="2">
-        <v>45908.562800925924</v>
+        <v>45909.579212962963</v>
       </c>
       <c r="D42" s="2">
-        <v>45910.003263888888</v>
+        <v>45911.07608796296</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
@@ -1330,71 +1354,71 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C43" s="2">
-        <v>45906.065810185188</v>
+        <v>45908.210324074076</v>
       </c>
       <c r="D43" s="2">
-        <v>45907.50099537037</v>
+        <v>45909.712118055555</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C44" s="2">
-        <v>45912.567314814813</v>
+        <v>45910.534502314818</v>
       </c>
       <c r="D44" s="2">
-        <v>45914.04074074074</v>
+        <v>45912.012048611112</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C45" s="2">
-        <v>45906.087141203701</v>
+        <v>45906.573877314811</v>
       </c>
       <c r="D45" s="2">
-        <v>45907.494085648148</v>
+        <v>45908.008958333332</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="2">
-        <v>45912.627604166664</v>
+        <v>45912.567314814813</v>
       </c>
       <c r="D46" s="2">
-        <v>45914.005208333336</v>
+        <v>45914.04074074074</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
@@ -1402,107 +1426,107 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C47" s="2">
-        <v>45910.054398148146</v>
+        <v>45908.562800925924</v>
       </c>
       <c r="D47" s="2">
-        <v>45911.384293981479</v>
+        <v>45910.003263888888</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C48" s="2">
-        <v>45907.194444444445</v>
+        <v>45906.065810185188</v>
       </c>
       <c r="D48" s="2">
-        <v>45908.530740740738</v>
+        <v>45907.50099537037</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C49" s="2">
-        <v>45906.810439814813</v>
+        <v>45906.087141203701</v>
       </c>
       <c r="D49" s="2">
-        <v>45908.090266203704</v>
+        <v>45907.494085648148</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C50" s="2">
-        <v>45907.24454861111</v>
+        <v>45912.627604166664</v>
       </c>
       <c r="D50" s="2">
-        <v>45908.508622685185</v>
+        <v>45914.005208333336</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C51" s="2">
-        <v>45910.247546296298</v>
+        <v>45907.194444444445</v>
       </c>
       <c r="D51" s="2">
-        <v>45911.529826388891</v>
+        <v>45908.530740740738</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C52" s="2">
-        <v>45906.221956018519</v>
+        <v>45909.039467592593</v>
       </c>
       <c r="D52" s="2">
-        <v>45907.510810185187</v>
+        <v>45910.373379629629</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
@@ -1510,17 +1534,17 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C53" s="2">
-        <v>45910.029456018521</v>
+        <v>45910.054398148146</v>
       </c>
       <c r="D53" s="2">
-        <v>45911.331701388888</v>
+        <v>45911.384293981479</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
@@ -1535,46 +1559,46 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2">
-        <v>45914.320879629631</v>
+        <v>45914.373865740738</v>
       </c>
       <c r="F54">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C55" s="2">
-        <v>45909.260914351849</v>
-      </c>
-      <c r="D55" s="2">
-        <v>45910.524594907409</v>
-      </c>
-      <c r="E55" s="2"/>
+        <v>45913.052685185183</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2">
+        <v>45914.373865740738</v>
+      </c>
       <c r="F55">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C56" s="2">
-        <v>45913.052685185183</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2">
-        <v>45914.320879629631</v>
-      </c>
+        <v>45906.810439814813</v>
+      </c>
+      <c r="D56" s="2">
+        <v>45908.090266203704</v>
+      </c>
+      <c r="E56" s="2"/>
       <c r="F56">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
@@ -1582,17 +1606,17 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C57" s="2">
-        <v>45913.050844907404</v>
+        <v>45907.24454861111</v>
       </c>
       <c r="D57" s="2">
-        <v>45914.284895833334</v>
+        <v>45908.508622685185</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
@@ -1600,17 +1624,17 @@
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C58" s="2">
-        <v>45910.067824074074</v>
+        <v>45910.247546296298</v>
       </c>
       <c r="D58" s="2">
-        <v>45911.284560185188</v>
+        <v>45911.529826388891</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
@@ -1618,17 +1642,17 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C59" s="2">
-        <v>45907.051342592589</v>
+        <v>45906.221956018519</v>
       </c>
       <c r="D59" s="2">
-        <v>45908.250138888892</v>
+        <v>45907.510810185187</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
@@ -1636,89 +1660,89 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C60" s="2">
-        <v>45907.389652777776</v>
+        <v>45910.029456018521</v>
       </c>
       <c r="D60" s="2">
-        <v>45908.550567129627</v>
+        <v>45911.331701388888</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C61" s="2">
-        <v>45910.356319444443</v>
+        <v>45909.260914351849</v>
       </c>
       <c r="D61" s="2">
-        <v>45911.500925925924</v>
+        <v>45910.524594907409</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C62" s="2">
-        <v>45909.373738425929</v>
+        <v>45905.7655787037</v>
       </c>
       <c r="D62" s="2">
-        <v>45910.524085648147</v>
+        <v>45907.012766203705</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C63" s="2">
-        <v>45905.566099537034</v>
+        <v>45913.050844907404</v>
       </c>
       <c r="D63" s="2">
-        <v>45906.734594907408</v>
+        <v>45914.284895833334</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C64" s="2">
-        <v>45907.048576388886</v>
+        <v>45910.067824074074</v>
       </c>
       <c r="D64" s="2">
-        <v>45908.228101851855</v>
+        <v>45911.284560185188</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
@@ -1726,71 +1750,71 @@
         <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C65" s="2">
-        <v>45906.042974537035</v>
+        <v>45907.051342592589</v>
       </c>
       <c r="D65" s="2">
-        <v>45907.169976851852</v>
+        <v>45908.250138888892</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C66" s="2">
-        <v>45909.091203703705</v>
+        <v>45909.373738425929</v>
       </c>
       <c r="D66" s="2">
-        <v>45910.220127314817</v>
+        <v>45910.524085648147</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C67" s="2">
-        <v>45907.094305555554</v>
+        <v>45905.566099537034</v>
       </c>
       <c r="D67" s="2">
-        <v>45908.213356481479</v>
+        <v>45906.734594907408</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C68" s="2">
-        <v>45906.575902777775</v>
+        <v>45907.048576388886</v>
       </c>
       <c r="D68" s="2">
-        <v>45907.67150462963</v>
+        <v>45908.228101851855</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
@@ -1798,49 +1822,49 @@
         <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C69" s="2">
-        <v>45912.041076388887</v>
+        <v>45907.389652777776</v>
       </c>
       <c r="D69" s="2">
-        <v>45913.145925925928</v>
+        <v>45908.550567129627</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C70" s="2">
-        <v>45913.042430555557</v>
+        <v>45910.356319444443</v>
       </c>
       <c r="D70" s="2">
-        <v>45914.200810185182</v>
+        <v>45911.500925925924</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C71" s="2">
-        <v>45911.012094907404</v>
+        <v>45913.042430555557</v>
       </c>
       <c r="D71" s="2">
-        <v>45912.137696759259</v>
+        <v>45914.200810185182</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71">
@@ -1849,20 +1873,20 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C72" s="2">
-        <v>45908.118969907409</v>
+        <v>45911.012094907404</v>
       </c>
       <c r="D72" s="2">
-        <v>45909.179571759261</v>
+        <v>45912.137696759259</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
@@ -1870,17 +1894,17 @@
         <v>6</v>
       </c>
       <c r="B73" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C73" s="2">
-        <v>45906.047337962962</v>
+        <v>45909.091203703705</v>
       </c>
       <c r="D73" s="2">
-        <v>45907.137569444443</v>
+        <v>45910.220127314817</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
@@ -1888,211 +1912,211 @@
         <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C74" s="2">
-        <v>45913.23265046296</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2">
-        <v>45914.320879629631</v>
-      </c>
+        <v>45906.042974537035</v>
+      </c>
+      <c r="D74" s="2">
+        <v>45907.169976851852</v>
+      </c>
+      <c r="E74" s="2"/>
       <c r="F74">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C75" s="2">
-        <v>45909.039143518516</v>
+        <v>45907.094305555554</v>
       </c>
       <c r="D75" s="2">
-        <v>45910.102083333331</v>
+        <v>45908.213356481479</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C76" s="2">
-        <v>45907.134444444448</v>
+        <v>45906.575902777775</v>
       </c>
       <c r="D76" s="2">
-        <v>45908.224537037036</v>
+        <v>45907.67150462963</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C77" s="2">
-        <v>45913.064467592594</v>
+        <v>45912.041076388887</v>
       </c>
       <c r="D77" s="2">
-        <v>45914.140983796293</v>
+        <v>45913.145925925928</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C78" s="2">
-        <v>45909.514016203706</v>
-      </c>
-      <c r="D78" s="2">
-        <v>45910.611180555556</v>
-      </c>
-      <c r="E78" s="2"/>
+        <v>45913.23265046296</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2">
+        <v>45914.373865740738</v>
+      </c>
       <c r="F78">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C79" s="2">
-        <v>45912.043020833335</v>
+        <v>45909.039143518516</v>
       </c>
       <c r="D79" s="2">
-        <v>45913.113923611112</v>
+        <v>45910.102083333331</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C80" s="2">
-        <v>45911.684641203705</v>
+        <v>45907.134444444448</v>
       </c>
       <c r="D80" s="2">
-        <v>45912.726527777777</v>
+        <v>45908.224537037036</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C81" s="2">
-        <v>45911.994386574072</v>
+        <v>45913.064467592594</v>
       </c>
       <c r="D81" s="2">
-        <v>45913.008622685185</v>
+        <v>45914.140983796293</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C82" s="2">
-        <v>45908.570671296293</v>
+        <v>45909.514016203706</v>
       </c>
       <c r="D82" s="2">
-        <v>45909.609884259262</v>
+        <v>45910.611180555556</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C83" s="2">
-        <v>45913.021006944444</v>
+        <v>45908.118969907409</v>
       </c>
       <c r="D83" s="2">
-        <v>45914.078969907408</v>
+        <v>45909.179571759261</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C84" s="2">
-        <v>45908.567731481482</v>
+        <v>45906.047337962962</v>
       </c>
       <c r="D84" s="2">
-        <v>45909.606053240743</v>
+        <v>45907.137569444443</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C85" s="2">
-        <v>45908.19803240741</v>
+        <v>45913.021006944444</v>
       </c>
       <c r="D85" s="2">
-        <v>45909.213159722225</v>
+        <v>45914.078969907408</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85">
@@ -2101,16 +2125,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B86" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C86" s="2">
-        <v>45910.196134259262</v>
+        <v>45909.239444444444</v>
       </c>
       <c r="D86" s="2">
-        <v>45911.248784722222</v>
+        <v>45910.265706018516</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86">
@@ -2119,16 +2143,16 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B87" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C87" s="2">
-        <v>45905.577847222223</v>
+        <v>45911.244166666664</v>
       </c>
       <c r="D87" s="2">
-        <v>45906.623020833336</v>
+        <v>45912.265601851854</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87">
@@ -2137,16 +2161,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B88" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C88" s="2">
-        <v>45907.620358796295</v>
+        <v>45911.504976851851</v>
       </c>
       <c r="D88" s="2">
-        <v>45908.656805555554</v>
+        <v>45912.543333333335</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88">
@@ -2155,110 +2179,110 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C89" s="2">
-        <v>45906.993020833332</v>
+        <v>45906.5156712963</v>
       </c>
       <c r="D89" s="2">
-        <v>45907.99009259259</v>
+        <v>45907.565092592595</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C90" s="2">
-        <v>45905.558854166666</v>
+        <v>45908.19803240741</v>
       </c>
       <c r="D90" s="2">
-        <v>45906.555868055555</v>
+        <v>45909.213159722225</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C91" s="2">
-        <v>45909.531261574077</v>
+        <v>45908.567731481482</v>
       </c>
       <c r="D91" s="2">
-        <v>45910.523888888885</v>
+        <v>45909.606053240743</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="C92" s="2">
-        <v>45913.030231481483</v>
+        <v>45910.196134259262</v>
       </c>
       <c r="D92" s="2">
-        <v>45914.003888888888</v>
+        <v>45911.248784722222</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C93" s="2">
-        <v>45905.028263888889</v>
+        <v>45905.577847222223</v>
       </c>
       <c r="D93" s="2">
-        <v>45906.015115740738</v>
+        <v>45906.623020833336</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C94" s="2">
-        <v>45905.033067129632</v>
+        <v>45907.620358796295</v>
       </c>
       <c r="D94" s="2">
-        <v>45906.00104166667</v>
+        <v>45908.656805555554</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.15">
@@ -2266,17 +2290,17 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C95" s="2">
-        <v>45910.584328703706</v>
+        <v>45912.043020833335</v>
       </c>
       <c r="D95" s="2">
-        <v>45911.616053240738</v>
+        <v>45913.113923611112</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.15">
@@ -2284,17 +2308,17 @@
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C96" s="2">
-        <v>45906.572326388887</v>
+        <v>45911.684641203705</v>
       </c>
       <c r="D96" s="2">
-        <v>45907.549814814818</v>
+        <v>45912.726527777777</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
@@ -2302,17 +2326,17 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C97" s="2">
-        <v>45910.041087962964</v>
+        <v>45911.994386574072</v>
       </c>
       <c r="D97" s="2">
-        <v>45911.026550925926</v>
+        <v>45913.008622685185</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.15">
@@ -2320,17 +2344,17 @@
         <v>6</v>
       </c>
       <c r="B98" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C98" s="2">
-        <v>45913.029675925929</v>
+        <v>45908.570671296293</v>
       </c>
       <c r="D98" s="2">
-        <v>45914.000960648147</v>
+        <v>45909.609884259262</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
@@ -2425,16 +2449,16 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B104" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C104" s="2">
-        <v>45909.029490740744</v>
+        <v>45912.242094907408</v>
       </c>
       <c r="D104" s="2">
-        <v>45910.00445601852</v>
+        <v>45913.231030092589</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104">
@@ -2446,13 +2470,13 @@
         <v>8</v>
       </c>
       <c r="B105" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C105" s="2">
-        <v>45912.03328703704</v>
+        <v>45909.029490740744</v>
       </c>
       <c r="D105" s="2">
-        <v>45913.003379629627</v>
+        <v>45910.00445601852</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105">
@@ -2464,13 +2488,13 @@
         <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C106" s="2">
-        <v>45911.556932870371</v>
+        <v>45912.03328703704</v>
       </c>
       <c r="D106" s="2">
-        <v>45912.543055555558</v>
+        <v>45913.003379629627</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106">
@@ -2482,13 +2506,13 @@
         <v>8</v>
       </c>
       <c r="B107" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C107" s="2">
-        <v>45910.02920138889</v>
+        <v>45911.556932870371</v>
       </c>
       <c r="D107" s="2">
-        <v>45911.005185185182</v>
+        <v>45912.543055555558</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107">
@@ -2503,10 +2527,10 @@
         <v>31</v>
       </c>
       <c r="C108" s="2">
-        <v>45911.034571759257</v>
+        <v>45910.02920138889</v>
       </c>
       <c r="D108" s="2">
-        <v>45912.001400462963</v>
+        <v>45911.005185185182</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108">
@@ -2518,13 +2542,13 @@
         <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C109" s="2">
-        <v>45907.019560185188</v>
+        <v>45911.034571759257</v>
       </c>
       <c r="D109" s="2">
-        <v>45908.010844907411</v>
+        <v>45912.001400462963</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109">
@@ -2539,13 +2563,211 @@
         <v>52</v>
       </c>
       <c r="C110" s="2">
-        <v>45913.032546296294</v>
+        <v>45907.019560185188</v>
       </c>
       <c r="D110" s="2">
-        <v>45914.002326388887</v>
+        <v>45908.010844907411</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A111" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" t="s">
+        <v>52</v>
+      </c>
+      <c r="C111" s="2">
+        <v>45913.032546296294</v>
+      </c>
+      <c r="D111" s="2">
+        <v>45914.002326388887</v>
+      </c>
+      <c r="E111" s="2"/>
+      <c r="F111">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A112" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" t="s">
+        <v>51</v>
+      </c>
+      <c r="C112" s="2">
+        <v>45906.993020833332</v>
+      </c>
+      <c r="D112" s="2">
+        <v>45907.99009259259</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="F112">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A113" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" s="2">
+        <v>45905.558854166666</v>
+      </c>
+      <c r="D113" s="2">
+        <v>45906.555868055555</v>
+      </c>
+      <c r="E113" s="2"/>
+      <c r="F113">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A114" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="2">
+        <v>45909.531261574077</v>
+      </c>
+      <c r="D114" s="2">
+        <v>45910.523888888885</v>
+      </c>
+      <c r="E114" s="2"/>
+      <c r="F114">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A115" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" t="s">
+        <v>57</v>
+      </c>
+      <c r="C115" s="2">
+        <v>45913.030231481483</v>
+      </c>
+      <c r="D115" s="2">
+        <v>45914.003888888888</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A116" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116" t="s">
+        <v>49</v>
+      </c>
+      <c r="C116" s="2">
+        <v>45905.028263888889</v>
+      </c>
+      <c r="D116" s="2">
+        <v>45906.015115740738</v>
+      </c>
+      <c r="E116" s="2"/>
+      <c r="F116">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A117" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117" t="s">
+        <v>45</v>
+      </c>
+      <c r="C117" s="2">
+        <v>45905.033067129632</v>
+      </c>
+      <c r="D117" s="2">
+        <v>45906.00104166667</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A118" t="s">
+        <v>6</v>
+      </c>
+      <c r="B118" t="s">
+        <v>45</v>
+      </c>
+      <c r="C118" s="2">
+        <v>45910.584328703706</v>
+      </c>
+      <c r="D118" s="2">
+        <v>45911.616053240738</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A119" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C119" s="2">
+        <v>45906.572326388887</v>
+      </c>
+      <c r="D119" s="2">
+        <v>45907.549814814818</v>
+      </c>
+      <c r="E119" s="2"/>
+      <c r="F119">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120" t="s">
+        <v>6</v>
+      </c>
+      <c r="B120" t="s">
+        <v>28</v>
+      </c>
+      <c r="C120" s="2">
+        <v>45910.041087962964</v>
+      </c>
+      <c r="D120" s="2">
+        <v>45911.026550925926</v>
+      </c>
+      <c r="E120" s="2"/>
+      <c r="F120">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121" t="s">
+        <v>39</v>
+      </c>
+      <c r="C121" s="2">
+        <v>45913.029675925929</v>
+      </c>
+      <c r="D121" s="2">
+        <v>45914.000960648147</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-17  8:19:04.95
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="69">
   <si>
     <t>电站名称</t>
   </si>
@@ -163,12 +163,6 @@
     <t>A04号直流</t>
   </si>
   <si>
-    <t>704号直流</t>
-  </si>
-  <si>
-    <t>A05号直流</t>
-  </si>
-  <si>
     <t>203号直流</t>
   </si>
   <si>
@@ -199,15 +193,6 @@
     <t>107号直流</t>
   </si>
   <si>
-    <t>109号直流</t>
-  </si>
-  <si>
-    <t>208号直流</t>
-  </si>
-  <si>
-    <t>302号直流</t>
-  </si>
-  <si>
     <t>111号直流</t>
   </si>
   <si>
@@ -233,6 +218,12 @@
   </si>
   <si>
     <t>006B号直流</t>
+  </si>
+  <si>
+    <t>A03号直流</t>
+  </si>
+  <si>
+    <t>804号直流</t>
   </si>
 </sst>
 </file>
@@ -596,10 +587,13 @@
   <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -623,128 +617,128 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
-        <v>45907.567233796297</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45915.492719907408</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>45908.603506944448</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F2">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2">
-        <v>45908.603506944448</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45907.567233796297</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45915.492719907408</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="F3">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2">
-        <v>45906.578356481485</v>
+        <v>45908.550717592596</v>
       </c>
       <c r="D4" s="2">
-        <v>45913.004490740743</v>
+        <v>45913.021585648145</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4">
-        <v>155</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2">
-        <v>45908.550717592596</v>
+        <v>45909.602083333331</v>
       </c>
       <c r="D5" s="2">
-        <v>45913.021585648145</v>
+        <v>45914.000115740739</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>45909.602083333331</v>
+        <v>45909.236574074072</v>
       </c>
       <c r="D6" s="2">
-        <v>45914.000115740739</v>
+        <v>45913.535138888888</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2">
-        <v>45909.236574074072</v>
+        <v>45911.52857638889</v>
       </c>
       <c r="D7" s="2">
-        <v>45913.535138888888</v>
+        <v>45915.503275462965</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2">
-        <v>45911.52857638889</v>
+        <v>45909.053182870368</v>
       </c>
       <c r="D8" s="2">
-        <v>45915.503275462965</v>
+        <v>45912.756840277776</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -752,107 +746,107 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
-        <v>45909.053182870368</v>
+        <v>45908.525706018518</v>
       </c>
       <c r="D9" s="2">
-        <v>45912.756840277776</v>
+        <v>45912.034201388888</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2">
-        <v>45905.534791666665</v>
+        <v>45913.650914351849</v>
       </c>
       <c r="D10" s="2">
-        <v>45909.203703703701</v>
+        <v>45917.025937500002</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
-        <v>45908.525706018518</v>
+        <v>45913.052685185183</v>
       </c>
       <c r="D11" s="2">
-        <v>45912.034201388888</v>
+        <v>45916.265127314815</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2">
-        <v>45905.263715277775</v>
+        <v>45907.570555555554</v>
       </c>
       <c r="D12" s="2">
-        <v>45908.553703703707</v>
+        <v>45910.500289351854</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2">
-        <v>45913.052685185183</v>
+        <v>45914.186030092591</v>
       </c>
       <c r="D13" s="2">
-        <v>45916.265127314815</v>
+        <v>45917.006539351853</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2">
-        <v>45906.271747685183</v>
+        <v>45910.540219907409</v>
       </c>
       <c r="D14" s="2">
-        <v>45909.218194444446</v>
+        <v>45913.224270833336</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -860,35 +854,35 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2">
-        <v>45907.570555555554</v>
+        <v>45912.328969907408</v>
       </c>
       <c r="D15" s="2">
-        <v>45910.500289351854</v>
+        <v>45915.001701388886</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2">
-        <v>45913.650914351849</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45910.021134259259</v>
+      </c>
+      <c r="D16" s="2">
+        <v>45912.686157407406</v>
+      </c>
+      <c r="E16" s="2"/>
       <c r="F16">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -896,35 +890,35 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2">
-        <v>45912.328969907408</v>
+        <v>45913.006967592592</v>
       </c>
       <c r="D17" s="2">
-        <v>45915.001701388886</v>
+        <v>45915.473703703705</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2">
-        <v>45910.540219907409</v>
+        <v>45907.401435185187</v>
       </c>
       <c r="D18" s="2">
-        <v>45913.224270833336</v>
+        <v>45909.52579861111</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -932,35 +926,35 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C19" s="2">
-        <v>45910.021134259259</v>
+        <v>45908.552488425928</v>
       </c>
       <c r="D19" s="2">
-        <v>45912.686157407406</v>
+        <v>45910.652662037035</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2">
-        <v>45913.006967592592</v>
+        <v>45910.355798611112</v>
       </c>
       <c r="D20" s="2">
-        <v>45915.473703703705</v>
+        <v>45912.393368055556</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -968,197 +962,197 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2">
-        <v>45906.25440972222</v>
+        <v>45907.522546296299</v>
       </c>
       <c r="D21" s="2">
-        <v>45908.543657407405</v>
+        <v>45909.570775462962</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2">
-        <v>45914.186030092591</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45911.040381944447</v>
+      </c>
+      <c r="D22" s="2">
+        <v>45913.023263888892</v>
+      </c>
+      <c r="E22" s="2"/>
       <c r="F22">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="2">
-        <v>45907.401435185187</v>
+        <v>45908.570474537039</v>
       </c>
       <c r="D23" s="2">
-        <v>45909.52579861111</v>
+        <v>45910.550486111111</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2">
-        <v>45908.552488425928</v>
+        <v>45910.561724537038</v>
       </c>
       <c r="D24" s="2">
-        <v>45910.652662037035</v>
+        <v>45912.509375000001</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C25" s="2">
-        <v>45905.060277777775</v>
+        <v>45910.5781712963</v>
       </c>
       <c r="D25" s="2">
-        <v>45907.134097222224</v>
+        <v>45912.528969907406</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2">
-        <v>45907.522546296299</v>
+        <v>45908.082407407404</v>
       </c>
       <c r="D26" s="2">
-        <v>45909.570775462962</v>
+        <v>45910.006041666667</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2">
-        <v>45910.355798611112</v>
+        <v>45912.060983796298</v>
       </c>
       <c r="D27" s="2">
-        <v>45912.393368055556</v>
+        <v>45914.012141203704</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C28" s="2">
-        <v>45911.040381944447</v>
+        <v>45914.560046296298</v>
       </c>
       <c r="D28" s="2">
-        <v>45913.023263888892</v>
+        <v>45916.478472222225</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C29" s="2">
-        <v>45908.570474537039</v>
+        <v>45911.562384259261</v>
       </c>
       <c r="D29" s="2">
-        <v>45910.550486111111</v>
+        <v>45913.435532407406</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C30" s="2">
-        <v>45908.082407407404</v>
+        <v>45911.646747685183</v>
       </c>
       <c r="D30" s="2">
-        <v>45910.006041666667</v>
+        <v>45913.523923611108</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C31" s="2">
-        <v>45910.5781712963</v>
-      </c>
-      <c r="D31" s="2">
-        <v>45912.528969907406</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>45915.503680555557</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F31">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -1166,71 +1160,71 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2">
-        <v>45912.060983796298</v>
+        <v>45915.231793981482</v>
       </c>
       <c r="D32" s="2">
-        <v>45914.012141203704</v>
+        <v>45917.019432870373</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2">
-        <v>45906.549328703702</v>
+        <v>45913.76421296296</v>
       </c>
       <c r="D33" s="2">
-        <v>45908.533761574072</v>
+        <v>45915.539942129632</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C34" s="2">
-        <v>45910.561724537038</v>
-      </c>
-      <c r="D34" s="2">
-        <v>45912.509375000001</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>45915.583414351851</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F34">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C35" s="2">
-        <v>45905.58865740741</v>
+        <v>45909.261608796296</v>
       </c>
       <c r="D35" s="2">
-        <v>45907.541539351849</v>
+        <v>45911.001076388886</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
@@ -1238,35 +1232,35 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36" s="2">
-        <v>45906.091840277775</v>
+        <v>45913.23265046296</v>
       </c>
       <c r="D36" s="2">
-        <v>45908.0002662037</v>
+        <v>45914.981087962966</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C37" s="2">
-        <v>45911.646747685183</v>
+        <v>45909.799317129633</v>
       </c>
       <c r="D37" s="2">
-        <v>45913.523923611108</v>
+        <v>45911.513888888891</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -1274,35 +1268,35 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C38" s="2">
-        <v>45911.562384259261</v>
+        <v>45914.040277777778</v>
       </c>
       <c r="D38" s="2">
-        <v>45913.435532407406</v>
+        <v>45915.733287037037</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="2">
-        <v>45914.560046296298</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45911.531018518515</v>
+      </c>
+      <c r="D39" s="2">
+        <v>45913.206875000003</v>
+      </c>
+      <c r="E39" s="2"/>
       <c r="F39">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -1310,125 +1304,125 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C40" s="2">
-        <v>45913.23265046296</v>
+        <v>45915.111643518518</v>
       </c>
       <c r="D40" s="2">
-        <v>45914.981087962966</v>
+        <v>45916.694467592592</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="C41" s="2">
-        <v>45913.76421296296</v>
+        <v>45907.705949074072</v>
       </c>
       <c r="D41" s="2">
-        <v>45915.539942129632</v>
+        <v>45909.21980324074</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C42" s="2">
-        <v>45909.261608796296</v>
+        <v>45914.486261574071</v>
       </c>
       <c r="D42" s="2">
-        <v>45911.001076388886</v>
+        <v>45916.002962962964</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C43" s="2">
-        <v>45914.040277777778</v>
+        <v>45915.025833333333</v>
       </c>
       <c r="D43" s="2">
-        <v>45915.733287037037</v>
+        <v>45916.511203703703</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C44" s="2">
-        <v>45909.799317129633</v>
+        <v>45915.061967592592</v>
       </c>
       <c r="D44" s="2">
-        <v>45911.513888888891</v>
+        <v>45916.546516203707</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C45" s="2">
-        <v>45911.531018518515</v>
+        <v>45907.729745370372</v>
       </c>
       <c r="D45" s="2">
-        <v>45913.206875000003</v>
+        <v>45909.231006944443</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="C46" s="2">
-        <v>45906.348958333336</v>
+        <v>45908.210324074076</v>
       </c>
       <c r="D46" s="2">
-        <v>45908.012199074074</v>
+        <v>45909.712118055555</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
@@ -1436,17 +1430,17 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C47" s="2">
-        <v>45914.486261574071</v>
+        <v>45910.534502314818</v>
       </c>
       <c r="D47" s="2">
-        <v>45916.002962962964</v>
+        <v>45912.012048611112</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
@@ -1454,17 +1448,17 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C48" s="2">
-        <v>45907.705949074072</v>
+        <v>45908.058252314811</v>
       </c>
       <c r="D48" s="2">
-        <v>45909.21980324074</v>
+        <v>45909.559004629627</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
@@ -1472,13 +1466,13 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C49" s="2">
-        <v>45908.210324074076</v>
+        <v>45909.579212962963</v>
       </c>
       <c r="D49" s="2">
-        <v>45909.712118055555</v>
+        <v>45911.07608796296</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49">
@@ -1487,20 +1481,20 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C50" s="2">
-        <v>45910.534502314818</v>
+        <v>45912.567314814813</v>
       </c>
       <c r="D50" s="2">
-        <v>45912.012048611112</v>
+        <v>45914.04074074074</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
@@ -1508,17 +1502,17 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C51" s="2">
-        <v>45908.058252314811</v>
+        <v>45913.566805555558</v>
       </c>
       <c r="D51" s="2">
-        <v>45909.559004629627</v>
+        <v>45915.004942129628</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
@@ -1526,53 +1520,53 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C52" s="2">
-        <v>45909.579212962963</v>
+        <v>45913.717233796298</v>
       </c>
       <c r="D52" s="2">
-        <v>45911.07608796296</v>
+        <v>45915.203182870369</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C53" s="2">
-        <v>45907.729745370372</v>
+        <v>45908.562800925924</v>
       </c>
       <c r="D53" s="2">
-        <v>45909.231006944443</v>
+        <v>45910.003263888888</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C54" s="2">
-        <v>45912.567314814813</v>
+        <v>45914.050219907411</v>
       </c>
       <c r="D54" s="2">
-        <v>45914.04074074074</v>
+        <v>45915.466817129629</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -1580,179 +1574,179 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C55" s="2">
-        <v>45906.065810185188</v>
+        <v>45915.541979166665</v>
       </c>
       <c r="D55" s="2">
-        <v>45907.50099537037</v>
+        <v>45916.988449074073</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="C56" s="2">
-        <v>45913.566805555558</v>
+        <v>45912.627604166664</v>
       </c>
       <c r="D56" s="2">
-        <v>45915.004942129628</v>
+        <v>45914.005208333336</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C57" s="2">
-        <v>45908.562800925924</v>
+        <v>45909.039467592593</v>
       </c>
       <c r="D57" s="2">
-        <v>45910.003263888888</v>
+        <v>45910.373379629629</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C58" s="2">
-        <v>45913.717233796298</v>
+        <v>45907.194444444445</v>
       </c>
       <c r="D58" s="2">
-        <v>45915.203182870369</v>
+        <v>45908.530740740738</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C59" s="2">
-        <v>45906.573877314811</v>
+        <v>45910.054398148146</v>
       </c>
       <c r="D59" s="2">
-        <v>45908.008958333332</v>
+        <v>45911.384293981479</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C60" s="2">
-        <v>45914.050219907411</v>
-      </c>
-      <c r="D60" s="2">
-        <v>45915.466817129629</v>
-      </c>
-      <c r="E60" s="2"/>
+        <v>45916.041956018518</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F60">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C61" s="2">
-        <v>45915.025833333333</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45910.247546296298</v>
+      </c>
+      <c r="D61" s="2">
+        <v>45911.529826388891</v>
+      </c>
+      <c r="E61" s="2"/>
       <c r="F61">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C62" s="2">
-        <v>45906.087141203701</v>
+        <v>45907.24454861111</v>
       </c>
       <c r="D62" s="2">
-        <v>45907.494085648148</v>
+        <v>45908.508622685185</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C63" s="2">
-        <v>45912.627604166664</v>
+        <v>45910.029456018521</v>
       </c>
       <c r="D63" s="2">
-        <v>45914.005208333336</v>
+        <v>45911.331701388888</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C64" s="2">
-        <v>45915.061967592592</v>
-      </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45915.259062500001</v>
+      </c>
+      <c r="D64" s="2">
+        <v>45916.545428240737</v>
+      </c>
+      <c r="E64" s="2"/>
       <c r="F64">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
@@ -1760,35 +1754,35 @@
         <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C65" s="2">
-        <v>45910.054398148146</v>
-      </c>
-      <c r="D65" s="2">
-        <v>45911.384293981479</v>
-      </c>
-      <c r="E65" s="2"/>
+        <v>45916.051249999997</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F65">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C66" s="2">
-        <v>45909.039467592593</v>
-      </c>
-      <c r="D66" s="2">
-        <v>45910.373379629629</v>
-      </c>
-      <c r="E66" s="2"/>
+        <v>45916.059074074074</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F66">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
@@ -1796,53 +1790,53 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C67" s="2">
-        <v>45907.194444444445</v>
+        <v>45909.260914351849</v>
       </c>
       <c r="D67" s="2">
-        <v>45908.530740740738</v>
+        <v>45910.524594907409</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C68" s="2">
-        <v>45906.810439814813</v>
+        <v>45914.304675925923</v>
       </c>
       <c r="D68" s="2">
-        <v>45908.090266203704</v>
+        <v>45915.505648148152</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C69" s="2">
-        <v>45910.029456018521</v>
+        <v>45914.064189814817</v>
       </c>
       <c r="D69" s="2">
-        <v>45911.331701388888</v>
+        <v>45915.274594907409</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
@@ -1850,17 +1844,17 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C70" s="2">
-        <v>45910.247546296298</v>
+        <v>45913.050844907404</v>
       </c>
       <c r="D70" s="2">
-        <v>45911.529826388891</v>
+        <v>45914.284895833334</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
@@ -1868,17 +1862,17 @@
         <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C71" s="2">
-        <v>45906.221956018519</v>
+        <v>45910.067824074074</v>
       </c>
       <c r="D71" s="2">
-        <v>45907.510810185187</v>
+        <v>45911.284560185188</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
@@ -1886,17 +1880,17 @@
         <v>6</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="C72" s="2">
-        <v>45915.111643518518</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45915.250428240739</v>
+      </c>
+      <c r="D72" s="2">
+        <v>45916.492291666669</v>
+      </c>
+      <c r="E72" s="2"/>
       <c r="F72">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
@@ -1904,35 +1898,35 @@
         <v>6</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C73" s="2">
-        <v>45907.24454861111</v>
+        <v>45907.051342592589</v>
       </c>
       <c r="D73" s="2">
-        <v>45908.508622685185</v>
+        <v>45908.250138888892</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="C74" s="2">
-        <v>45905.7655787037</v>
+        <v>45907.048576388886</v>
       </c>
       <c r="D74" s="2">
-        <v>45907.012766203705</v>
+        <v>45908.228101851855</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
@@ -1940,35 +1934,35 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C75" s="2">
-        <v>45909.260914351849</v>
+        <v>45909.373738425929</v>
       </c>
       <c r="D75" s="2">
-        <v>45910.524594907409</v>
+        <v>45910.524085648147</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B76" t="s">
         <v>13</v>
       </c>
       <c r="C76" s="2">
-        <v>45914.064189814817</v>
+        <v>45914.060752314814</v>
       </c>
       <c r="D76" s="2">
-        <v>45915.274594907409</v>
+        <v>45915.225474537037</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
@@ -1976,17 +1970,17 @@
         <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C77" s="2">
-        <v>45913.050844907404</v>
+        <v>45914.011388888888</v>
       </c>
       <c r="D77" s="2">
-        <v>45914.284895833334</v>
+        <v>45915.187569444446</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
@@ -1994,17 +1988,17 @@
         <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C78" s="2">
-        <v>45907.051342592589</v>
+        <v>45910.356319444443</v>
       </c>
       <c r="D78" s="2">
-        <v>45908.250138888892</v>
+        <v>45911.500925925924</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
@@ -2012,35 +2006,35 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C79" s="2">
-        <v>45910.067824074074</v>
+        <v>45907.389652777776</v>
       </c>
       <c r="D79" s="2">
-        <v>45911.284560185188</v>
+        <v>45908.550567129627</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C80" s="2">
-        <v>45914.304675925923</v>
+        <v>45915.035682870373</v>
       </c>
       <c r="D80" s="2">
-        <v>45915.505648148152</v>
+        <v>45916.204282407409</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
@@ -2048,35 +2042,35 @@
         <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C81" s="2">
-        <v>45907.048576388886</v>
+        <v>45911.012094907404</v>
       </c>
       <c r="D81" s="2">
-        <v>45908.228101851855</v>
+        <v>45912.137696759259</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C82" s="2">
-        <v>45905.566099537034</v>
+        <v>45913.042430555557</v>
       </c>
       <c r="D82" s="2">
-        <v>45906.734594907408</v>
+        <v>45914.200810185182</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
@@ -2084,17 +2078,17 @@
         <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C83" s="2">
-        <v>45914.011388888888</v>
+        <v>45913.579629629632</v>
       </c>
       <c r="D83" s="2">
-        <v>45915.187569444446</v>
+        <v>45914.686932870369</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
@@ -2102,17 +2096,17 @@
         <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C84" s="2">
-        <v>45915.035682870373</v>
+        <v>45914.045497685183</v>
       </c>
       <c r="D84" s="2">
-        <v>45916.204282407409</v>
+        <v>45915.202696759261</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
@@ -2120,17 +2114,17 @@
         <v>6</v>
       </c>
       <c r="B85" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C85" s="2">
-        <v>45907.389652777776</v>
+        <v>45915.075706018521</v>
       </c>
       <c r="D85" s="2">
-        <v>45908.550567129627</v>
+        <v>45916.188900462963</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
@@ -2138,17 +2132,17 @@
         <v>6</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C86" s="2">
-        <v>45915.231793981482</v>
-      </c>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45907.094305555554</v>
+      </c>
+      <c r="D86" s="2">
+        <v>45908.213356481479</v>
+      </c>
+      <c r="E86" s="2"/>
       <c r="F86">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
@@ -2156,53 +2150,53 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C87" s="2">
-        <v>45910.356319444443</v>
+        <v>45909.091203703705</v>
       </c>
       <c r="D87" s="2">
-        <v>45911.500925925924</v>
+        <v>45910.220127314817</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="C88" s="2">
-        <v>45909.373738425929</v>
+        <v>45914.151493055557</v>
       </c>
       <c r="D88" s="2">
-        <v>45910.524085648147</v>
+        <v>45915.287997685184</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C89" s="2">
-        <v>45914.060752314814</v>
+        <v>45912.041076388887</v>
       </c>
       <c r="D89" s="2">
-        <v>45915.225474537037</v>
+        <v>45913.145925925928</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
@@ -2210,89 +2204,89 @@
         <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C90" s="2">
-        <v>45911.012094907404</v>
+        <v>45909.514016203706</v>
       </c>
       <c r="D90" s="2">
-        <v>45912.137696759259</v>
+        <v>45910.611180555556</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C91" s="2">
-        <v>45909.091203703705</v>
+        <v>45913.064467592594</v>
       </c>
       <c r="D91" s="2">
-        <v>45910.220127314817</v>
+        <v>45914.140983796293</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="C92" s="2">
-        <v>45913.579629629632</v>
-      </c>
-      <c r="D92" s="2">
-        <v>45914.686932870369</v>
-      </c>
-      <c r="E92" s="2"/>
+        <v>45916.28261574074</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F92">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C93" s="2">
-        <v>45907.094305555554</v>
+        <v>45909.039143518516</v>
       </c>
       <c r="D93" s="2">
-        <v>45908.213356481479</v>
+        <v>45910.102083333331</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C94" s="2">
-        <v>45915.075706018521</v>
+        <v>45907.134444444448</v>
       </c>
       <c r="D94" s="2">
-        <v>45916.188900462963</v>
+        <v>45908.224537037036</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.15">
@@ -2300,143 +2294,143 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C95" s="2">
-        <v>45914.151493055557</v>
+        <v>45908.118969907409</v>
       </c>
       <c r="D95" s="2">
-        <v>45915.287997685184</v>
+        <v>45909.179571759261</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B96" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C96" s="2">
-        <v>45906.042974537035</v>
+        <v>45915.525405092594</v>
       </c>
       <c r="D96" s="2">
-        <v>45907.169976851852</v>
+        <v>45916.54210648148</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C97" s="2">
-        <v>45915.250428240739</v>
-      </c>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2">
-        <v>45916.395532407405</v>
-      </c>
+        <v>45909.239444444444</v>
+      </c>
+      <c r="D97" s="2">
+        <v>45910.265706018516</v>
+      </c>
+      <c r="E97" s="2"/>
       <c r="F97">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B98" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C98" s="2">
-        <v>45906.575902777775</v>
+        <v>45911.244166666664</v>
       </c>
       <c r="D98" s="2">
-        <v>45907.67150462963</v>
+        <v>45912.265601851854</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B99" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C99" s="2">
-        <v>45912.041076388887</v>
+        <v>45911.504976851851</v>
       </c>
       <c r="D99" s="2">
-        <v>45913.145925925928</v>
+        <v>45912.543333333335</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B100" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" s="2">
+        <v>45914.036979166667</v>
+      </c>
+      <c r="D100" s="2">
+        <v>45915.079004629632</v>
+      </c>
+      <c r="E100" s="2"/>
+      <c r="F100">
         <v>25</v>
-      </c>
-      <c r="C100" s="2">
-        <v>45915.259062500001</v>
-      </c>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2">
-        <v>45916.395532407405</v>
-      </c>
-      <c r="F100">
-        <v>27</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B101" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C101" s="2">
-        <v>45914.045497685183</v>
+        <v>45910.196134259262</v>
       </c>
       <c r="D101" s="2">
-        <v>45915.202696759261</v>
+        <v>45911.248784722222</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C102" s="2">
-        <v>45913.042430555557</v>
+        <v>45908.19803240741</v>
       </c>
       <c r="D102" s="2">
-        <v>45914.200810185182</v>
+        <v>45909.213159722225</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.15">
@@ -2444,17 +2438,17 @@
         <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C103" s="2">
-        <v>45913.064467592594</v>
+        <v>45908.567731481482</v>
       </c>
       <c r="D103" s="2">
-        <v>45914.140983796293</v>
+        <v>45909.606053240743</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
@@ -2462,35 +2456,35 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C104" s="2">
-        <v>45909.514016203706</v>
+        <v>45907.620358796295</v>
       </c>
       <c r="D104" s="2">
-        <v>45910.611180555556</v>
+        <v>45908.656805555554</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C105" s="2">
-        <v>45908.118969907409</v>
+        <v>45913.021006944444</v>
       </c>
       <c r="D105" s="2">
-        <v>45909.179571759261</v>
+        <v>45914.078969907408</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.15">
@@ -2498,67 +2492,67 @@
         <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C106" s="2">
-        <v>45906.047337962962</v>
+        <v>45908.570671296293</v>
       </c>
       <c r="D106" s="2">
-        <v>45907.137569444443</v>
+        <v>45909.609884259262</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C107" s="2">
-        <v>45909.039143518516</v>
+        <v>45911.684641203705</v>
       </c>
       <c r="D107" s="2">
-        <v>45910.102083333331</v>
+        <v>45912.726527777777</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C108" s="2">
-        <v>45907.134444444448</v>
+        <v>45915.475578703707</v>
       </c>
       <c r="D108" s="2">
-        <v>45908.224537037036</v>
+        <v>45916.538958333331</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C109" s="2">
-        <v>45910.196134259262</v>
+        <v>45912.043020833335</v>
       </c>
       <c r="D109" s="2">
-        <v>45911.248784722222</v>
+        <v>45913.113923611112</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109">
@@ -2567,16 +2561,16 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C110" s="2">
-        <v>45907.620358796295</v>
+        <v>45911.994386574072</v>
       </c>
       <c r="D110" s="2">
-        <v>45908.656805555554</v>
+        <v>45913.008622685185</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110">
@@ -2585,16 +2579,16 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C111" s="2">
-        <v>45914.036979166667</v>
+        <v>45915.483831018515</v>
       </c>
       <c r="D111" s="2">
-        <v>45915.079004629632</v>
+        <v>45916.511701388888</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111">
@@ -2603,16 +2597,16 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B112" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C112" s="2">
-        <v>45905.577847222223</v>
+        <v>45915.055277777778</v>
       </c>
       <c r="D112" s="2">
-        <v>45906.623020833336</v>
+        <v>45916.095949074072</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112">
@@ -2621,232 +2615,232 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C113" s="2">
-        <v>45908.19803240741</v>
+        <v>45913.530856481484</v>
       </c>
       <c r="D113" s="2">
-        <v>45909.213159722225</v>
+        <v>45914.507928240739</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C114" s="2">
-        <v>45908.567731481482</v>
+        <v>45912.242094907408</v>
       </c>
       <c r="D114" s="2">
-        <v>45909.606053240743</v>
+        <v>45913.231030092589</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B115" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C115" s="2">
-        <v>45911.684641203705</v>
-      </c>
-      <c r="D115" s="2">
-        <v>45912.726527777777</v>
-      </c>
-      <c r="E115" s="2"/>
+        <v>45916.350173611114</v>
+      </c>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F115">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B116" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C116" s="2">
-        <v>45915.055277777778</v>
+        <v>45912.03328703704</v>
       </c>
       <c r="D116" s="2">
-        <v>45916.095949074072</v>
+        <v>45913.003379629627</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B117" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C117" s="2">
-        <v>45912.043020833335</v>
+        <v>45907.019560185188</v>
       </c>
       <c r="D117" s="2">
-        <v>45913.113923611112</v>
+        <v>45908.010844907411</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B118" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C118" s="2">
-        <v>45911.994386574072</v>
+        <v>45913.032546296294</v>
       </c>
       <c r="D118" s="2">
-        <v>45913.008622685185</v>
+        <v>45914.002326388887</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C119" s="2">
-        <v>45908.570671296293</v>
+        <v>45909.029490740744</v>
       </c>
       <c r="D119" s="2">
-        <v>45909.609884259262</v>
+        <v>45910.00445601852</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B120" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C120" s="2">
-        <v>45909.239444444444</v>
+        <v>45911.556932870371</v>
       </c>
       <c r="D120" s="2">
-        <v>45910.265706018516</v>
+        <v>45912.543055555558</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B121" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="C121" s="2">
-        <v>45911.244166666664</v>
+        <v>45916.019108796296</v>
       </c>
       <c r="D121" s="2">
-        <v>45912.265601851854</v>
+        <v>45917.00277777778</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B122" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C122" s="2">
-        <v>45911.504976851851</v>
+        <v>45910.02920138889</v>
       </c>
       <c r="D122" s="2">
-        <v>45912.543333333335</v>
+        <v>45911.005185185182</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B123" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C123" s="2">
-        <v>45906.5156712963</v>
+        <v>45911.034571759257</v>
       </c>
       <c r="D123" s="2">
-        <v>45907.565092592595</v>
+        <v>45912.001400462963</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B124" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C124" s="2">
-        <v>45913.021006944444</v>
+        <v>45914.0625</v>
       </c>
       <c r="D124" s="2">
-        <v>45914.078969907408</v>
+        <v>45915.059525462966</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B125" t="s">
         <v>13</v>
       </c>
       <c r="C125" s="2">
-        <v>45911.556932870371</v>
+        <v>45915.540833333333</v>
       </c>
       <c r="D125" s="2">
-        <v>45912.543055555558</v>
+        <v>45916.513043981482</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125">
@@ -2855,16 +2849,16 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B126" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C126" s="2">
-        <v>45912.03328703704</v>
+        <v>45908.923564814817</v>
       </c>
       <c r="D126" s="2">
-        <v>45913.003379629627</v>
+        <v>45909.953576388885</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126">
@@ -2873,16 +2867,16 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C127" s="2">
-        <v>45907.019560185188</v>
+        <v>45915.55263888889</v>
       </c>
       <c r="D127" s="2">
-        <v>45908.010844907411</v>
+        <v>45916.542962962965</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127">
@@ -2891,16 +2885,16 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C128" s="2">
-        <v>45913.032546296294</v>
+        <v>45914.043333333335</v>
       </c>
       <c r="D128" s="2">
-        <v>45914.002326388887</v>
+        <v>45915.064780092594</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128">
@@ -2909,16 +2903,16 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C129" s="2">
-        <v>45909.029490740744</v>
+        <v>45914.019074074073</v>
       </c>
       <c r="D129" s="2">
-        <v>45910.00445601852</v>
+        <v>45915.000347222223</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129">
@@ -2927,16 +2921,16 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C130" s="2">
-        <v>45910.02920138889</v>
+        <v>45907.041504629633</v>
       </c>
       <c r="D130" s="2">
-        <v>45911.005185185182</v>
+        <v>45908.003831018519</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130">
@@ -2945,16 +2939,16 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B131" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C131" s="2">
-        <v>45911.034571759257</v>
+        <v>45909.532372685186</v>
       </c>
       <c r="D131" s="2">
-        <v>45912.001400462963</v>
+        <v>45910.502280092594</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131">
@@ -2963,16 +2957,16 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B132" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C132" s="2">
-        <v>45914.0625</v>
+        <v>45910.510555555556</v>
       </c>
       <c r="D132" s="2">
-        <v>45915.059525462966</v>
+        <v>45911.524016203701</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132">
@@ -2984,13 +2978,13 @@
         <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C133" s="2">
-        <v>45913.030231481483</v>
+        <v>45915.220127314817</v>
       </c>
       <c r="D133" s="2">
-        <v>45914.003888888888</v>
+        <v>45916.216979166667</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133">
@@ -3002,13 +2996,13 @@
         <v>6</v>
       </c>
       <c r="B134" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C134" s="2">
-        <v>45915.220127314817</v>
+        <v>45910.041087962964</v>
       </c>
       <c r="D134" s="2">
-        <v>45916.216979166667</v>
+        <v>45911.026550925926</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134">
@@ -3020,13 +3014,13 @@
         <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C135" s="2">
-        <v>45915.020277777781</v>
+        <v>45915.572175925925</v>
       </c>
       <c r="D135" s="2">
-        <v>45916.002210648148</v>
+        <v>45916.543171296296</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135">
@@ -3038,13 +3032,13 @@
         <v>6</v>
       </c>
       <c r="B136" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C136" s="2">
-        <v>45906.993020833332</v>
+        <v>45909.531261574077</v>
       </c>
       <c r="D136" s="2">
-        <v>45907.99009259259</v>
+        <v>45910.523888888885</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136">
@@ -3056,13 +3050,13 @@
         <v>6</v>
       </c>
       <c r="B137" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C137" s="2">
-        <v>45906.572326388887</v>
+        <v>45913.030231481483</v>
       </c>
       <c r="D137" s="2">
-        <v>45907.549814814818</v>
+        <v>45914.003888888888</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137">
@@ -3074,13 +3068,13 @@
         <v>6</v>
       </c>
       <c r="B138" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C138" s="2">
-        <v>45910.041087962964</v>
+        <v>45913.701620370368</v>
       </c>
       <c r="D138" s="2">
-        <v>45911.026550925926</v>
+        <v>45914.694907407407</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138">
@@ -3092,13 +3086,13 @@
         <v>6</v>
       </c>
       <c r="B139" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C139" s="2">
-        <v>45905.033067129632</v>
+        <v>45915.020277777781</v>
       </c>
       <c r="D139" s="2">
-        <v>45906.00104166667</v>
+        <v>45916.002210648148</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139">
@@ -3128,15 +3122,15 @@
         <v>6</v>
       </c>
       <c r="B141" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="C141" s="2">
-        <v>45913.029675925929</v>
-      </c>
-      <c r="D141" s="2">
-        <v>45914.000960648147</v>
-      </c>
-      <c r="E141" s="2"/>
+        <v>45916.352418981478</v>
+      </c>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2">
+        <v>45917.338078703702</v>
+      </c>
       <c r="F141">
         <v>24</v>
       </c>
@@ -3146,13 +3140,13 @@
         <v>6</v>
       </c>
       <c r="B142" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C142" s="2">
-        <v>45909.531261574077</v>
+        <v>45913.029675925929</v>
       </c>
       <c r="D142" s="2">
-        <v>45910.523888888885</v>
+        <v>45914.000960648147</v>
       </c>
       <c r="E142" s="2"/>
       <c r="F142">
@@ -3160,220 +3154,64 @@
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A143" t="s">
-        <v>6</v>
-      </c>
-      <c r="B143" t="s">
-        <v>67</v>
-      </c>
-      <c r="C143" s="2">
-        <v>45913.701620370368</v>
-      </c>
-      <c r="D143" s="2">
-        <v>45914.694907407407</v>
-      </c>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
       <c r="E143" s="2"/>
-      <c r="F143">
-        <v>24</v>
-      </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A144" t="s">
-        <v>6</v>
-      </c>
-      <c r="B144" t="s">
-        <v>19</v>
-      </c>
-      <c r="C144" s="2">
-        <v>45905.558854166666</v>
-      </c>
-      <c r="D144" s="2">
-        <v>45906.555868055555</v>
-      </c>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
       <c r="E144" s="2"/>
-      <c r="F144">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A145" t="s">
-        <v>6</v>
-      </c>
-      <c r="B145" t="s">
-        <v>49</v>
-      </c>
-      <c r="C145" s="2">
-        <v>45905.028263888889</v>
-      </c>
-      <c r="D145" s="2">
-        <v>45906.015115740738</v>
-      </c>
+    </row>
+    <row r="145" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
       <c r="E145" s="2"/>
-      <c r="F145">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A146" t="s">
-        <v>58</v>
-      </c>
-      <c r="B146" t="s">
-        <v>65</v>
-      </c>
-      <c r="C146" s="2">
-        <v>45912.242094907408</v>
-      </c>
-      <c r="D146" s="2">
-        <v>45913.231030092589</v>
-      </c>
+    </row>
+    <row r="146" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
       <c r="E146" s="2"/>
-      <c r="F146">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A147" t="s">
-        <v>58</v>
-      </c>
-      <c r="B147" t="s">
-        <v>50</v>
-      </c>
-      <c r="C147" s="2">
-        <v>45913.530856481484</v>
-      </c>
-      <c r="D147" s="2">
-        <v>45914.507928240739</v>
-      </c>
+    </row>
+    <row r="147" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
       <c r="E147" s="2"/>
-      <c r="F147">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A148" t="s">
-        <v>11</v>
-      </c>
-      <c r="B148" t="s">
-        <v>20</v>
-      </c>
-      <c r="C148" s="2">
-        <v>45908.923564814817</v>
-      </c>
-      <c r="D148" s="2">
-        <v>45909.953576388885</v>
-      </c>
+    </row>
+    <row r="148" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
       <c r="E148" s="2"/>
-      <c r="F148">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A149" t="s">
-        <v>11</v>
-      </c>
-      <c r="B149" t="s">
-        <v>29</v>
-      </c>
-      <c r="C149" s="2">
-        <v>45907.041504629633</v>
-      </c>
-      <c r="D149" s="2">
-        <v>45908.003831018519</v>
-      </c>
+    </row>
+    <row r="149" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
       <c r="E149" s="2"/>
-      <c r="F149">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A150" t="s">
-        <v>11</v>
-      </c>
-      <c r="B150" t="s">
-        <v>43</v>
-      </c>
-      <c r="C150" s="2">
-        <v>45914.019074074073</v>
-      </c>
-      <c r="D150" s="2">
-        <v>45915.000347222223</v>
-      </c>
+    </row>
+    <row r="150" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
       <c r="E150" s="2"/>
-      <c r="F150">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A151" t="s">
-        <v>11</v>
-      </c>
-      <c r="B151" t="s">
-        <v>71</v>
-      </c>
-      <c r="C151" s="2">
-        <v>45914.043333333335</v>
-      </c>
-      <c r="D151" s="2">
-        <v>45915.064780092594</v>
-      </c>
+    </row>
+    <row r="151" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
       <c r="E151" s="2"/>
-      <c r="F151">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A152" t="s">
-        <v>11</v>
-      </c>
-      <c r="B152" t="s">
-        <v>36</v>
-      </c>
-      <c r="C152" s="2">
-        <v>45909.532372685186</v>
-      </c>
-      <c r="D152" s="2">
-        <v>45910.502280092594</v>
-      </c>
+    </row>
+    <row r="152" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
       <c r="E152" s="2"/>
-      <c r="F152">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A153" t="s">
-        <v>11</v>
-      </c>
-      <c r="B153" t="s">
-        <v>36</v>
-      </c>
-      <c r="C153" s="2">
-        <v>45910.510555555556</v>
-      </c>
-      <c r="D153" s="2">
-        <v>45911.524016203701</v>
-      </c>
+    </row>
+    <row r="153" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
       <c r="E153" s="2"/>
-      <c r="F153">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A154" t="s">
-        <v>11</v>
-      </c>
-      <c r="B154" t="s">
-        <v>53</v>
-      </c>
-      <c r="C154" s="2">
-        <v>45906.520752314813</v>
-      </c>
-      <c r="D154" s="2">
-        <v>45907.527858796297</v>
-      </c>
+    </row>
+    <row r="154" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
       <c r="E154" s="2"/>
-      <c r="F154">
-        <v>24</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Auto commit at 2025-09-20  8:19:17.79
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="67">
   <si>
     <t>电站名称</t>
   </si>
@@ -115,9 +115,6 @@
     <t>105号直流</t>
   </si>
   <si>
-    <t>703号直流</t>
-  </si>
-  <si>
     <t>402号直流</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>106号直流</t>
   </si>
   <si>
-    <t>301号直流</t>
-  </si>
-  <si>
     <t>B04号直流</t>
   </si>
   <si>
@@ -215,6 +209,15 @@
   </si>
   <si>
     <t>305号直流</t>
+  </si>
+  <si>
+    <t>303号直流</t>
+  </si>
+  <si>
+    <t>302号直流</t>
+  </si>
+  <si>
+    <t>011A号直流</t>
   </si>
 </sst>
 </file>
@@ -575,17 +578,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="42.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.875" customWidth="1"/>
+    <col min="4" max="4" width="23.25" customWidth="1"/>
+    <col min="5" max="5" width="22.25" customWidth="1"/>
     <col min="6" max="6" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -603,7 +608,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -611,20 +616,20 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2">
-        <v>45909.602083333331</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45914.000115740739</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>45915.503680555557</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F2">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -632,17 +637,17 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2">
-        <v>45909.236574074072</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45913.535138888888</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>45916.28261574074</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F3">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -650,7 +655,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2">
         <v>45911.52857638889</v>
@@ -665,17 +670,17 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
-        <v>45915.503680555557</v>
+        <v>45916.534282407411</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>45919.361435185187</v>
+        <v>45920.341481481482</v>
       </c>
       <c r="F5">
         <v>92</v>
@@ -683,71 +688,71 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2">
-        <v>45909.053182870368</v>
+        <v>45913.650914351849</v>
       </c>
       <c r="D6" s="2">
-        <v>45912.756840277776</v>
+        <v>45917.025937500002</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
-        <v>45913.650914351849</v>
+        <v>45913.052685185183</v>
       </c>
       <c r="D7" s="2">
-        <v>45917.025937500002</v>
+        <v>45916.265127314815</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>45913.052685185183</v>
-      </c>
-      <c r="D8" s="2">
-        <v>45916.265127314815</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>45917.260844907411</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F8">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
-        <v>45916.28261574074</v>
+        <v>45917.258240740739</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
-        <v>45919.361435185187</v>
+        <v>45920.341481481482</v>
       </c>
       <c r="F9">
         <v>74</v>
@@ -776,17 +781,17 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2">
-        <v>45916.534282407411</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45910.540219907409</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45913.224270833336</v>
+      </c>
+      <c r="E11" s="2"/>
       <c r="F11">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
@@ -794,13 +799,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2">
-        <v>45910.540219907409</v>
+        <v>45912.328969907408</v>
       </c>
       <c r="D12" s="2">
-        <v>45913.224270833336</v>
+        <v>45915.001701388886</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12">
@@ -812,17 +817,17 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2">
-        <v>45912.328969907408</v>
+        <v>45910.021134259259</v>
       </c>
       <c r="D13" s="2">
-        <v>45915.001701388886</v>
+        <v>45912.686157407406</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -830,17 +835,17 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2">
-        <v>45910.021134259259</v>
+        <v>45913.006967592592</v>
       </c>
       <c r="D14" s="2">
-        <v>45912.686157407406</v>
+        <v>45915.473703703705</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -848,17 +853,17 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2">
-        <v>45913.006967592592</v>
-      </c>
-      <c r="D15" s="2">
-        <v>45915.473703703705</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>45918.06113425926</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F15">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -881,56 +886,56 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>45917.260844907411</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45910.355798611112</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45912.393368055556</v>
+      </c>
+      <c r="E17" s="2"/>
       <c r="F17">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2">
-        <v>45917.258240740739</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45911.040381944447</v>
+      </c>
+      <c r="D18" s="2">
+        <v>45913.023263888892</v>
+      </c>
+      <c r="E18" s="2"/>
       <c r="F18">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2">
-        <v>45910.355798611112</v>
+        <v>45912.060983796298</v>
       </c>
       <c r="D19" s="2">
-        <v>45912.393368055556</v>
+        <v>45914.012141203704</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -938,31 +943,31 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2">
-        <v>45911.040381944447</v>
+        <v>45915.583414351851</v>
       </c>
       <c r="D20" s="2">
-        <v>45913.023263888892</v>
+        <v>45917.582627314812</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2">
-        <v>45912.060983796298</v>
+        <v>45910.5781712963</v>
       </c>
       <c r="D21" s="2">
-        <v>45914.012141203704</v>
+        <v>45912.528969907406</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21">
@@ -971,10 +976,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="2">
         <v>45910.561724537038</v>
@@ -989,70 +994,70 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2">
-        <v>45915.583414351851</v>
+        <v>45914.560046296298</v>
       </c>
       <c r="D23" s="2">
-        <v>45917.582627314812</v>
+        <v>45916.478472222225</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2">
-        <v>45910.5781712963</v>
+        <v>45911.646747685183</v>
       </c>
       <c r="D24" s="2">
-        <v>45912.528969907406</v>
+        <v>45913.523923611108</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C25" s="2">
-        <v>45914.560046296298</v>
+        <v>45911.562384259261</v>
       </c>
       <c r="D25" s="2">
-        <v>45916.478472222225</v>
+        <v>45913.435532407406</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C26" s="2">
-        <v>45917.219965277778</v>
+        <v>45917.638888888891</v>
       </c>
       <c r="D26" s="2">
-        <v>45919.087418981479</v>
+        <v>45919.518240740741</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26">
@@ -1061,16 +1066,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2">
-        <v>45911.646747685183</v>
+        <v>45917.219965277778</v>
       </c>
       <c r="D27" s="2">
-        <v>45913.523923611108</v>
+        <v>45919.087418981479</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27">
@@ -1082,17 +1087,17 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2">
-        <v>45911.562384259261</v>
+        <v>45917.200092592589</v>
       </c>
       <c r="D28" s="2">
-        <v>45913.435532407406</v>
+        <v>45918.990624999999</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
@@ -1100,13 +1105,13 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C29" s="2">
-        <v>45917.200092592589</v>
+        <v>45915.231793981482</v>
       </c>
       <c r="D29" s="2">
-        <v>45918.990624999999</v>
+        <v>45917.019432870373</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29">
@@ -1115,16 +1120,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C30" s="2">
-        <v>45915.231793981482</v>
+        <v>45918.238622685189</v>
       </c>
       <c r="D30" s="2">
-        <v>45917.019432870373</v>
+        <v>45920.002534722225</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30">
@@ -1136,17 +1141,17 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C31" s="2">
-        <v>45909.261608796296</v>
-      </c>
-      <c r="D31" s="2">
-        <v>45911.001076388886</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>45918.557500000003</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F31">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -1154,31 +1159,31 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C32" s="2">
-        <v>45913.23265046296</v>
-      </c>
-      <c r="D32" s="2">
-        <v>45914.981087962966</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>45918.603634259256</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F32">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="C33" s="2">
-        <v>45913.76421296296</v>
+        <v>45913.23265046296</v>
       </c>
       <c r="D33" s="2">
-        <v>45915.539942129632</v>
+        <v>45914.981087962966</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33">
@@ -1187,20 +1192,20 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C34" s="2">
-        <v>45909.799317129633</v>
+        <v>45913.76421296296</v>
       </c>
       <c r="D34" s="2">
-        <v>45911.513888888891</v>
+        <v>45915.539942129632</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
@@ -1223,18 +1228,18 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C36" s="2">
-        <v>45917.638888888891</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45918.02584490741</v>
+      </c>
+      <c r="D36" s="2">
+        <v>45919.731539351851</v>
+      </c>
+      <c r="E36" s="2"/>
       <c r="F36">
         <v>41</v>
       </c>
@@ -1244,7 +1249,7 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C37" s="2">
         <v>45911.531018518515</v>
@@ -1259,20 +1264,20 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C38" s="2">
-        <v>45915.111643518518</v>
-      </c>
-      <c r="D38" s="2">
-        <v>45916.694467592592</v>
-      </c>
-      <c r="E38" s="2"/>
+        <v>45918.673472222225</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F38">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -1280,17 +1285,17 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C39" s="2">
-        <v>45914.486261574071</v>
-      </c>
-      <c r="D39" s="2">
-        <v>45916.002962962964</v>
-      </c>
-      <c r="E39" s="2"/>
+        <v>45918.715682870374</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F39">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -1298,17 +1303,17 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C40" s="2">
-        <v>45909.579212962963</v>
+        <v>45915.111643518518</v>
       </c>
       <c r="D40" s="2">
-        <v>45911.07608796296</v>
+        <v>45916.694467592592</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -1316,17 +1321,17 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C41" s="2">
-        <v>45910.534502314818</v>
+        <v>45914.486261574071</v>
       </c>
       <c r="D41" s="2">
-        <v>45912.012048611112</v>
+        <v>45916.002962962964</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
@@ -1334,13 +1339,13 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C42" s="2">
-        <v>45916.051249999997</v>
+        <v>45910.534502314818</v>
       </c>
       <c r="D42" s="2">
-        <v>45917.567256944443</v>
+        <v>45912.012048611112</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42">
@@ -1349,16 +1354,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C43" s="2">
-        <v>45915.061967592592</v>
+        <v>45916.051249999997</v>
       </c>
       <c r="D43" s="2">
-        <v>45916.546516203707</v>
+        <v>45917.567256944443</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43">
@@ -1370,13 +1375,13 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C44" s="2">
-        <v>45915.025833333333</v>
+        <v>45915.061967592592</v>
       </c>
       <c r="D44" s="2">
-        <v>45916.511203703703</v>
+        <v>45916.546516203707</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44">
@@ -1385,70 +1390,70 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C45" s="2">
-        <v>45917.128229166665</v>
+        <v>45915.025833333333</v>
       </c>
       <c r="D45" s="2">
-        <v>45918.609236111108</v>
+        <v>45916.511203703703</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C46" s="2">
-        <v>45913.566805555558</v>
+        <v>45918.539907407408</v>
       </c>
       <c r="D46" s="2">
-        <v>45915.004942129628</v>
+        <v>45920.001921296294</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C47" s="2">
-        <v>45913.717233796298</v>
+        <v>45918.526932870373</v>
       </c>
       <c r="D47" s="2">
-        <v>45915.203182870369</v>
+        <v>45920.000578703701</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C48" s="2">
-        <v>45912.567314814813</v>
+        <v>45913.717233796298</v>
       </c>
       <c r="D48" s="2">
-        <v>45914.04074074074</v>
+        <v>45915.203182870369</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48">
@@ -1457,20 +1462,20 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C49" s="2">
-        <v>45914.050219907411</v>
+        <v>45913.566805555558</v>
       </c>
       <c r="D49" s="2">
-        <v>45915.466817129629</v>
+        <v>45915.004942129628</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -1478,17 +1483,17 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C50" s="2">
-        <v>45915.541979166665</v>
+        <v>45918.54587962963</v>
       </c>
       <c r="D50" s="2">
-        <v>45916.988449074073</v>
+        <v>45920.000509259262</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
@@ -1496,35 +1501,35 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C51" s="2">
-        <v>45916.059074074074</v>
+        <v>45917.128229166665</v>
       </c>
       <c r="D51" s="2">
-        <v>45917.468865740739</v>
+        <v>45918.609236111108</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C52" s="2">
-        <v>45916.623356481483</v>
+        <v>45912.567314814813</v>
       </c>
       <c r="D52" s="2">
-        <v>45918.0237037037</v>
+        <v>45914.04074074074</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
@@ -1532,13 +1537,13 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C53" s="2">
-        <v>45917.589189814818</v>
+        <v>45916.059074074074</v>
       </c>
       <c r="D53" s="2">
-        <v>45919.000393518516</v>
+        <v>45917.468865740739</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53">
@@ -1547,20 +1552,20 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C54" s="2">
-        <v>45912.627604166664</v>
+        <v>45916.623356481483</v>
       </c>
       <c r="D54" s="2">
-        <v>45914.005208333336</v>
+        <v>45918.0237037037</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -1568,17 +1573,17 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C55" s="2">
-        <v>45910.054398148146</v>
+        <v>45917.589189814818</v>
       </c>
       <c r="D55" s="2">
-        <v>45911.384293981479</v>
+        <v>45919.000393518516</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -1586,53 +1591,53 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C56" s="2">
-        <v>45918.02584490741</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45915.541979166665</v>
+      </c>
+      <c r="D56" s="2">
+        <v>45916.988449074073</v>
+      </c>
+      <c r="E56" s="2"/>
       <c r="F56">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C57" s="2">
-        <v>45909.039467592593</v>
+        <v>45914.050219907411</v>
       </c>
       <c r="D57" s="2">
-        <v>45910.373379629629</v>
+        <v>45915.466817129629</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C58" s="2">
-        <v>45910.029456018521</v>
+        <v>45912.627604166664</v>
       </c>
       <c r="D58" s="2">
-        <v>45911.331701388888</v>
+        <v>45914.005208333336</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
@@ -1640,17 +1645,17 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C59" s="2">
-        <v>45915.259062500001</v>
+        <v>45910.054398148146</v>
       </c>
       <c r="D59" s="2">
-        <v>45916.545428240737</v>
+        <v>45911.384293981479</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
@@ -1658,13 +1663,13 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C60" s="2">
-        <v>45917.051562499997</v>
+        <v>45915.259062500001</v>
       </c>
       <c r="D60" s="2">
-        <v>45918.348865740743</v>
+        <v>45916.545428240737</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60">
@@ -1676,15 +1681,15 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C61" s="2">
-        <v>45918.06113425926</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45917.051562499997</v>
+      </c>
+      <c r="D61" s="2">
+        <v>45918.348865740743</v>
+      </c>
+      <c r="E61" s="2"/>
       <c r="F61">
         <v>31</v>
       </c>
@@ -1712,53 +1717,53 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C63" s="2">
-        <v>45910.247546296298</v>
-      </c>
-      <c r="D63" s="2">
-        <v>45911.529826388891</v>
-      </c>
-      <c r="E63" s="2"/>
+        <v>45919.051585648151</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F63">
         <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C64" s="2">
-        <v>45909.260914351849</v>
+        <v>45910.247546296298</v>
       </c>
       <c r="D64" s="2">
-        <v>45910.524594907409</v>
+        <v>45911.529826388891</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C65" s="2">
-        <v>45917.038738425923</v>
+        <v>45918.712372685186</v>
       </c>
       <c r="D65" s="2">
-        <v>45918.261030092595</v>
+        <v>45920.004004629627</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
@@ -1766,17 +1771,17 @@
         <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C66" s="2">
-        <v>45913.050844907404</v>
+        <v>45917.038738425923</v>
       </c>
       <c r="D66" s="2">
-        <v>45914.284895833334</v>
+        <v>45918.261030092595</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
@@ -1784,17 +1789,17 @@
         <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C67" s="2">
-        <v>45910.067824074074</v>
+        <v>45918.264537037037</v>
       </c>
       <c r="D67" s="2">
-        <v>45911.284560185188</v>
+        <v>45919.504305555558</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
@@ -1802,31 +1807,31 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="C68" s="2">
-        <v>45915.250428240739</v>
+        <v>45918.257824074077</v>
       </c>
       <c r="D68" s="2">
-        <v>45916.492291666669</v>
+        <v>45919.535219907404</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C69" s="2">
-        <v>45916.350173611114</v>
+        <v>45913.050844907404</v>
       </c>
       <c r="D69" s="2">
-        <v>45917.544189814813</v>
+        <v>45914.284895833334</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69">
@@ -1835,16 +1840,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C70" s="2">
-        <v>45914.304675925923</v>
+        <v>45915.250428240739</v>
       </c>
       <c r="D70" s="2">
-        <v>45915.505648148152</v>
+        <v>45916.492291666669</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70">
@@ -1853,16 +1858,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C71" s="2">
-        <v>45914.064189814817</v>
+        <v>45910.067824074074</v>
       </c>
       <c r="D71" s="2">
-        <v>45915.274594907409</v>
+        <v>45911.284560185188</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71">
@@ -1871,20 +1876,20 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C72" s="2">
-        <v>45909.373738425929</v>
+        <v>45914.064189814817</v>
       </c>
       <c r="D72" s="2">
-        <v>45910.524085648147</v>
+        <v>45915.274594907409</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
@@ -1892,53 +1897,53 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C73" s="2">
-        <v>45914.060752314814</v>
+        <v>45918.558819444443</v>
       </c>
       <c r="D73" s="2">
-        <v>45915.225474537037</v>
+        <v>45919.759699074071</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B74" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C74" s="2">
-        <v>45914.011388888888</v>
+        <v>45914.304675925923</v>
       </c>
       <c r="D74" s="2">
-        <v>45915.187569444446</v>
+        <v>45915.505648148152</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B75" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C75" s="2">
-        <v>45910.356319444443</v>
+        <v>45916.350173611114</v>
       </c>
       <c r="D75" s="2">
-        <v>45911.500925925924</v>
+        <v>45917.544189814813</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
@@ -1946,13 +1951,13 @@
         <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C76" s="2">
-        <v>45917.046249999999</v>
+        <v>45910.356319444443</v>
       </c>
       <c r="D76" s="2">
-        <v>45918.227696759262</v>
+        <v>45911.500925925924</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76">
@@ -1964,13 +1969,13 @@
         <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C77" s="2">
-        <v>45915.035682870373</v>
+        <v>45917.046249999999</v>
       </c>
       <c r="D77" s="2">
-        <v>45916.204282407409</v>
+        <v>45918.227696759262</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77">
@@ -1979,16 +1984,16 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C78" s="2">
-        <v>45917.862303240741</v>
+        <v>45914.011388888888</v>
       </c>
       <c r="D78" s="2">
-        <v>45919.004907407405</v>
+        <v>45915.187569444446</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78">
@@ -1997,74 +2002,74 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C79" s="2">
-        <v>45913.042430555557</v>
+        <v>45915.035682870373</v>
       </c>
       <c r="D79" s="2">
-        <v>45914.200810185182</v>
+        <v>45916.204282407409</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="C80" s="2">
-        <v>45918.238622685189</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45919.064259259256</v>
+      </c>
+      <c r="D80" s="2">
+        <v>45920.216261574074</v>
+      </c>
+      <c r="E80" s="2"/>
       <c r="F80">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
         <v>44</v>
       </c>
       <c r="C81" s="2">
-        <v>45909.091203703705</v>
+        <v>45917.862303240741</v>
       </c>
       <c r="D81" s="2">
-        <v>45910.220127314817</v>
+        <v>45919.004907407405</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="C82" s="2">
-        <v>45914.151493055557</v>
+        <v>45914.060752314814</v>
       </c>
       <c r="D82" s="2">
-        <v>45915.287997685184</v>
+        <v>45915.225474537037</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
@@ -2072,13 +2077,13 @@
         <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C83" s="2">
-        <v>45915.075706018521</v>
+        <v>45912.041076388887</v>
       </c>
       <c r="D83" s="2">
-        <v>45916.188900462963</v>
+        <v>45913.145925925928</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83">
@@ -2090,13 +2095,13 @@
         <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C84" s="2">
-        <v>45912.041076388887</v>
+        <v>45915.075706018521</v>
       </c>
       <c r="D84" s="2">
-        <v>45913.145925925928</v>
+        <v>45916.188900462963</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84">
@@ -2108,7 +2113,7 @@
         <v>6</v>
       </c>
       <c r="B85" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C85" s="2">
         <v>45913.579629629632</v>
@@ -2126,13 +2131,13 @@
         <v>6</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C86" s="2">
-        <v>45914.045497685183</v>
+        <v>45914.151493055557</v>
       </c>
       <c r="D86" s="2">
-        <v>45915.202696759261</v>
+        <v>45915.287997685184</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86">
@@ -2141,16 +2146,16 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C87" s="2">
-        <v>45911.012094907404</v>
+        <v>45914.045497685183</v>
       </c>
       <c r="D87" s="2">
-        <v>45912.137696759259</v>
+        <v>45915.202696759261</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87">
@@ -2159,106 +2164,106 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C88" s="2">
-        <v>45909.039143518516</v>
+        <v>45911.012094907404</v>
       </c>
       <c r="D88" s="2">
-        <v>45910.102083333331</v>
+        <v>45912.137696759259</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C89" s="2">
-        <v>45918.264537037037</v>
-      </c>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45913.042430555557</v>
+      </c>
+      <c r="D89" s="2">
+        <v>45914.200810185182</v>
+      </c>
+      <c r="E89" s="2"/>
       <c r="F89">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C90" s="2">
-        <v>45918.257824074077</v>
-      </c>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2">
-        <v>45919.361435185187</v>
-      </c>
+        <v>45913.064467592594</v>
+      </c>
+      <c r="D90" s="2">
+        <v>45914.140983796293</v>
+      </c>
+      <c r="E90" s="2"/>
       <c r="F90">
         <v>26</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C91" s="2">
-        <v>45909.514016203706</v>
-      </c>
-      <c r="D91" s="2">
-        <v>45910.611180555556</v>
-      </c>
-      <c r="E91" s="2"/>
+        <v>45919.267326388886</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F91">
         <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C92" s="2">
-        <v>45913.064467592594</v>
+        <v>45911.684641203705</v>
       </c>
       <c r="D92" s="2">
-        <v>45914.140983796293</v>
+        <v>45912.726527777777</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B93" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="C93" s="2">
-        <v>45913.021006944444</v>
+        <v>45919.067708333336</v>
       </c>
       <c r="D93" s="2">
-        <v>45914.078969907408</v>
+        <v>45920.088587962964</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93">
@@ -2270,13 +2275,13 @@
         <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="C94" s="2">
-        <v>45911.994386574072</v>
+        <v>45915.475578703707</v>
       </c>
       <c r="D94" s="2">
-        <v>45913.008622685185</v>
+        <v>45916.538958333331</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94">
@@ -2288,13 +2293,13 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C95" s="2">
-        <v>45918.199444444443</v>
+        <v>45917.244652777779</v>
       </c>
       <c r="D95" s="2">
-        <v>45919.209988425922</v>
+        <v>45918.285451388889</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95">
@@ -2306,13 +2311,13 @@
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C96" s="2">
-        <v>45911.684641203705</v>
+        <v>45911.994386574072</v>
       </c>
       <c r="D96" s="2">
-        <v>45912.726527777777</v>
+        <v>45913.008622685185</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96">
@@ -2324,13 +2329,13 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C97" s="2">
-        <v>45917.244652777779</v>
+        <v>45918.199444444443</v>
       </c>
       <c r="D97" s="2">
-        <v>45918.285451388889</v>
+        <v>45919.209988425922</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97">
@@ -2342,13 +2347,13 @@
         <v>6</v>
       </c>
       <c r="B98" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C98" s="2">
-        <v>45915.055277777778</v>
+        <v>45912.043020833335</v>
       </c>
       <c r="D98" s="2">
-        <v>45916.095949074072</v>
+        <v>45913.113923611112</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98">
@@ -2360,15 +2365,15 @@
         <v>6</v>
       </c>
       <c r="B99" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C99" s="2">
-        <v>45912.043020833335</v>
-      </c>
-      <c r="D99" s="2">
-        <v>45913.113923611112</v>
-      </c>
-      <c r="E99" s="2"/>
+        <v>45919.2965625</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2">
+        <v>45920.341481481482</v>
+      </c>
       <c r="F99">
         <v>25</v>
       </c>
@@ -2378,13 +2383,13 @@
         <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="C100" s="2">
-        <v>45915.475578703707</v>
+        <v>45915.055277777778</v>
       </c>
       <c r="D100" s="2">
-        <v>45916.538958333331</v>
+        <v>45916.095949074072</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100">
@@ -2411,16 +2416,16 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C102" s="2">
-        <v>45909.239444444444</v>
+        <v>45914.036979166667</v>
       </c>
       <c r="D102" s="2">
-        <v>45910.265706018516</v>
+        <v>45915.079004629632</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102">
@@ -2429,16 +2434,16 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C103" s="2">
-        <v>45911.244166666664</v>
+        <v>45919.036516203705</v>
       </c>
       <c r="D103" s="2">
-        <v>45912.265601851854</v>
+        <v>45920.041701388887</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103">
@@ -2447,16 +2452,16 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="C104" s="2">
-        <v>45911.504976851851</v>
+        <v>45910.196134259262</v>
       </c>
       <c r="D104" s="2">
-        <v>45912.543333333335</v>
+        <v>45911.248784722222</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104">
@@ -2465,16 +2470,16 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C105" s="2">
-        <v>45915.525405092594</v>
+        <v>45913.021006944444</v>
       </c>
       <c r="D105" s="2">
-        <v>45916.54210648148</v>
+        <v>45914.078969907408</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105">
@@ -2483,16 +2488,16 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B106" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C106" s="2">
-        <v>45910.196134259262</v>
+        <v>45911.244166666664</v>
       </c>
       <c r="D106" s="2">
-        <v>45911.248784722222</v>
+        <v>45912.265601851854</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106">
@@ -2501,16 +2506,16 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B107" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C107" s="2">
-        <v>45914.036979166667</v>
+        <v>45911.504976851851</v>
       </c>
       <c r="D107" s="2">
-        <v>45915.079004629632</v>
+        <v>45912.543333333335</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107">
@@ -2519,34 +2524,34 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B108" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C108" s="2">
-        <v>45915.55263888889</v>
+        <v>45915.525405092594</v>
       </c>
       <c r="D108" s="2">
-        <v>45916.542962962965</v>
+        <v>45916.54210648148</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C109" s="2">
-        <v>45917.562847222223</v>
+        <v>45917.243622685186</v>
       </c>
       <c r="D109" s="2">
-        <v>45918.543981481482</v>
+        <v>45918.209560185183</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109">
@@ -2555,16 +2560,16 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C110" s="2">
-        <v>45914.043333333335</v>
+        <v>45913.701620370368</v>
       </c>
       <c r="D110" s="2">
-        <v>45915.064780092594</v>
+        <v>45914.694907407407</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110">
@@ -2573,16 +2578,16 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C111" s="2">
-        <v>45914.019074074073</v>
+        <v>45915.220127314817</v>
       </c>
       <c r="D111" s="2">
-        <v>45915.000347222223</v>
+        <v>45916.216979166667</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111">
@@ -2591,16 +2596,16 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B112" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C112" s="2">
-        <v>45915.540833333333</v>
+        <v>45917.543113425927</v>
       </c>
       <c r="D112" s="2">
-        <v>45916.513043981482</v>
+        <v>45918.545127314814</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112">
@@ -2609,16 +2614,16 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B113" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C113" s="2">
-        <v>45909.532372685186</v>
+        <v>45910.041087962964</v>
       </c>
       <c r="D113" s="2">
-        <v>45910.502280092594</v>
+        <v>45911.026550925926</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113">
@@ -2627,16 +2632,16 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C114" s="2">
-        <v>45910.510555555556</v>
+        <v>45919.033101851855</v>
       </c>
       <c r="D114" s="2">
-        <v>45911.524016203701</v>
+        <v>45920.037638888891</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114">
@@ -2648,13 +2653,13 @@
         <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C115" s="2">
-        <v>45915.220127314817</v>
+        <v>45915.020277777781</v>
       </c>
       <c r="D115" s="2">
-        <v>45916.216979166667</v>
+        <v>45916.002210648148</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115">
@@ -2666,13 +2671,13 @@
         <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C116" s="2">
-        <v>45915.020277777781</v>
+        <v>45913.029675925929</v>
       </c>
       <c r="D116" s="2">
-        <v>45916.002210648148</v>
+        <v>45914.000960648147</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116">
@@ -2684,13 +2689,13 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C117" s="2">
-        <v>45917.243622685186</v>
+        <v>45919.028819444444</v>
       </c>
       <c r="D117" s="2">
-        <v>45918.209560185183</v>
+        <v>45920.000590277778</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117">
@@ -2702,13 +2707,13 @@
         <v>6</v>
       </c>
       <c r="B118" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C118" s="2">
-        <v>45909.531261574077</v>
+        <v>45913.030231481483</v>
       </c>
       <c r="D118" s="2">
-        <v>45910.523888888885</v>
+        <v>45914.003888888888</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118">
@@ -2720,13 +2725,13 @@
         <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C119" s="2">
-        <v>45913.701620370368</v>
+        <v>45918.378263888888</v>
       </c>
       <c r="D119" s="2">
-        <v>45914.694907407407</v>
+        <v>45919.401689814818</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119">
@@ -2756,13 +2761,13 @@
         <v>6</v>
       </c>
       <c r="B121" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C121" s="2">
-        <v>45913.030231481483</v>
+        <v>45915.572175925925</v>
       </c>
       <c r="D121" s="2">
-        <v>45914.003888888888</v>
+        <v>45916.543171296296</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121">
@@ -2774,13 +2779,13 @@
         <v>6</v>
       </c>
       <c r="B122" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C122" s="2">
-        <v>45913.029675925929</v>
+        <v>45910.584328703706</v>
       </c>
       <c r="D122" s="2">
-        <v>45914.000960648147</v>
+        <v>45911.616053240738</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122">
@@ -2789,16 +2794,16 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B123" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C123" s="2">
-        <v>45910.041087962964</v>
+        <v>45919.277962962966</v>
       </c>
       <c r="D123" s="2">
-        <v>45911.026550925926</v>
+        <v>45920.264999999999</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123">
@@ -2807,16 +2812,16 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B124" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C124" s="2">
-        <v>45915.572175925925</v>
+        <v>45916.019108796296</v>
       </c>
       <c r="D124" s="2">
-        <v>45916.543171296296</v>
+        <v>45917.00277777778</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124">
@@ -2825,16 +2830,16 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B125" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="C125" s="2">
-        <v>45917.543113425927</v>
+        <v>45916.579988425925</v>
       </c>
       <c r="D125" s="2">
-        <v>45918.545127314814</v>
+        <v>45917.561284722222</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125">
@@ -2843,16 +2848,16 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B126" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="C126" s="2">
-        <v>45910.584328703706</v>
+        <v>45911.556932870371</v>
       </c>
       <c r="D126" s="2">
-        <v>45911.616053240738</v>
+        <v>45912.543055555558</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126">
@@ -2861,16 +2866,16 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B127" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C127" s="2">
-        <v>45912.242094907408</v>
+        <v>45912.03328703704</v>
       </c>
       <c r="D127" s="2">
-        <v>45913.231030092589</v>
+        <v>45913.003379629627</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127">
@@ -2879,16 +2884,16 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B128" t="s">
         <v>45</v>
       </c>
       <c r="C128" s="2">
-        <v>45913.530856481484</v>
+        <v>45913.032546296294</v>
       </c>
       <c r="D128" s="2">
-        <v>45914.507928240739</v>
+        <v>45914.002326388887</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128">
@@ -2900,13 +2905,13 @@
         <v>8</v>
       </c>
       <c r="B129" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C129" s="2">
-        <v>45916.019108796296</v>
+        <v>45910.02920138889</v>
       </c>
       <c r="D129" s="2">
-        <v>45917.00277777778</v>
+        <v>45911.005185185182</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129">
@@ -2918,13 +2923,13 @@
         <v>8</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C130" s="2">
-        <v>45916.579988425925</v>
+        <v>45911.034571759257</v>
       </c>
       <c r="D130" s="2">
-        <v>45917.561284722222</v>
+        <v>45912.001400462963</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130">
@@ -2936,13 +2941,13 @@
         <v>8</v>
       </c>
       <c r="B131" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C131" s="2">
-        <v>45913.032546296294</v>
+        <v>45914.0625</v>
       </c>
       <c r="D131" s="2">
-        <v>45914.002326388887</v>
+        <v>45915.059525462966</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131">
@@ -2954,13 +2959,13 @@
         <v>8</v>
       </c>
       <c r="B132" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C132" s="2">
-        <v>45910.02920138889</v>
+        <v>45919.031469907408</v>
       </c>
       <c r="D132" s="2">
-        <v>45911.005185185182</v>
+        <v>45920.003437500003</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132">
@@ -2969,16 +2974,16 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B133" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C133" s="2">
-        <v>45911.034571759257</v>
+        <v>45915.55263888889</v>
       </c>
       <c r="D133" s="2">
-        <v>45912.001400462963</v>
+        <v>45916.542962962965</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133">
@@ -2987,16 +2992,16 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B134" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C134" s="2">
-        <v>45914.0625</v>
+        <v>45914.043333333335</v>
       </c>
       <c r="D134" s="2">
-        <v>45915.059525462966</v>
+        <v>45915.064780092594</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134">
@@ -3005,16 +3010,16 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B135" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C135" s="2">
-        <v>45909.029490740744</v>
+        <v>45915.540833333333</v>
       </c>
       <c r="D135" s="2">
-        <v>45910.00445601852</v>
+        <v>45916.513043981482</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135">
@@ -3023,16 +3028,16 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B136" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C136" s="2">
-        <v>45911.556932870371</v>
+        <v>45914.019074074073</v>
       </c>
       <c r="D136" s="2">
-        <v>45912.543055555558</v>
+        <v>45915.000347222223</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136">
@@ -3041,19 +3046,109 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B137" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C137" s="2">
-        <v>45912.03328703704</v>
+        <v>45917.562847222223</v>
       </c>
       <c r="D137" s="2">
-        <v>45913.003379629627</v>
+        <v>45918.543981481482</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A138" t="s">
+        <v>11</v>
+      </c>
+      <c r="B138" t="s">
+        <v>32</v>
+      </c>
+      <c r="C138" s="2">
+        <v>45910.510555555556</v>
+      </c>
+      <c r="D138" s="2">
+        <v>45911.524016203701</v>
+      </c>
+      <c r="E138" s="2"/>
+      <c r="F138">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A139" t="s">
+        <v>51</v>
+      </c>
+      <c r="B139" t="s">
+        <v>55</v>
+      </c>
+      <c r="C139" s="2">
+        <v>45912.242094907408</v>
+      </c>
+      <c r="D139" s="2">
+        <v>45913.231030092589</v>
+      </c>
+      <c r="E139" s="2"/>
+      <c r="F139">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A140" t="s">
+        <v>51</v>
+      </c>
+      <c r="B140" t="s">
+        <v>43</v>
+      </c>
+      <c r="C140" s="2">
+        <v>45913.530856481484</v>
+      </c>
+      <c r="D140" s="2">
+        <v>45914.507928240739</v>
+      </c>
+      <c r="E140" s="2"/>
+      <c r="F140">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A141" t="s">
+        <v>51</v>
+      </c>
+      <c r="B141" t="s">
+        <v>31</v>
+      </c>
+      <c r="C141" s="2">
+        <v>45919.362210648149</v>
+      </c>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2">
+        <v>45920.341481481482</v>
+      </c>
+      <c r="F141">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A142" t="s">
+        <v>51</v>
+      </c>
+      <c r="B142" t="s">
+        <v>56</v>
+      </c>
+      <c r="C142" s="2">
+        <v>45919.351388888892</v>
+      </c>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2">
+        <v>45920.341481481482</v>
+      </c>
+      <c r="F142">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-20 15:42:57.96
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="71">
   <si>
     <t>电站名称</t>
   </si>
@@ -218,6 +218,18 @@
   </si>
   <si>
     <t>011A号直流</t>
+  </si>
+  <si>
+    <t>307号直流</t>
+  </si>
+  <si>
+    <t>207号直流</t>
+  </si>
+  <si>
+    <t>208号直流</t>
+  </si>
+  <si>
+    <t>308号直流</t>
   </si>
 </sst>
 </file>
@@ -578,19 +590,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="42.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="23.25" customWidth="1"/>
-    <col min="5" max="5" width="22.25" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
+    <col min="4" max="4" width="25.25" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -626,10 +638,10 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>45920.341481481482</v>
+        <v>45920.649699074071</v>
       </c>
       <c r="F2">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -644,46 +656,46 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
-        <v>45920.341481481482</v>
+        <v>45920.649699074071</v>
       </c>
       <c r="F3">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
-        <v>45911.52857638889</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45915.503275462965</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>45916.534282407411</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F4">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2">
-        <v>45916.534282407411</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45911.52857638889</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45915.503275462965</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -706,20 +718,20 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2">
-        <v>45913.052685185183</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45916.265127314815</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>45917.258240740739</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F7">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -732,30 +744,30 @@
       <c r="C8" s="2">
         <v>45917.260844907411</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>45920.341481481482</v>
-      </c>
+      <c r="D8" s="2">
+        <v>45920.502418981479</v>
+      </c>
+      <c r="E8" s="2"/>
       <c r="F8">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2">
-        <v>45917.258240740739</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45913.052685185183</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45916.265127314815</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -835,17 +847,17 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2">
-        <v>45913.006967592592</v>
+        <v>45918.06113425926</v>
       </c>
       <c r="D14" s="2">
-        <v>45915.473703703705</v>
+        <v>45920.554386574076</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -853,17 +865,17 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
-        <v>45918.06113425926</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45913.006967592592</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45915.473703703705</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -886,38 +898,38 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2">
-        <v>45910.355798611112</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45912.393368055556</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>45918.557500000003</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F17">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2">
-        <v>45911.040381944447</v>
+        <v>45910.355798611112</v>
       </c>
       <c r="D18" s="2">
-        <v>45913.023263888892</v>
+        <v>45912.393368055556</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -925,17 +937,17 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2">
-        <v>45912.060983796298</v>
+        <v>45918.603634259256</v>
       </c>
       <c r="D19" s="2">
-        <v>45914.012141203704</v>
+        <v>45920.611122685186</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -943,31 +955,31 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2">
-        <v>45915.583414351851</v>
+        <v>45911.040381944447</v>
       </c>
       <c r="D20" s="2">
-        <v>45917.582627314812</v>
+        <v>45913.023263888892</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2">
-        <v>45910.5781712963</v>
+        <v>45910.561724537038</v>
       </c>
       <c r="D21" s="2">
-        <v>45912.528969907406</v>
+        <v>45912.509375000001</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21">
@@ -976,16 +988,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2">
-        <v>45910.561724537038</v>
+        <v>45912.060983796298</v>
       </c>
       <c r="D22" s="2">
-        <v>45912.509375000001</v>
+        <v>45914.012141203704</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22">
@@ -994,70 +1006,70 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C23" s="2">
-        <v>45914.560046296298</v>
+        <v>45915.583414351851</v>
       </c>
       <c r="D23" s="2">
-        <v>45916.478472222225</v>
+        <v>45917.582627314812</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C24" s="2">
-        <v>45911.646747685183</v>
+        <v>45910.5781712963</v>
       </c>
       <c r="D24" s="2">
-        <v>45913.523923611108</v>
+        <v>45912.528969907406</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2">
-        <v>45911.562384259261</v>
+        <v>45914.560046296298</v>
       </c>
       <c r="D25" s="2">
-        <v>45913.435532407406</v>
+        <v>45916.478472222225</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C26" s="2">
-        <v>45917.638888888891</v>
+        <v>45917.219965277778</v>
       </c>
       <c r="D26" s="2">
-        <v>45919.518240740741</v>
+        <v>45919.087418981479</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26">
@@ -1066,16 +1078,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C27" s="2">
-        <v>45917.219965277778</v>
+        <v>45911.646747685183</v>
       </c>
       <c r="D27" s="2">
-        <v>45919.087418981479</v>
+        <v>45913.523923611108</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27">
@@ -1087,35 +1099,35 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C28" s="2">
-        <v>45917.200092592589</v>
+        <v>45911.562384259261</v>
       </c>
       <c r="D28" s="2">
-        <v>45918.990624999999</v>
+        <v>45913.435532407406</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2">
-        <v>45915.231793981482</v>
+        <v>45917.638888888891</v>
       </c>
       <c r="D29" s="2">
-        <v>45917.019432870373</v>
+        <v>45919.518240740741</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -1138,18 +1150,18 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C31" s="2">
-        <v>45918.557500000003</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45915.231793981482</v>
+      </c>
+      <c r="D31" s="2">
+        <v>45917.019432870373</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="F31">
         <v>43</v>
       </c>
@@ -1159,31 +1171,31 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C32" s="2">
-        <v>45918.603634259256</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45917.200092592589</v>
+      </c>
+      <c r="D32" s="2">
+        <v>45918.990624999999</v>
+      </c>
+      <c r="E32" s="2"/>
       <c r="F32">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2">
-        <v>45913.23265046296</v>
+        <v>45913.76421296296</v>
       </c>
       <c r="D33" s="2">
-        <v>45914.981087962966</v>
+        <v>45915.539942129632</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33">
@@ -1192,16 +1204,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2">
-        <v>45913.76421296296</v>
+        <v>45913.23265046296</v>
       </c>
       <c r="D34" s="2">
-        <v>45915.539942129632</v>
+        <v>45914.981087962966</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34">
@@ -1246,36 +1258,36 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C37" s="2">
-        <v>45911.531018518515</v>
+        <v>45918.673472222225</v>
       </c>
       <c r="D37" s="2">
-        <v>45913.206875000003</v>
+        <v>45920.394062500003</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C38" s="2">
-        <v>45918.673472222225</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45911.531018518515</v>
+      </c>
+      <c r="D38" s="2">
+        <v>45913.206875000003</v>
+      </c>
+      <c r="E38" s="2"/>
       <c r="F38">
         <v>40</v>
       </c>
@@ -1285,17 +1297,17 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45915.111643518518</v>
+      </c>
+      <c r="D39" s="2">
+        <v>45916.694467592592</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39">
         <v>38</v>
-      </c>
-      <c r="C39" s="2">
-        <v>45918.715682870374</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2">
-        <v>45920.341481481482</v>
-      </c>
-      <c r="F39">
-        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -1303,13 +1315,13 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C40" s="2">
-        <v>45915.111643518518</v>
+        <v>45918.715682870374</v>
       </c>
       <c r="D40" s="2">
-        <v>45916.694467592592</v>
+        <v>45920.332812499997</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40">
@@ -1321,17 +1333,17 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C41" s="2">
-        <v>45914.486261574071</v>
-      </c>
-      <c r="D41" s="2">
-        <v>45916.002962962964</v>
-      </c>
-      <c r="E41" s="2"/>
+        <v>45919.051585648151</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F41">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
@@ -1339,31 +1351,31 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C42" s="2">
-        <v>45910.534502314818</v>
+        <v>45914.486261574071</v>
       </c>
       <c r="D42" s="2">
-        <v>45912.012048611112</v>
+        <v>45916.002962962964</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C43" s="2">
-        <v>45916.051249999997</v>
+        <v>45918.526932870373</v>
       </c>
       <c r="D43" s="2">
-        <v>45917.567256944443</v>
+        <v>45920.000578703701</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43">
@@ -1372,16 +1384,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C44" s="2">
-        <v>45915.061967592592</v>
+        <v>45918.539907407408</v>
       </c>
       <c r="D44" s="2">
-        <v>45916.546516203707</v>
+        <v>45920.001921296294</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44">
@@ -1390,16 +1402,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C45" s="2">
-        <v>45915.025833333333</v>
+        <v>45910.534502314818</v>
       </c>
       <c r="D45" s="2">
-        <v>45916.511203703703</v>
+        <v>45912.012048611112</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45">
@@ -1408,16 +1420,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C46" s="2">
-        <v>45918.539907407408</v>
+        <v>45916.051249999997</v>
       </c>
       <c r="D46" s="2">
-        <v>45920.001921296294</v>
+        <v>45917.567256944443</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46">
@@ -1426,16 +1438,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C47" s="2">
-        <v>45918.526932870373</v>
+        <v>45915.061967592592</v>
       </c>
       <c r="D47" s="2">
-        <v>45920.000578703701</v>
+        <v>45916.546516203707</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47">
@@ -1444,20 +1456,20 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C48" s="2">
-        <v>45913.717233796298</v>
+        <v>45915.025833333333</v>
       </c>
       <c r="D48" s="2">
-        <v>45915.203182870369</v>
+        <v>45916.511203703703</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
@@ -1465,13 +1477,13 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C49" s="2">
-        <v>45913.566805555558</v>
+        <v>45918.54587962963</v>
       </c>
       <c r="D49" s="2">
-        <v>45915.004942129628</v>
+        <v>45920.000509259262</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49">
@@ -1483,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C50" s="2">
-        <v>45918.54587962963</v>
+        <v>45913.717233796298</v>
       </c>
       <c r="D50" s="2">
-        <v>45920.000509259262</v>
+        <v>45915.203182870369</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50">
@@ -1501,13 +1513,13 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C51" s="2">
-        <v>45917.128229166665</v>
+        <v>45913.566805555558</v>
       </c>
       <c r="D51" s="2">
-        <v>45918.609236111108</v>
+        <v>45915.004942129628</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51">
@@ -1516,16 +1528,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C52" s="2">
-        <v>45912.567314814813</v>
+        <v>45917.128229166665</v>
       </c>
       <c r="D52" s="2">
-        <v>45914.04074074074</v>
+        <v>45918.609236111108</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52">
@@ -1534,34 +1546,34 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C53" s="2">
-        <v>45916.059074074074</v>
+        <v>45912.567314814813</v>
       </c>
       <c r="D53" s="2">
-        <v>45917.468865740739</v>
+        <v>45914.04074074074</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C54" s="2">
-        <v>45916.623356481483</v>
+        <v>45914.050219907411</v>
       </c>
       <c r="D54" s="2">
-        <v>45918.0237037037</v>
+        <v>45915.466817129629</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54">
@@ -1573,13 +1585,13 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C55" s="2">
-        <v>45917.589189814818</v>
+        <v>45915.541979166665</v>
       </c>
       <c r="D55" s="2">
-        <v>45919.000393518516</v>
+        <v>45916.988449074073</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55">
@@ -1591,13 +1603,13 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C56" s="2">
-        <v>45915.541979166665</v>
+        <v>45916.059074074074</v>
       </c>
       <c r="D56" s="2">
-        <v>45916.988449074073</v>
+        <v>45917.468865740739</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56">
@@ -1606,16 +1618,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C57" s="2">
-        <v>45914.050219907411</v>
+        <v>45916.623356481483</v>
       </c>
       <c r="D57" s="2">
-        <v>45915.466817129629</v>
+        <v>45918.0237037037</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57">
@@ -1624,38 +1636,38 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C58" s="2">
-        <v>45912.627604166664</v>
+        <v>45917.589189814818</v>
       </c>
       <c r="D58" s="2">
-        <v>45914.005208333336</v>
+        <v>45919.000393518516</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C59" s="2">
-        <v>45910.054398148146</v>
+        <v>45912.627604166664</v>
       </c>
       <c r="D59" s="2">
-        <v>45911.384293981479</v>
+        <v>45914.005208333336</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
@@ -1663,17 +1675,17 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C60" s="2">
-        <v>45915.259062500001</v>
+        <v>45910.054398148146</v>
       </c>
       <c r="D60" s="2">
-        <v>45916.545428240737</v>
+        <v>45911.384293981479</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
@@ -1681,17 +1693,17 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C61" s="2">
-        <v>45917.051562499997</v>
-      </c>
-      <c r="D61" s="2">
-        <v>45918.348865740743</v>
-      </c>
-      <c r="E61" s="2"/>
+        <v>45919.2965625</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F61">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
@@ -1699,13 +1711,13 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C62" s="2">
-        <v>45916.531759259262</v>
+        <v>45910.247546296298</v>
       </c>
       <c r="D62" s="2">
-        <v>45917.797986111109</v>
+        <v>45911.529826388891</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62">
@@ -1717,15 +1729,15 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C63" s="2">
-        <v>45919.051585648151</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45915.259062500001</v>
+      </c>
+      <c r="D63" s="2">
+        <v>45916.545428240737</v>
+      </c>
+      <c r="E63" s="2"/>
       <c r="F63">
         <v>31</v>
       </c>
@@ -1735,13 +1747,13 @@
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C64" s="2">
-        <v>45910.247546296298</v>
+        <v>45917.051562499997</v>
       </c>
       <c r="D64" s="2">
-        <v>45911.529826388891</v>
+        <v>45918.348865740743</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64">
@@ -1750,16 +1762,16 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C65" s="2">
-        <v>45918.712372685186</v>
+        <v>45916.531759259262</v>
       </c>
       <c r="D65" s="2">
-        <v>45920.004004629627</v>
+        <v>45917.797986111109</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65">
@@ -1768,34 +1780,34 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C66" s="2">
-        <v>45917.038738425923</v>
+        <v>45918.712372685186</v>
       </c>
       <c r="D66" s="2">
-        <v>45918.261030092595</v>
+        <v>45920.004004629627</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C67" s="2">
-        <v>45918.264537037037</v>
+        <v>45919.267326388886</v>
       </c>
       <c r="D67" s="2">
-        <v>45919.504305555558</v>
+        <v>45920.507592592592</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67">
@@ -1807,13 +1819,13 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C68" s="2">
-        <v>45918.257824074077</v>
+        <v>45918.264537037037</v>
       </c>
       <c r="D68" s="2">
-        <v>45919.535219907404</v>
+        <v>45919.504305555558</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68">
@@ -1825,17 +1837,17 @@
         <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C69" s="2">
-        <v>45913.050844907404</v>
+        <v>45917.038738425923</v>
       </c>
       <c r="D69" s="2">
-        <v>45914.284895833334</v>
+        <v>45918.261030092595</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
@@ -1843,31 +1855,31 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="C70" s="2">
-        <v>45915.250428240739</v>
+        <v>45918.257824074077</v>
       </c>
       <c r="D70" s="2">
-        <v>45916.492291666669</v>
+        <v>45919.535219907404</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C71" s="2">
-        <v>45910.067824074074</v>
+        <v>45914.304675925923</v>
       </c>
       <c r="D71" s="2">
-        <v>45911.284560185188</v>
+        <v>45915.505648148152</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71">
@@ -1876,16 +1888,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C72" s="2">
-        <v>45914.064189814817</v>
+        <v>45916.350173611114</v>
       </c>
       <c r="D72" s="2">
-        <v>45915.274594907409</v>
+        <v>45917.544189814813</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72">
@@ -1912,16 +1924,16 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C74" s="2">
-        <v>45914.304675925923</v>
+        <v>45915.250428240739</v>
       </c>
       <c r="D74" s="2">
-        <v>45915.505648148152</v>
+        <v>45916.492291666669</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74">
@@ -1930,16 +1942,16 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C75" s="2">
-        <v>45916.350173611114</v>
+        <v>45913.050844907404</v>
       </c>
       <c r="D75" s="2">
-        <v>45917.544189814813</v>
+        <v>45914.284895833334</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75">
@@ -1951,49 +1963,49 @@
         <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C76" s="2">
-        <v>45910.356319444443</v>
+        <v>45910.067824074074</v>
       </c>
       <c r="D76" s="2">
-        <v>45911.500925925924</v>
+        <v>45911.284560185188</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C77" s="2">
-        <v>45917.046249999999</v>
+        <v>45914.064189814817</v>
       </c>
       <c r="D77" s="2">
-        <v>45918.227696759262</v>
+        <v>45915.274594907409</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C78" s="2">
-        <v>45914.011388888888</v>
+        <v>45914.060752314814</v>
       </c>
       <c r="D78" s="2">
-        <v>45915.187569444446</v>
+        <v>45915.225474537037</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78">
@@ -2005,13 +2017,13 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C79" s="2">
-        <v>45915.035682870373</v>
+        <v>45910.356319444443</v>
       </c>
       <c r="D79" s="2">
-        <v>45916.204282407409</v>
+        <v>45911.500925925924</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79">
@@ -2020,16 +2032,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="C80" s="2">
-        <v>45919.064259259256</v>
+        <v>45917.046249999999</v>
       </c>
       <c r="D80" s="2">
-        <v>45920.216261574074</v>
+        <v>45918.227696759262</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80">
@@ -2038,16 +2050,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C81" s="2">
-        <v>45917.862303240741</v>
+        <v>45914.011388888888</v>
       </c>
       <c r="D81" s="2">
-        <v>45919.004907407405</v>
+        <v>45915.187569444446</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81">
@@ -2056,16 +2068,16 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C82" s="2">
-        <v>45914.060752314814</v>
+        <v>45915.035682870373</v>
       </c>
       <c r="D82" s="2">
-        <v>45915.225474537037</v>
+        <v>45916.204282407409</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82">
@@ -2074,52 +2086,52 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C83" s="2">
-        <v>45912.041076388887</v>
+        <v>45919.064259259256</v>
       </c>
       <c r="D83" s="2">
-        <v>45913.145925925928</v>
+        <v>45920.216261574074</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B84" t="s">
         <v>44</v>
       </c>
       <c r="C84" s="2">
-        <v>45915.075706018521</v>
+        <v>45917.862303240741</v>
       </c>
       <c r="D84" s="2">
-        <v>45916.188900462963</v>
+        <v>45919.004907407405</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B85" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C85" s="2">
-        <v>45913.579629629632</v>
+        <v>45919.362210648149</v>
       </c>
       <c r="D85" s="2">
-        <v>45914.686932870369</v>
+        <v>45920.481516203705</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85">
@@ -2128,16 +2140,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C86" s="2">
-        <v>45914.151493055557</v>
+        <v>45913.042430555557</v>
       </c>
       <c r="D86" s="2">
-        <v>45915.287997685184</v>
+        <v>45914.200810185182</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86">
@@ -2164,16 +2176,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C88" s="2">
-        <v>45911.012094907404</v>
+        <v>45915.075706018521</v>
       </c>
       <c r="D88" s="2">
-        <v>45912.137696759259</v>
+        <v>45916.188900462963</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88">
@@ -2182,16 +2194,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C89" s="2">
-        <v>45913.042430555557</v>
+        <v>45912.041076388887</v>
       </c>
       <c r="D89" s="2">
-        <v>45914.200810185182</v>
+        <v>45913.145925925928</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89">
@@ -2200,124 +2212,124 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C90" s="2">
-        <v>45913.064467592594</v>
+        <v>45913.579629629632</v>
       </c>
       <c r="D90" s="2">
-        <v>45914.140983796293</v>
+        <v>45914.686932870369</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C91" s="2">
-        <v>45919.267326388886</v>
-      </c>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45914.151493055557</v>
+      </c>
+      <c r="D91" s="2">
+        <v>45915.287997685184</v>
+      </c>
+      <c r="E91" s="2"/>
       <c r="F91">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C92" s="2">
-        <v>45911.684641203705</v>
+        <v>45911.012094907404</v>
       </c>
       <c r="D92" s="2">
-        <v>45912.726527777777</v>
+        <v>45912.137696759259</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="C93" s="2">
-        <v>45919.067708333336</v>
-      </c>
-      <c r="D93" s="2">
-        <v>45920.088587962964</v>
-      </c>
-      <c r="E93" s="2"/>
+        <v>45919.528935185182</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F93">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B94" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C94" s="2">
-        <v>45915.475578703707</v>
+        <v>45919.351388888892</v>
       </c>
       <c r="D94" s="2">
-        <v>45916.538958333331</v>
+        <v>45920.447187500002</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C95" s="2">
-        <v>45917.244652777779</v>
+        <v>45913.064467592594</v>
       </c>
       <c r="D95" s="2">
-        <v>45918.285451388889</v>
+        <v>45914.140983796293</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B96" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C96" s="2">
-        <v>45911.994386574072</v>
+        <v>45911.244166666664</v>
       </c>
       <c r="D96" s="2">
-        <v>45913.008622685185</v>
+        <v>45912.265601851854</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96">
@@ -2326,16 +2338,16 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B97" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C97" s="2">
-        <v>45918.199444444443</v>
+        <v>45911.504976851851</v>
       </c>
       <c r="D97" s="2">
-        <v>45919.209988425922</v>
+        <v>45912.543333333335</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97">
@@ -2344,16 +2356,16 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B98" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C98" s="2">
-        <v>45912.043020833335</v>
+        <v>45915.525405092594</v>
       </c>
       <c r="D98" s="2">
-        <v>45913.113923611112</v>
+        <v>45916.54210648148</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98">
@@ -2362,70 +2374,70 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B99" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C99" s="2">
-        <v>45919.2965625</v>
-      </c>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45919.499756944446</v>
+      </c>
+      <c r="D99" s="2">
+        <v>45920.505324074074</v>
+      </c>
+      <c r="E99" s="2"/>
       <c r="F99">
         <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B100" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C100" s="2">
-        <v>45915.055277777778</v>
-      </c>
-      <c r="D100" s="2">
-        <v>45916.095949074072</v>
-      </c>
-      <c r="E100" s="2"/>
+        <v>45919.605023148149</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F100">
         <v>25</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="C101" s="2">
-        <v>45915.483831018515</v>
-      </c>
-      <c r="D101" s="2">
-        <v>45916.511701388888</v>
-      </c>
-      <c r="E101" s="2"/>
+        <v>45919.589224537034</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F101">
         <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C102" s="2">
-        <v>45914.036979166667</v>
+        <v>45919.472337962965</v>
       </c>
       <c r="D102" s="2">
-        <v>45915.079004629632</v>
+        <v>45920.537222222221</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102">
@@ -2434,16 +2446,16 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C103" s="2">
-        <v>45919.036516203705</v>
+        <v>45913.021006944444</v>
       </c>
       <c r="D103" s="2">
-        <v>45920.041701388887</v>
+        <v>45914.078969907408</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103">
@@ -2452,16 +2464,16 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B104" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C104" s="2">
-        <v>45910.196134259262</v>
+        <v>45915.475578703707</v>
       </c>
       <c r="D104" s="2">
-        <v>45911.248784722222</v>
+        <v>45916.538958333331</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104">
@@ -2470,16 +2482,16 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C105" s="2">
-        <v>45913.021006944444</v>
+        <v>45911.994386574072</v>
       </c>
       <c r="D105" s="2">
-        <v>45914.078969907408</v>
+        <v>45913.008622685185</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105">
@@ -2488,16 +2500,16 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C106" s="2">
-        <v>45911.244166666664</v>
+        <v>45918.199444444443</v>
       </c>
       <c r="D106" s="2">
-        <v>45912.265601851854</v>
+        <v>45919.209988425922</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106">
@@ -2506,16 +2518,16 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C107" s="2">
-        <v>45911.504976851851</v>
+        <v>45912.043020833335</v>
       </c>
       <c r="D107" s="2">
-        <v>45912.543333333335</v>
+        <v>45913.113923611112</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107">
@@ -2524,16 +2536,16 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C108" s="2">
-        <v>45915.525405092594</v>
+        <v>45911.684641203705</v>
       </c>
       <c r="D108" s="2">
-        <v>45916.54210648148</v>
+        <v>45912.726527777777</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108">
@@ -2545,17 +2557,17 @@
         <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C109" s="2">
-        <v>45917.243622685186</v>
+        <v>45919.067708333336</v>
       </c>
       <c r="D109" s="2">
-        <v>45918.209560185183</v>
+        <v>45920.088587962964</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
@@ -2563,17 +2575,17 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C110" s="2">
-        <v>45913.701620370368</v>
+        <v>45917.244652777779</v>
       </c>
       <c r="D110" s="2">
-        <v>45914.694907407407</v>
+        <v>45918.285451388889</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
@@ -2581,17 +2593,17 @@
         <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="C111" s="2">
-        <v>45915.220127314817</v>
+        <v>45915.055277777778</v>
       </c>
       <c r="D111" s="2">
-        <v>45916.216979166667</v>
+        <v>45916.095949074072</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
@@ -2599,85 +2611,85 @@
         <v>6</v>
       </c>
       <c r="B112" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C112" s="2">
-        <v>45917.543113425927</v>
+        <v>45915.483831018515</v>
       </c>
       <c r="D112" s="2">
-        <v>45918.545127314814</v>
+        <v>45916.511701388888</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C113" s="2">
-        <v>45910.041087962964</v>
+        <v>45914.036979166667</v>
       </c>
       <c r="D113" s="2">
-        <v>45911.026550925926</v>
+        <v>45915.079004629632</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B114" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C114" s="2">
-        <v>45919.033101851855</v>
+        <v>45919.036516203705</v>
       </c>
       <c r="D114" s="2">
-        <v>45920.037638888891</v>
+        <v>45920.041701388887</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B115" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C115" s="2">
-        <v>45915.020277777781</v>
+        <v>45910.196134259262</v>
       </c>
       <c r="D115" s="2">
-        <v>45916.002210648148</v>
+        <v>45911.248784722222</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B116" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C116" s="2">
-        <v>45913.029675925929</v>
+        <v>45919.566770833335</v>
       </c>
       <c r="D116" s="2">
-        <v>45914.000960648147</v>
+        <v>45920.544930555552</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116">
@@ -2686,16 +2698,16 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B117" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C117" s="2">
-        <v>45919.028819444444</v>
+        <v>45912.242094907408</v>
       </c>
       <c r="D117" s="2">
-        <v>45920.000590277778</v>
+        <v>45913.231030092589</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117">
@@ -2704,16 +2716,16 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B118" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C118" s="2">
-        <v>45913.030231481483</v>
+        <v>45913.530856481484</v>
       </c>
       <c r="D118" s="2">
-        <v>45914.003888888888</v>
+        <v>45914.507928240739</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118">
@@ -2722,16 +2734,16 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B119" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C119" s="2">
-        <v>45918.378263888888</v>
+        <v>45914.043333333335</v>
       </c>
       <c r="D119" s="2">
-        <v>45919.401689814818</v>
+        <v>45915.064780092594</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119">
@@ -2740,16 +2752,16 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B120" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C120" s="2">
-        <v>45918.039143518516</v>
+        <v>45914.019074074073</v>
       </c>
       <c r="D120" s="2">
-        <v>45919.000752314816</v>
+        <v>45915.000347222223</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120">
@@ -2758,16 +2770,16 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B121" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C121" s="2">
-        <v>45915.572175925925</v>
+        <v>45917.562847222223</v>
       </c>
       <c r="D121" s="2">
-        <v>45916.543171296296</v>
+        <v>45918.543981481482</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121">
@@ -2776,16 +2788,16 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B122" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C122" s="2">
-        <v>45910.584328703706</v>
+        <v>45915.540833333333</v>
       </c>
       <c r="D122" s="2">
-        <v>45911.616053240738</v>
+        <v>45916.513043981482</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122">
@@ -2794,16 +2806,16 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B123" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C123" s="2">
-        <v>45919.277962962966</v>
+        <v>45915.55263888889</v>
       </c>
       <c r="D123" s="2">
-        <v>45920.264999999999</v>
+        <v>45916.542962962965</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123">
@@ -2812,34 +2824,34 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B124" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C124" s="2">
-        <v>45916.019108796296</v>
-      </c>
-      <c r="D124" s="2">
-        <v>45917.00277777778</v>
-      </c>
-      <c r="E124" s="2"/>
+        <v>45919.638368055559</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F124">
         <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C125" s="2">
-        <v>45916.579988425925</v>
+        <v>45910.510555555556</v>
       </c>
       <c r="D125" s="2">
-        <v>45917.561284722222</v>
+        <v>45911.524016203701</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125">
@@ -2848,16 +2860,16 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B126" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C126" s="2">
-        <v>45911.556932870371</v>
+        <v>45913.030231481483</v>
       </c>
       <c r="D126" s="2">
-        <v>45912.543055555558</v>
+        <v>45914.003888888888</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126">
@@ -2866,16 +2878,16 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B127" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C127" s="2">
-        <v>45912.03328703704</v>
+        <v>45917.543113425927</v>
       </c>
       <c r="D127" s="2">
-        <v>45913.003379629627</v>
+        <v>45918.545127314814</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127">
@@ -2884,16 +2896,16 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B128" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C128" s="2">
-        <v>45913.032546296294</v>
+        <v>45910.584328703706</v>
       </c>
       <c r="D128" s="2">
-        <v>45914.002326388887</v>
+        <v>45911.616053240738</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128">
@@ -2902,16 +2914,16 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B129" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C129" s="2">
-        <v>45910.02920138889</v>
+        <v>45915.020277777781</v>
       </c>
       <c r="D129" s="2">
-        <v>45911.005185185182</v>
+        <v>45916.002210648148</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129">
@@ -2920,16 +2932,16 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B130" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C130" s="2">
-        <v>45911.034571759257</v>
+        <v>45918.378263888888</v>
       </c>
       <c r="D130" s="2">
-        <v>45912.001400462963</v>
+        <v>45919.401689814818</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130">
@@ -2938,16 +2950,16 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B131" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C131" s="2">
-        <v>45914.0625</v>
+        <v>45917.243622685186</v>
       </c>
       <c r="D131" s="2">
-        <v>45915.059525462966</v>
+        <v>45918.209560185183</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131">
@@ -2956,16 +2968,16 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B132" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C132" s="2">
-        <v>45919.031469907408</v>
+        <v>45915.572175925925</v>
       </c>
       <c r="D132" s="2">
-        <v>45920.003437500003</v>
+        <v>45916.543171296296</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132">
@@ -2974,16 +2986,16 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="C133" s="2">
-        <v>45915.55263888889</v>
+        <v>45913.701620370368</v>
       </c>
       <c r="D133" s="2">
-        <v>45916.542962962965</v>
+        <v>45914.694907407407</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133">
@@ -2992,16 +3004,16 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B134" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C134" s="2">
-        <v>45914.043333333335</v>
+        <v>45915.220127314817</v>
       </c>
       <c r="D134" s="2">
-        <v>45915.064780092594</v>
+        <v>45916.216979166667</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134">
@@ -3010,16 +3022,16 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C135" s="2">
-        <v>45915.540833333333</v>
+        <v>45910.041087962964</v>
       </c>
       <c r="D135" s="2">
-        <v>45916.513043981482</v>
+        <v>45911.026550925926</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135">
@@ -3028,16 +3040,16 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B136" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C136" s="2">
-        <v>45914.019074074073</v>
+        <v>45919.033101851855</v>
       </c>
       <c r="D136" s="2">
-        <v>45915.000347222223</v>
+        <v>45920.037638888891</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136">
@@ -3046,16 +3058,16 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B137" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C137" s="2">
-        <v>45917.562847222223</v>
+        <v>45913.029675925929</v>
       </c>
       <c r="D137" s="2">
-        <v>45918.543981481482</v>
+        <v>45914.000960648147</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137">
@@ -3064,16 +3076,16 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B138" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C138" s="2">
-        <v>45910.510555555556</v>
+        <v>45919.028819444444</v>
       </c>
       <c r="D138" s="2">
-        <v>45911.524016203701</v>
+        <v>45920.000590277778</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138">
@@ -3082,16 +3094,16 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B139" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C139" s="2">
-        <v>45912.242094907408</v>
+        <v>45918.039143518516</v>
       </c>
       <c r="D139" s="2">
-        <v>45913.231030092589</v>
+        <v>45919.000752314816</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139">
@@ -3100,16 +3112,16 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B140" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C140" s="2">
-        <v>45913.530856481484</v>
+        <v>45916.019108796296</v>
       </c>
       <c r="D140" s="2">
-        <v>45914.507928240739</v>
+        <v>45917.00277777778</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140">
@@ -3118,37 +3130,163 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B141" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C141" s="2">
-        <v>45919.362210648149</v>
-      </c>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45910.02920138889</v>
+      </c>
+      <c r="D141" s="2">
+        <v>45911.005185185182</v>
+      </c>
+      <c r="E141" s="2"/>
       <c r="F141">
         <v>24</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B142" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C142" s="2">
-        <v>45919.351388888892</v>
-      </c>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45911.034571759257</v>
+      </c>
+      <c r="D142" s="2">
+        <v>45912.001400462963</v>
+      </c>
+      <c r="E142" s="2"/>
       <c r="F142">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A143" t="s">
+        <v>8</v>
+      </c>
+      <c r="B143" t="s">
+        <v>30</v>
+      </c>
+      <c r="C143" s="2">
+        <v>45914.0625</v>
+      </c>
+      <c r="D143" s="2">
+        <v>45915.059525462966</v>
+      </c>
+      <c r="E143" s="2"/>
+      <c r="F143">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A144" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" s="2">
+        <v>45919.277962962966</v>
+      </c>
+      <c r="D144" s="2">
+        <v>45920.264999999999</v>
+      </c>
+      <c r="E144" s="2"/>
+      <c r="F144">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A145" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" t="s">
+        <v>13</v>
+      </c>
+      <c r="C145" s="2">
+        <v>45911.556932870371</v>
+      </c>
+      <c r="D145" s="2">
+        <v>45912.543055555558</v>
+      </c>
+      <c r="E145" s="2"/>
+      <c r="F145">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A146" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" s="2">
+        <v>45916.579988425925</v>
+      </c>
+      <c r="D146" s="2">
+        <v>45917.561284722222</v>
+      </c>
+      <c r="E146" s="2"/>
+      <c r="F146">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A147" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147" t="s">
+        <v>49</v>
+      </c>
+      <c r="C147" s="2">
+        <v>45912.03328703704</v>
+      </c>
+      <c r="D147" s="2">
+        <v>45913.003379629627</v>
+      </c>
+      <c r="E147" s="2"/>
+      <c r="F147">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A148" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" t="s">
+        <v>45</v>
+      </c>
+      <c r="C148" s="2">
+        <v>45913.032546296294</v>
+      </c>
+      <c r="D148" s="2">
+        <v>45914.002326388887</v>
+      </c>
+      <c r="E148" s="2"/>
+      <c r="F148">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A149" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" t="s">
+        <v>36</v>
+      </c>
+      <c r="C149" s="2">
+        <v>45919.031469907408</v>
+      </c>
+      <c r="D149" s="2">
+        <v>45920.003437500003</v>
+      </c>
+      <c r="E149" s="2"/>
+      <c r="F149">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-20 16:50:22.64
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="71">
   <si>
     <t>电站名称</t>
   </si>
@@ -218,6 +218,18 @@
   </si>
   <si>
     <t>011A号直流</t>
+  </si>
+  <si>
+    <t>307号直流</t>
+  </si>
+  <si>
+    <t>207号直流</t>
+  </si>
+  <si>
+    <t>208号直流</t>
+  </si>
+  <si>
+    <t>308号直流</t>
   </si>
 </sst>
 </file>
@@ -578,21 +590,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="42.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="23.25" customWidth="1"/>
-    <col min="5" max="5" width="22.25" customWidth="1"/>
-    <col min="6" max="6" width="16.75" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="31.375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -626,10 +630,10 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>45920.341481481482</v>
+        <v>45920.649699074071</v>
       </c>
       <c r="F2">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -644,46 +648,46 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
-        <v>45920.341481481482</v>
+        <v>45920.649699074071</v>
       </c>
       <c r="F3">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
-        <v>45911.52857638889</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45915.503275462965</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>45916.534282407411</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F4">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2">
-        <v>45916.534282407411</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45911.52857638889</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45915.503275462965</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -706,20 +710,20 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2">
-        <v>45913.052685185183</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45916.265127314815</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>45917.258240740739</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F7">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -732,30 +736,30 @@
       <c r="C8" s="2">
         <v>45917.260844907411</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>45920.341481481482</v>
-      </c>
+      <c r="D8" s="2">
+        <v>45920.502418981479</v>
+      </c>
+      <c r="E8" s="2"/>
       <c r="F8">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2">
-        <v>45917.258240740739</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45913.052685185183</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45916.265127314815</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -835,17 +839,17 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2">
-        <v>45913.006967592592</v>
+        <v>45918.06113425926</v>
       </c>
       <c r="D14" s="2">
-        <v>45915.473703703705</v>
+        <v>45920.554386574076</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -853,17 +857,17 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
-        <v>45918.06113425926</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45913.006967592592</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45915.473703703705</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -886,38 +890,38 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2">
-        <v>45910.355798611112</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45912.393368055556</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>45918.557500000003</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F17">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2">
-        <v>45911.040381944447</v>
+        <v>45910.355798611112</v>
       </c>
       <c r="D18" s="2">
-        <v>45913.023263888892</v>
+        <v>45912.393368055556</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -925,17 +929,17 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2">
-        <v>45912.060983796298</v>
+        <v>45918.603634259256</v>
       </c>
       <c r="D19" s="2">
-        <v>45914.012141203704</v>
+        <v>45920.611122685186</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -943,31 +947,31 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2">
-        <v>45915.583414351851</v>
+        <v>45911.040381944447</v>
       </c>
       <c r="D20" s="2">
-        <v>45917.582627314812</v>
+        <v>45913.023263888892</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2">
-        <v>45910.5781712963</v>
+        <v>45910.561724537038</v>
       </c>
       <c r="D21" s="2">
-        <v>45912.528969907406</v>
+        <v>45912.509375000001</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21">
@@ -976,16 +980,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2">
-        <v>45910.561724537038</v>
+        <v>45912.060983796298</v>
       </c>
       <c r="D22" s="2">
-        <v>45912.509375000001</v>
+        <v>45914.012141203704</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22">
@@ -994,70 +998,70 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C23" s="2">
-        <v>45914.560046296298</v>
+        <v>45915.583414351851</v>
       </c>
       <c r="D23" s="2">
-        <v>45916.478472222225</v>
+        <v>45917.582627314812</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C24" s="2">
-        <v>45911.646747685183</v>
+        <v>45910.5781712963</v>
       </c>
       <c r="D24" s="2">
-        <v>45913.523923611108</v>
+        <v>45912.528969907406</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2">
-        <v>45911.562384259261</v>
+        <v>45914.560046296298</v>
       </c>
       <c r="D25" s="2">
-        <v>45913.435532407406</v>
+        <v>45916.478472222225</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C26" s="2">
-        <v>45917.638888888891</v>
+        <v>45917.219965277778</v>
       </c>
       <c r="D26" s="2">
-        <v>45919.518240740741</v>
+        <v>45919.087418981479</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26">
@@ -1066,16 +1070,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C27" s="2">
-        <v>45917.219965277778</v>
+        <v>45911.646747685183</v>
       </c>
       <c r="D27" s="2">
-        <v>45919.087418981479</v>
+        <v>45913.523923611108</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27">
@@ -1087,35 +1091,35 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C28" s="2">
-        <v>45917.200092592589</v>
+        <v>45911.562384259261</v>
       </c>
       <c r="D28" s="2">
-        <v>45918.990624999999</v>
+        <v>45913.435532407406</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2">
-        <v>45915.231793981482</v>
+        <v>45917.638888888891</v>
       </c>
       <c r="D29" s="2">
-        <v>45917.019432870373</v>
+        <v>45919.518240740741</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -1138,18 +1142,18 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C31" s="2">
-        <v>45918.557500000003</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45915.231793981482</v>
+      </c>
+      <c r="D31" s="2">
+        <v>45917.019432870373</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="F31">
         <v>43</v>
       </c>
@@ -1159,31 +1163,31 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C32" s="2">
-        <v>45918.603634259256</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45917.200092592589</v>
+      </c>
+      <c r="D32" s="2">
+        <v>45918.990624999999</v>
+      </c>
+      <c r="E32" s="2"/>
       <c r="F32">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2">
-        <v>45913.23265046296</v>
+        <v>45913.76421296296</v>
       </c>
       <c r="D33" s="2">
-        <v>45914.981087962966</v>
+        <v>45915.539942129632</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33">
@@ -1192,16 +1196,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2">
-        <v>45913.76421296296</v>
+        <v>45913.23265046296</v>
       </c>
       <c r="D34" s="2">
-        <v>45915.539942129632</v>
+        <v>45914.981087962966</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34">
@@ -1246,36 +1250,36 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C37" s="2">
-        <v>45911.531018518515</v>
+        <v>45918.673472222225</v>
       </c>
       <c r="D37" s="2">
-        <v>45913.206875000003</v>
+        <v>45920.394062500003</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C38" s="2">
-        <v>45918.673472222225</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45911.531018518515</v>
+      </c>
+      <c r="D38" s="2">
+        <v>45913.206875000003</v>
+      </c>
+      <c r="E38" s="2"/>
       <c r="F38">
         <v>40</v>
       </c>
@@ -1285,17 +1289,17 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45915.111643518518</v>
+      </c>
+      <c r="D39" s="2">
+        <v>45916.694467592592</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39">
         <v>38</v>
-      </c>
-      <c r="C39" s="2">
-        <v>45918.715682870374</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2">
-        <v>45920.341481481482</v>
-      </c>
-      <c r="F39">
-        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -1303,13 +1307,13 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C40" s="2">
-        <v>45915.111643518518</v>
+        <v>45918.715682870374</v>
       </c>
       <c r="D40" s="2">
-        <v>45916.694467592592</v>
+        <v>45920.332812499997</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40">
@@ -1321,17 +1325,17 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C41" s="2">
-        <v>45914.486261574071</v>
-      </c>
-      <c r="D41" s="2">
-        <v>45916.002962962964</v>
-      </c>
-      <c r="E41" s="2"/>
+        <v>45919.051585648151</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F41">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
@@ -1339,31 +1343,31 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C42" s="2">
-        <v>45910.534502314818</v>
+        <v>45914.486261574071</v>
       </c>
       <c r="D42" s="2">
-        <v>45912.012048611112</v>
+        <v>45916.002962962964</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C43" s="2">
-        <v>45916.051249999997</v>
+        <v>45918.526932870373</v>
       </c>
       <c r="D43" s="2">
-        <v>45917.567256944443</v>
+        <v>45920.000578703701</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43">
@@ -1372,16 +1376,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C44" s="2">
-        <v>45915.061967592592</v>
+        <v>45918.539907407408</v>
       </c>
       <c r="D44" s="2">
-        <v>45916.546516203707</v>
+        <v>45920.001921296294</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44">
@@ -1390,16 +1394,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C45" s="2">
-        <v>45915.025833333333</v>
+        <v>45910.534502314818</v>
       </c>
       <c r="D45" s="2">
-        <v>45916.511203703703</v>
+        <v>45912.012048611112</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45">
@@ -1408,16 +1412,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C46" s="2">
-        <v>45918.539907407408</v>
+        <v>45916.051249999997</v>
       </c>
       <c r="D46" s="2">
-        <v>45920.001921296294</v>
+        <v>45917.567256944443</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46">
@@ -1426,16 +1430,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C47" s="2">
-        <v>45918.526932870373</v>
+        <v>45915.061967592592</v>
       </c>
       <c r="D47" s="2">
-        <v>45920.000578703701</v>
+        <v>45916.546516203707</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47">
@@ -1444,20 +1448,20 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C48" s="2">
-        <v>45913.717233796298</v>
+        <v>45915.025833333333</v>
       </c>
       <c r="D48" s="2">
-        <v>45915.203182870369</v>
+        <v>45916.511203703703</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
@@ -1465,13 +1469,13 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C49" s="2">
-        <v>45913.566805555558</v>
+        <v>45918.54587962963</v>
       </c>
       <c r="D49" s="2">
-        <v>45915.004942129628</v>
+        <v>45920.000509259262</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49">
@@ -1483,13 +1487,13 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C50" s="2">
-        <v>45918.54587962963</v>
+        <v>45913.717233796298</v>
       </c>
       <c r="D50" s="2">
-        <v>45920.000509259262</v>
+        <v>45915.203182870369</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50">
@@ -1501,13 +1505,13 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C51" s="2">
-        <v>45917.128229166665</v>
+        <v>45913.566805555558</v>
       </c>
       <c r="D51" s="2">
-        <v>45918.609236111108</v>
+        <v>45915.004942129628</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51">
@@ -1516,16 +1520,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C52" s="2">
-        <v>45912.567314814813</v>
+        <v>45917.128229166665</v>
       </c>
       <c r="D52" s="2">
-        <v>45914.04074074074</v>
+        <v>45918.609236111108</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52">
@@ -1534,34 +1538,34 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C53" s="2">
-        <v>45916.059074074074</v>
+        <v>45912.567314814813</v>
       </c>
       <c r="D53" s="2">
-        <v>45917.468865740739</v>
+        <v>45914.04074074074</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C54" s="2">
-        <v>45916.623356481483</v>
+        <v>45914.050219907411</v>
       </c>
       <c r="D54" s="2">
-        <v>45918.0237037037</v>
+        <v>45915.466817129629</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54">
@@ -1573,13 +1577,13 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C55" s="2">
-        <v>45917.589189814818</v>
+        <v>45915.541979166665</v>
       </c>
       <c r="D55" s="2">
-        <v>45919.000393518516</v>
+        <v>45916.988449074073</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55">
@@ -1591,13 +1595,13 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C56" s="2">
-        <v>45915.541979166665</v>
+        <v>45916.059074074074</v>
       </c>
       <c r="D56" s="2">
-        <v>45916.988449074073</v>
+        <v>45917.468865740739</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56">
@@ -1606,16 +1610,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C57" s="2">
-        <v>45914.050219907411</v>
+        <v>45916.623356481483</v>
       </c>
       <c r="D57" s="2">
-        <v>45915.466817129629</v>
+        <v>45918.0237037037</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57">
@@ -1624,38 +1628,38 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C58" s="2">
-        <v>45912.627604166664</v>
+        <v>45917.589189814818</v>
       </c>
       <c r="D58" s="2">
-        <v>45914.005208333336</v>
+        <v>45919.000393518516</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C59" s="2">
-        <v>45910.054398148146</v>
+        <v>45912.627604166664</v>
       </c>
       <c r="D59" s="2">
-        <v>45911.384293981479</v>
+        <v>45914.005208333336</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
@@ -1663,17 +1667,17 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C60" s="2">
-        <v>45915.259062500001</v>
+        <v>45910.054398148146</v>
       </c>
       <c r="D60" s="2">
-        <v>45916.545428240737</v>
+        <v>45911.384293981479</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
@@ -1681,17 +1685,17 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C61" s="2">
-        <v>45917.051562499997</v>
-      </c>
-      <c r="D61" s="2">
-        <v>45918.348865740743</v>
-      </c>
-      <c r="E61" s="2"/>
+        <v>45919.2965625</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F61">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
@@ -1699,13 +1703,13 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C62" s="2">
-        <v>45916.531759259262</v>
+        <v>45910.247546296298</v>
       </c>
       <c r="D62" s="2">
-        <v>45917.797986111109</v>
+        <v>45911.529826388891</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62">
@@ -1717,15 +1721,15 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C63" s="2">
-        <v>45919.051585648151</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45915.259062500001</v>
+      </c>
+      <c r="D63" s="2">
+        <v>45916.545428240737</v>
+      </c>
+      <c r="E63" s="2"/>
       <c r="F63">
         <v>31</v>
       </c>
@@ -1735,13 +1739,13 @@
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C64" s="2">
-        <v>45910.247546296298</v>
+        <v>45917.051562499997</v>
       </c>
       <c r="D64" s="2">
-        <v>45911.529826388891</v>
+        <v>45918.348865740743</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64">
@@ -1750,16 +1754,16 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C65" s="2">
-        <v>45918.712372685186</v>
+        <v>45916.531759259262</v>
       </c>
       <c r="D65" s="2">
-        <v>45920.004004629627</v>
+        <v>45917.797986111109</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65">
@@ -1768,34 +1772,34 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C66" s="2">
-        <v>45917.038738425923</v>
+        <v>45918.712372685186</v>
       </c>
       <c r="D66" s="2">
-        <v>45918.261030092595</v>
+        <v>45920.004004629627</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C67" s="2">
-        <v>45918.264537037037</v>
+        <v>45919.267326388886</v>
       </c>
       <c r="D67" s="2">
-        <v>45919.504305555558</v>
+        <v>45920.507592592592</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67">
@@ -1807,13 +1811,13 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C68" s="2">
-        <v>45918.257824074077</v>
+        <v>45918.264537037037</v>
       </c>
       <c r="D68" s="2">
-        <v>45919.535219907404</v>
+        <v>45919.504305555558</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68">
@@ -1825,17 +1829,17 @@
         <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C69" s="2">
-        <v>45913.050844907404</v>
+        <v>45917.038738425923</v>
       </c>
       <c r="D69" s="2">
-        <v>45914.284895833334</v>
+        <v>45918.261030092595</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
@@ -1843,31 +1847,31 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="C70" s="2">
-        <v>45915.250428240739</v>
+        <v>45918.257824074077</v>
       </c>
       <c r="D70" s="2">
-        <v>45916.492291666669</v>
+        <v>45919.535219907404</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C71" s="2">
-        <v>45910.067824074074</v>
+        <v>45914.304675925923</v>
       </c>
       <c r="D71" s="2">
-        <v>45911.284560185188</v>
+        <v>45915.505648148152</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71">
@@ -1876,16 +1880,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C72" s="2">
-        <v>45914.064189814817</v>
+        <v>45916.350173611114</v>
       </c>
       <c r="D72" s="2">
-        <v>45915.274594907409</v>
+        <v>45917.544189814813</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72">
@@ -1912,16 +1916,16 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C74" s="2">
-        <v>45914.304675925923</v>
+        <v>45915.250428240739</v>
       </c>
       <c r="D74" s="2">
-        <v>45915.505648148152</v>
+        <v>45916.492291666669</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74">
@@ -1930,16 +1934,16 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C75" s="2">
-        <v>45916.350173611114</v>
+        <v>45913.050844907404</v>
       </c>
       <c r="D75" s="2">
-        <v>45917.544189814813</v>
+        <v>45914.284895833334</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75">
@@ -1951,49 +1955,49 @@
         <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C76" s="2">
-        <v>45910.356319444443</v>
+        <v>45910.067824074074</v>
       </c>
       <c r="D76" s="2">
-        <v>45911.500925925924</v>
+        <v>45911.284560185188</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C77" s="2">
-        <v>45917.046249999999</v>
+        <v>45914.064189814817</v>
       </c>
       <c r="D77" s="2">
-        <v>45918.227696759262</v>
+        <v>45915.274594907409</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C78" s="2">
-        <v>45914.011388888888</v>
+        <v>45914.060752314814</v>
       </c>
       <c r="D78" s="2">
-        <v>45915.187569444446</v>
+        <v>45915.225474537037</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78">
@@ -2005,13 +2009,13 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C79" s="2">
-        <v>45915.035682870373</v>
+        <v>45910.356319444443</v>
       </c>
       <c r="D79" s="2">
-        <v>45916.204282407409</v>
+        <v>45911.500925925924</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79">
@@ -2020,16 +2024,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="C80" s="2">
-        <v>45919.064259259256</v>
+        <v>45917.046249999999</v>
       </c>
       <c r="D80" s="2">
-        <v>45920.216261574074</v>
+        <v>45918.227696759262</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80">
@@ -2038,16 +2042,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C81" s="2">
-        <v>45917.862303240741</v>
+        <v>45914.011388888888</v>
       </c>
       <c r="D81" s="2">
-        <v>45919.004907407405</v>
+        <v>45915.187569444446</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81">
@@ -2056,16 +2060,16 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C82" s="2">
-        <v>45914.060752314814</v>
+        <v>45915.035682870373</v>
       </c>
       <c r="D82" s="2">
-        <v>45915.225474537037</v>
+        <v>45916.204282407409</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82">
@@ -2074,52 +2078,52 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C83" s="2">
-        <v>45912.041076388887</v>
+        <v>45919.064259259256</v>
       </c>
       <c r="D83" s="2">
-        <v>45913.145925925928</v>
+        <v>45920.216261574074</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B84" t="s">
         <v>44</v>
       </c>
       <c r="C84" s="2">
-        <v>45915.075706018521</v>
+        <v>45917.862303240741</v>
       </c>
       <c r="D84" s="2">
-        <v>45916.188900462963</v>
+        <v>45919.004907407405</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B85" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C85" s="2">
-        <v>45913.579629629632</v>
+        <v>45919.362210648149</v>
       </c>
       <c r="D85" s="2">
-        <v>45914.686932870369</v>
+        <v>45920.481516203705</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85">
@@ -2128,16 +2132,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C86" s="2">
-        <v>45914.151493055557</v>
+        <v>45913.042430555557</v>
       </c>
       <c r="D86" s="2">
-        <v>45915.287997685184</v>
+        <v>45914.200810185182</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86">
@@ -2164,16 +2168,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C88" s="2">
-        <v>45911.012094907404</v>
+        <v>45915.075706018521</v>
       </c>
       <c r="D88" s="2">
-        <v>45912.137696759259</v>
+        <v>45916.188900462963</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88">
@@ -2182,16 +2186,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C89" s="2">
-        <v>45913.042430555557</v>
+        <v>45912.041076388887</v>
       </c>
       <c r="D89" s="2">
-        <v>45914.200810185182</v>
+        <v>45913.145925925928</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89">
@@ -2200,124 +2204,124 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C90" s="2">
-        <v>45913.064467592594</v>
+        <v>45913.579629629632</v>
       </c>
       <c r="D90" s="2">
-        <v>45914.140983796293</v>
+        <v>45914.686932870369</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C91" s="2">
-        <v>45919.267326388886</v>
-      </c>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45914.151493055557</v>
+      </c>
+      <c r="D91" s="2">
+        <v>45915.287997685184</v>
+      </c>
+      <c r="E91" s="2"/>
       <c r="F91">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C92" s="2">
-        <v>45911.684641203705</v>
+        <v>45911.012094907404</v>
       </c>
       <c r="D92" s="2">
-        <v>45912.726527777777</v>
+        <v>45912.137696759259</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="C93" s="2">
-        <v>45919.067708333336</v>
-      </c>
-      <c r="D93" s="2">
-        <v>45920.088587962964</v>
-      </c>
-      <c r="E93" s="2"/>
+        <v>45919.528935185182</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F93">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B94" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C94" s="2">
-        <v>45915.475578703707</v>
+        <v>45919.351388888892</v>
       </c>
       <c r="D94" s="2">
-        <v>45916.538958333331</v>
+        <v>45920.447187500002</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C95" s="2">
-        <v>45917.244652777779</v>
+        <v>45913.064467592594</v>
       </c>
       <c r="D95" s="2">
-        <v>45918.285451388889</v>
+        <v>45914.140983796293</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B96" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C96" s="2">
-        <v>45911.994386574072</v>
+        <v>45911.244166666664</v>
       </c>
       <c r="D96" s="2">
-        <v>45913.008622685185</v>
+        <v>45912.265601851854</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96">
@@ -2326,16 +2330,16 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B97" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C97" s="2">
-        <v>45918.199444444443</v>
+        <v>45911.504976851851</v>
       </c>
       <c r="D97" s="2">
-        <v>45919.209988425922</v>
+        <v>45912.543333333335</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97">
@@ -2344,16 +2348,16 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B98" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C98" s="2">
-        <v>45912.043020833335</v>
+        <v>45915.525405092594</v>
       </c>
       <c r="D98" s="2">
-        <v>45913.113923611112</v>
+        <v>45916.54210648148</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98">
@@ -2362,70 +2366,70 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B99" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C99" s="2">
-        <v>45919.2965625</v>
-      </c>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45919.499756944446</v>
+      </c>
+      <c r="D99" s="2">
+        <v>45920.505324074074</v>
+      </c>
+      <c r="E99" s="2"/>
       <c r="F99">
         <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B100" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C100" s="2">
-        <v>45915.055277777778</v>
-      </c>
-      <c r="D100" s="2">
-        <v>45916.095949074072</v>
-      </c>
-      <c r="E100" s="2"/>
+        <v>45919.605023148149</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F100">
         <v>25</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="C101" s="2">
-        <v>45915.483831018515</v>
-      </c>
-      <c r="D101" s="2">
-        <v>45916.511701388888</v>
-      </c>
-      <c r="E101" s="2"/>
+        <v>45919.589224537034</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F101">
         <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C102" s="2">
-        <v>45914.036979166667</v>
+        <v>45919.472337962965</v>
       </c>
       <c r="D102" s="2">
-        <v>45915.079004629632</v>
+        <v>45920.537222222221</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102">
@@ -2434,16 +2438,16 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C103" s="2">
-        <v>45919.036516203705</v>
+        <v>45913.021006944444</v>
       </c>
       <c r="D103" s="2">
-        <v>45920.041701388887</v>
+        <v>45914.078969907408</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103">
@@ -2452,16 +2456,16 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B104" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C104" s="2">
-        <v>45910.196134259262</v>
+        <v>45915.475578703707</v>
       </c>
       <c r="D104" s="2">
-        <v>45911.248784722222</v>
+        <v>45916.538958333331</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104">
@@ -2470,16 +2474,16 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C105" s="2">
-        <v>45913.021006944444</v>
+        <v>45911.994386574072</v>
       </c>
       <c r="D105" s="2">
-        <v>45914.078969907408</v>
+        <v>45913.008622685185</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105">
@@ -2488,16 +2492,16 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C106" s="2">
-        <v>45911.244166666664</v>
+        <v>45918.199444444443</v>
       </c>
       <c r="D106" s="2">
-        <v>45912.265601851854</v>
+        <v>45919.209988425922</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106">
@@ -2506,16 +2510,16 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C107" s="2">
-        <v>45911.504976851851</v>
+        <v>45912.043020833335</v>
       </c>
       <c r="D107" s="2">
-        <v>45912.543333333335</v>
+        <v>45913.113923611112</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107">
@@ -2524,16 +2528,16 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C108" s="2">
-        <v>45915.525405092594</v>
+        <v>45911.684641203705</v>
       </c>
       <c r="D108" s="2">
-        <v>45916.54210648148</v>
+        <v>45912.726527777777</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108">
@@ -2545,17 +2549,17 @@
         <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C109" s="2">
-        <v>45917.243622685186</v>
+        <v>45919.067708333336</v>
       </c>
       <c r="D109" s="2">
-        <v>45918.209560185183</v>
+        <v>45920.088587962964</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
@@ -2563,17 +2567,17 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C110" s="2">
-        <v>45913.701620370368</v>
+        <v>45917.244652777779</v>
       </c>
       <c r="D110" s="2">
-        <v>45914.694907407407</v>
+        <v>45918.285451388889</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
@@ -2581,17 +2585,17 @@
         <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="C111" s="2">
-        <v>45915.220127314817</v>
+        <v>45915.055277777778</v>
       </c>
       <c r="D111" s="2">
-        <v>45916.216979166667</v>
+        <v>45916.095949074072</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
@@ -2599,85 +2603,85 @@
         <v>6</v>
       </c>
       <c r="B112" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C112" s="2">
-        <v>45917.543113425927</v>
+        <v>45915.483831018515</v>
       </c>
       <c r="D112" s="2">
-        <v>45918.545127314814</v>
+        <v>45916.511701388888</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C113" s="2">
-        <v>45910.041087962964</v>
+        <v>45914.036979166667</v>
       </c>
       <c r="D113" s="2">
-        <v>45911.026550925926</v>
+        <v>45915.079004629632</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B114" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C114" s="2">
-        <v>45919.033101851855</v>
+        <v>45919.036516203705</v>
       </c>
       <c r="D114" s="2">
-        <v>45920.037638888891</v>
+        <v>45920.041701388887</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B115" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C115" s="2">
-        <v>45915.020277777781</v>
+        <v>45910.196134259262</v>
       </c>
       <c r="D115" s="2">
-        <v>45916.002210648148</v>
+        <v>45911.248784722222</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B116" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C116" s="2">
-        <v>45913.029675925929</v>
+        <v>45919.566770833335</v>
       </c>
       <c r="D116" s="2">
-        <v>45914.000960648147</v>
+        <v>45920.544930555552</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116">
@@ -2686,16 +2690,16 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B117" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C117" s="2">
-        <v>45919.028819444444</v>
+        <v>45912.242094907408</v>
       </c>
       <c r="D117" s="2">
-        <v>45920.000590277778</v>
+        <v>45913.231030092589</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117">
@@ -2704,16 +2708,16 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B118" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C118" s="2">
-        <v>45913.030231481483</v>
+        <v>45913.530856481484</v>
       </c>
       <c r="D118" s="2">
-        <v>45914.003888888888</v>
+        <v>45914.507928240739</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118">
@@ -2722,16 +2726,16 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B119" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C119" s="2">
-        <v>45918.378263888888</v>
+        <v>45914.043333333335</v>
       </c>
       <c r="D119" s="2">
-        <v>45919.401689814818</v>
+        <v>45915.064780092594</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119">
@@ -2740,16 +2744,16 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B120" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C120" s="2">
-        <v>45918.039143518516</v>
+        <v>45914.019074074073</v>
       </c>
       <c r="D120" s="2">
-        <v>45919.000752314816</v>
+        <v>45915.000347222223</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120">
@@ -2758,16 +2762,16 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B121" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C121" s="2">
-        <v>45915.572175925925</v>
+        <v>45917.562847222223</v>
       </c>
       <c r="D121" s="2">
-        <v>45916.543171296296</v>
+        <v>45918.543981481482</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121">
@@ -2776,16 +2780,16 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B122" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C122" s="2">
-        <v>45910.584328703706</v>
+        <v>45915.540833333333</v>
       </c>
       <c r="D122" s="2">
-        <v>45911.616053240738</v>
+        <v>45916.513043981482</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122">
@@ -2794,16 +2798,16 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B123" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C123" s="2">
-        <v>45919.277962962966</v>
+        <v>45915.55263888889</v>
       </c>
       <c r="D123" s="2">
-        <v>45920.264999999999</v>
+        <v>45916.542962962965</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123">
@@ -2812,34 +2816,34 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B124" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C124" s="2">
-        <v>45916.019108796296</v>
-      </c>
-      <c r="D124" s="2">
-        <v>45917.00277777778</v>
-      </c>
-      <c r="E124" s="2"/>
+        <v>45919.638368055559</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2">
+        <v>45920.649699074071</v>
+      </c>
       <c r="F124">
         <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C125" s="2">
-        <v>45916.579988425925</v>
+        <v>45910.510555555556</v>
       </c>
       <c r="D125" s="2">
-        <v>45917.561284722222</v>
+        <v>45911.524016203701</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125">
@@ -2848,16 +2852,16 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B126" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C126" s="2">
-        <v>45911.556932870371</v>
+        <v>45913.030231481483</v>
       </c>
       <c r="D126" s="2">
-        <v>45912.543055555558</v>
+        <v>45914.003888888888</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126">
@@ -2866,16 +2870,16 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B127" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C127" s="2">
-        <v>45912.03328703704</v>
+        <v>45917.543113425927</v>
       </c>
       <c r="D127" s="2">
-        <v>45913.003379629627</v>
+        <v>45918.545127314814</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127">
@@ -2884,16 +2888,16 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B128" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C128" s="2">
-        <v>45913.032546296294</v>
+        <v>45910.584328703706</v>
       </c>
       <c r="D128" s="2">
-        <v>45914.002326388887</v>
+        <v>45911.616053240738</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128">
@@ -2902,16 +2906,16 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B129" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C129" s="2">
-        <v>45910.02920138889</v>
+        <v>45915.020277777781</v>
       </c>
       <c r="D129" s="2">
-        <v>45911.005185185182</v>
+        <v>45916.002210648148</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129">
@@ -2920,16 +2924,16 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B130" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C130" s="2">
-        <v>45911.034571759257</v>
+        <v>45918.378263888888</v>
       </c>
       <c r="D130" s="2">
-        <v>45912.001400462963</v>
+        <v>45919.401689814818</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130">
@@ -2938,16 +2942,16 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B131" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C131" s="2">
-        <v>45914.0625</v>
+        <v>45917.243622685186</v>
       </c>
       <c r="D131" s="2">
-        <v>45915.059525462966</v>
+        <v>45918.209560185183</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131">
@@ -2956,16 +2960,16 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B132" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C132" s="2">
-        <v>45919.031469907408</v>
+        <v>45915.572175925925</v>
       </c>
       <c r="D132" s="2">
-        <v>45920.003437500003</v>
+        <v>45916.543171296296</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132">
@@ -2974,16 +2978,16 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="C133" s="2">
-        <v>45915.55263888889</v>
+        <v>45913.701620370368</v>
       </c>
       <c r="D133" s="2">
-        <v>45916.542962962965</v>
+        <v>45914.694907407407</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133">
@@ -2992,16 +2996,16 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B134" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C134" s="2">
-        <v>45914.043333333335</v>
+        <v>45915.220127314817</v>
       </c>
       <c r="D134" s="2">
-        <v>45915.064780092594</v>
+        <v>45916.216979166667</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134">
@@ -3010,16 +3014,16 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C135" s="2">
-        <v>45915.540833333333</v>
+        <v>45910.041087962964</v>
       </c>
       <c r="D135" s="2">
-        <v>45916.513043981482</v>
+        <v>45911.026550925926</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135">
@@ -3028,16 +3032,16 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B136" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C136" s="2">
-        <v>45914.019074074073</v>
+        <v>45919.033101851855</v>
       </c>
       <c r="D136" s="2">
-        <v>45915.000347222223</v>
+        <v>45920.037638888891</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136">
@@ -3046,16 +3050,16 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B137" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C137" s="2">
-        <v>45917.562847222223</v>
+        <v>45913.029675925929</v>
       </c>
       <c r="D137" s="2">
-        <v>45918.543981481482</v>
+        <v>45914.000960648147</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137">
@@ -3064,16 +3068,16 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B138" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C138" s="2">
-        <v>45910.510555555556</v>
+        <v>45919.028819444444</v>
       </c>
       <c r="D138" s="2">
-        <v>45911.524016203701</v>
+        <v>45920.000590277778</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138">
@@ -3082,16 +3086,16 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B139" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C139" s="2">
-        <v>45912.242094907408</v>
+        <v>45918.039143518516</v>
       </c>
       <c r="D139" s="2">
-        <v>45913.231030092589</v>
+        <v>45919.000752314816</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139">
@@ -3100,16 +3104,16 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B140" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C140" s="2">
-        <v>45913.530856481484</v>
+        <v>45916.019108796296</v>
       </c>
       <c r="D140" s="2">
-        <v>45914.507928240739</v>
+        <v>45917.00277777778</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140">
@@ -3118,37 +3122,163 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B141" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C141" s="2">
-        <v>45919.362210648149</v>
-      </c>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45910.02920138889</v>
+      </c>
+      <c r="D141" s="2">
+        <v>45911.005185185182</v>
+      </c>
+      <c r="E141" s="2"/>
       <c r="F141">
         <v>24</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B142" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C142" s="2">
-        <v>45919.351388888892</v>
-      </c>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2">
-        <v>45920.341481481482</v>
-      </c>
+        <v>45911.034571759257</v>
+      </c>
+      <c r="D142" s="2">
+        <v>45912.001400462963</v>
+      </c>
+      <c r="E142" s="2"/>
       <c r="F142">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A143" t="s">
+        <v>8</v>
+      </c>
+      <c r="B143" t="s">
+        <v>30</v>
+      </c>
+      <c r="C143" s="2">
+        <v>45914.0625</v>
+      </c>
+      <c r="D143" s="2">
+        <v>45915.059525462966</v>
+      </c>
+      <c r="E143" s="2"/>
+      <c r="F143">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A144" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" s="2">
+        <v>45919.277962962966</v>
+      </c>
+      <c r="D144" s="2">
+        <v>45920.264999999999</v>
+      </c>
+      <c r="E144" s="2"/>
+      <c r="F144">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A145" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" t="s">
+        <v>13</v>
+      </c>
+      <c r="C145" s="2">
+        <v>45911.556932870371</v>
+      </c>
+      <c r="D145" s="2">
+        <v>45912.543055555558</v>
+      </c>
+      <c r="E145" s="2"/>
+      <c r="F145">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A146" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" s="2">
+        <v>45916.579988425925</v>
+      </c>
+      <c r="D146" s="2">
+        <v>45917.561284722222</v>
+      </c>
+      <c r="E146" s="2"/>
+      <c r="F146">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A147" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147" t="s">
+        <v>49</v>
+      </c>
+      <c r="C147" s="2">
+        <v>45912.03328703704</v>
+      </c>
+      <c r="D147" s="2">
+        <v>45913.003379629627</v>
+      </c>
+      <c r="E147" s="2"/>
+      <c r="F147">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A148" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" t="s">
+        <v>45</v>
+      </c>
+      <c r="C148" s="2">
+        <v>45913.032546296294</v>
+      </c>
+      <c r="D148" s="2">
+        <v>45914.002326388887</v>
+      </c>
+      <c r="E148" s="2"/>
+      <c r="F148">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A149" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" t="s">
+        <v>36</v>
+      </c>
+      <c r="C149" s="2">
+        <v>45919.031469907408</v>
+      </c>
+      <c r="D149" s="2">
+        <v>45920.003437500003</v>
+      </c>
+      <c r="E149" s="2"/>
+      <c r="F149">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-21  8:49:10.94
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="73">
   <si>
     <t>电站名称</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>308号直流</t>
+  </si>
+  <si>
+    <t>805号直流</t>
+  </si>
+  <si>
+    <t>202号直流</t>
   </si>
 </sst>
 </file>
@@ -590,13 +596,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F149"/>
+  <dimension ref="A1:F160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31.375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="42.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -630,10 +642,10 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>45920.649699074071</v>
+        <v>45921.339629629627</v>
       </c>
       <c r="F2">
-        <v>123</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -648,10 +660,10 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
-        <v>45920.649699074071</v>
+        <v>45921.339629629627</v>
       </c>
       <c r="F3">
-        <v>105</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -666,28 +678,28 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>45920.649699074071</v>
+        <v>45921.339629629627</v>
       </c>
       <c r="F4">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
-        <v>45911.52857638889</v>
-      </c>
-      <c r="D5" s="2">
-        <v>45915.503275462965</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>45917.258240740739</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F5">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -695,33 +707,33 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2">
-        <v>45913.650914351849</v>
+        <v>45911.52857638889</v>
       </c>
       <c r="D6" s="2">
-        <v>45917.025937500002</v>
+        <v>45915.503275462965</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2">
-        <v>45917.258240740739</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>45920.649699074071</v>
-      </c>
+        <v>45913.650914351849</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45917.025937500002</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7">
         <v>81</v>
       </c>
@@ -785,13 +797,13 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2">
-        <v>45910.540219907409</v>
+        <v>45912.328969907408</v>
       </c>
       <c r="D11" s="2">
-        <v>45913.224270833336</v>
+        <v>45915.001701388886</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11">
@@ -803,13 +815,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2">
-        <v>45912.328969907408</v>
+        <v>45910.540219907409</v>
       </c>
       <c r="D12" s="2">
-        <v>45915.001701388886</v>
+        <v>45913.224270833336</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12">
@@ -854,16 +866,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2">
-        <v>45913.006967592592</v>
+        <v>45918.557500000003</v>
       </c>
       <c r="D15" s="2">
-        <v>45915.473703703705</v>
+        <v>45921.013229166667</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15">
@@ -872,38 +884,38 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2">
-        <v>45916.041956018518</v>
+        <v>45913.006967592592</v>
       </c>
       <c r="D16" s="2">
-        <v>45918.243055555555</v>
+        <v>45915.473703703705</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2">
-        <v>45918.557500000003</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2">
-        <v>45920.649699074071</v>
-      </c>
+        <v>45916.041956018518</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45918.243055555555</v>
+      </c>
+      <c r="E17" s="2"/>
       <c r="F17">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -929,31 +941,31 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2">
-        <v>45918.603634259256</v>
-      </c>
-      <c r="D19" s="2">
-        <v>45920.611122685186</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>45919.2965625</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F19">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2">
-        <v>45911.040381944447</v>
+        <v>45918.603634259256</v>
       </c>
       <c r="D20" s="2">
-        <v>45913.023263888892</v>
+        <v>45920.611122685186</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20">
@@ -962,34 +974,34 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2">
-        <v>45910.561724537038</v>
+        <v>45911.040381944447</v>
       </c>
       <c r="D21" s="2">
-        <v>45912.509375000001</v>
+        <v>45913.023263888892</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C22" s="2">
-        <v>45912.060983796298</v>
+        <v>45910.561724537038</v>
       </c>
       <c r="D22" s="2">
-        <v>45914.012141203704</v>
+        <v>45912.509375000001</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22">
@@ -998,16 +1010,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2">
-        <v>45915.583414351851</v>
+        <v>45912.060983796298</v>
       </c>
       <c r="D23" s="2">
-        <v>45917.582627314812</v>
+        <v>45914.012141203704</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23">
@@ -1034,20 +1046,20 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C25" s="2">
-        <v>45914.560046296298</v>
+        <v>45915.583414351851</v>
       </c>
       <c r="D25" s="2">
-        <v>45916.478472222225</v>
+        <v>45917.582627314812</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -1055,31 +1067,31 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C26" s="2">
-        <v>45917.219965277778</v>
+        <v>45914.560046296298</v>
       </c>
       <c r="D26" s="2">
-        <v>45919.087418981479</v>
+        <v>45916.478472222225</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2">
-        <v>45911.646747685183</v>
+        <v>45917.219965277778</v>
       </c>
       <c r="D27" s="2">
-        <v>45913.523923611108</v>
+        <v>45919.087418981479</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27">
@@ -1091,13 +1103,13 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C28" s="2">
-        <v>45911.562384259261</v>
+        <v>45911.646747685183</v>
       </c>
       <c r="D28" s="2">
-        <v>45913.435532407406</v>
+        <v>45913.523923611108</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28">
@@ -1106,16 +1118,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C29" s="2">
-        <v>45917.638888888891</v>
+        <v>45911.562384259261</v>
       </c>
       <c r="D29" s="2">
-        <v>45919.518240740741</v>
+        <v>45913.435532407406</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29">
@@ -1124,20 +1136,20 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2">
-        <v>45918.238622685189</v>
+        <v>45917.638888888891</v>
       </c>
       <c r="D30" s="2">
-        <v>45920.002534722225</v>
+        <v>45919.518240740741</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -1145,31 +1157,31 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2">
-        <v>45915.231793981482</v>
+        <v>45919.051585648151</v>
       </c>
       <c r="D31" s="2">
-        <v>45917.019432870373</v>
+        <v>45920.878449074073</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C32" s="2">
-        <v>45917.200092592589</v>
+        <v>45918.238622685189</v>
       </c>
       <c r="D32" s="2">
-        <v>45918.990624999999</v>
+        <v>45920.002534722225</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32">
@@ -1178,20 +1190,20 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C33" s="2">
-        <v>45913.76421296296</v>
+        <v>45915.231793981482</v>
       </c>
       <c r="D33" s="2">
-        <v>45915.539942129632</v>
+        <v>45917.019432870373</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
@@ -1199,71 +1211,71 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C34" s="2">
-        <v>45913.23265046296</v>
+        <v>45917.200092592589</v>
       </c>
       <c r="D34" s="2">
-        <v>45914.981087962966</v>
+        <v>45918.990624999999</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C35" s="2">
-        <v>45914.040277777778</v>
+        <v>45913.76421296296</v>
       </c>
       <c r="D35" s="2">
-        <v>45915.733287037037</v>
+        <v>45915.539942129632</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="C36" s="2">
-        <v>45918.02584490741</v>
-      </c>
-      <c r="D36" s="2">
-        <v>45919.731539351851</v>
-      </c>
-      <c r="E36" s="2"/>
+        <v>45919.589224537034</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F36">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C37" s="2">
-        <v>45918.673472222225</v>
+        <v>45913.23265046296</v>
       </c>
       <c r="D37" s="2">
-        <v>45920.394062500003</v>
+        <v>45914.981087962966</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -1271,17 +1283,17 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C38" s="2">
-        <v>45911.531018518515</v>
+        <v>45918.02584490741</v>
       </c>
       <c r="D38" s="2">
-        <v>45913.206875000003</v>
+        <v>45919.731539351851</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -1289,35 +1301,35 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C39" s="2">
-        <v>45915.111643518518</v>
+        <v>45914.040277777778</v>
       </c>
       <c r="D39" s="2">
-        <v>45916.694467592592</v>
+        <v>45915.733287037037</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C40" s="2">
-        <v>45918.715682870374</v>
+        <v>45918.673472222225</v>
       </c>
       <c r="D40" s="2">
-        <v>45920.332812499997</v>
+        <v>45920.394062500003</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -1325,35 +1337,35 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C41" s="2">
-        <v>45919.051585648151</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2">
-        <v>45920.649699074071</v>
-      </c>
+        <v>45911.531018518515</v>
+      </c>
+      <c r="D41" s="2">
+        <v>45913.206875000003</v>
+      </c>
+      <c r="E41" s="2"/>
       <c r="F41">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C42" s="2">
-        <v>45914.486261574071</v>
+        <v>45919.528935185182</v>
       </c>
       <c r="D42" s="2">
-        <v>45916.002962962964</v>
+        <v>45921.204571759263</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
@@ -1361,35 +1373,35 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C43" s="2">
-        <v>45918.526932870373</v>
+        <v>45919.638368055559</v>
       </c>
       <c r="D43" s="2">
-        <v>45920.000578703701</v>
+        <v>45921.272141203706</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C44" s="2">
-        <v>45918.539907407408</v>
+        <v>45915.111643518518</v>
       </c>
       <c r="D44" s="2">
-        <v>45920.001921296294</v>
+        <v>45916.694467592592</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
@@ -1397,17 +1409,17 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C45" s="2">
-        <v>45910.534502314818</v>
+        <v>45918.715682870374</v>
       </c>
       <c r="D45" s="2">
-        <v>45912.012048611112</v>
+        <v>45920.332812499997</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
@@ -1418,28 +1430,28 @@
         <v>35</v>
       </c>
       <c r="C46" s="2">
-        <v>45916.051249999997</v>
+        <v>45914.486261574071</v>
       </c>
       <c r="D46" s="2">
-        <v>45917.567256944443</v>
+        <v>45916.002962962964</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C47" s="2">
-        <v>45915.061967592592</v>
+        <v>45918.539907407408</v>
       </c>
       <c r="D47" s="2">
-        <v>45916.546516203707</v>
+        <v>45920.001921296294</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47">
@@ -1448,16 +1460,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C48" s="2">
-        <v>45915.025833333333</v>
+        <v>45918.526932870373</v>
       </c>
       <c r="D48" s="2">
-        <v>45916.511203703703</v>
+        <v>45920.000578703701</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48">
@@ -1466,20 +1478,20 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C49" s="2">
-        <v>45918.54587962963</v>
+        <v>45919.605023148149</v>
       </c>
       <c r="D49" s="2">
-        <v>45920.000509259262</v>
+        <v>45921.08798611111</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -1487,17 +1499,17 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C50" s="2">
-        <v>45913.717233796298</v>
+        <v>45910.534502314818</v>
       </c>
       <c r="D50" s="2">
-        <v>45915.203182870369</v>
+        <v>45912.012048611112</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
@@ -1505,35 +1517,35 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C51" s="2">
-        <v>45913.566805555558</v>
+        <v>45916.051249999997</v>
       </c>
       <c r="D51" s="2">
-        <v>45915.004942129628</v>
+        <v>45917.567256944443</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C52" s="2">
-        <v>45917.128229166665</v>
+        <v>45915.025833333333</v>
       </c>
       <c r="D52" s="2">
-        <v>45918.609236111108</v>
+        <v>45916.511203703703</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
@@ -1541,35 +1553,35 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C53" s="2">
-        <v>45912.567314814813</v>
+        <v>45915.061967592592</v>
       </c>
       <c r="D53" s="2">
-        <v>45914.04074074074</v>
+        <v>45916.546516203707</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B54" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C54" s="2">
-        <v>45914.050219907411</v>
+        <v>45913.566805555558</v>
       </c>
       <c r="D54" s="2">
-        <v>45915.466817129629</v>
+        <v>45915.004942129628</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -1577,17 +1589,17 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="C55" s="2">
-        <v>45915.541979166665</v>
+        <v>45919.726388888892</v>
       </c>
       <c r="D55" s="2">
-        <v>45916.988449074073</v>
+        <v>45921.203738425924</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -1595,17 +1607,17 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C56" s="2">
-        <v>45916.059074074074</v>
+        <v>45913.717233796298</v>
       </c>
       <c r="D56" s="2">
-        <v>45917.468865740739</v>
+        <v>45915.203182870369</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
@@ -1613,17 +1625,17 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C57" s="2">
-        <v>45916.623356481483</v>
+        <v>45918.54587962963</v>
       </c>
       <c r="D57" s="2">
-        <v>45918.0237037037</v>
+        <v>45920.000509259262</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
@@ -1631,53 +1643,53 @@
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C58" s="2">
-        <v>45917.589189814818</v>
+        <v>45917.128229166665</v>
       </c>
       <c r="D58" s="2">
-        <v>45919.000393518516</v>
+        <v>45918.609236111108</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
         <v>13</v>
       </c>
       <c r="C59" s="2">
-        <v>45912.627604166664</v>
+        <v>45912.567314814813</v>
       </c>
       <c r="D59" s="2">
-        <v>45914.005208333336</v>
+        <v>45914.04074074074</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C60" s="2">
-        <v>45910.054398148146</v>
+        <v>45914.050219907411</v>
       </c>
       <c r="D60" s="2">
-        <v>45911.384293981479</v>
+        <v>45915.466817129629</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
@@ -1685,17 +1697,17 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C61" s="2">
-        <v>45919.2965625</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2">
-        <v>45920.649699074071</v>
-      </c>
+        <v>45916.059074074074</v>
+      </c>
+      <c r="D61" s="2">
+        <v>45917.468865740739</v>
+      </c>
+      <c r="E61" s="2"/>
       <c r="F61">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
@@ -1703,17 +1715,17 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C62" s="2">
-        <v>45910.247546296298</v>
+        <v>45915.541979166665</v>
       </c>
       <c r="D62" s="2">
-        <v>45911.529826388891</v>
+        <v>45916.988449074073</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
@@ -1721,17 +1733,17 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C63" s="2">
-        <v>45915.259062500001</v>
+        <v>45916.623356481483</v>
       </c>
       <c r="D63" s="2">
-        <v>45916.545428240737</v>
+        <v>45918.0237037037</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
@@ -1739,53 +1751,53 @@
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C64" s="2">
-        <v>45917.051562499997</v>
+        <v>45917.589189814818</v>
       </c>
       <c r="D64" s="2">
-        <v>45918.348865740743</v>
+        <v>45919.000393518516</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C65" s="2">
-        <v>45916.531759259262</v>
+        <v>45912.627604166664</v>
       </c>
       <c r="D65" s="2">
-        <v>45917.797986111109</v>
+        <v>45914.005208333336</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C66" s="2">
-        <v>45918.712372685186</v>
+        <v>45910.054398148146</v>
       </c>
       <c r="D66" s="2">
-        <v>45920.004004629627</v>
+        <v>45911.384293981479</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
@@ -1793,17 +1805,17 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C67" s="2">
-        <v>45919.267326388886</v>
-      </c>
-      <c r="D67" s="2">
-        <v>45920.507592592592</v>
-      </c>
-      <c r="E67" s="2"/>
+        <v>45920.072627314818</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F67">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
@@ -1811,17 +1823,17 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C68" s="2">
-        <v>45918.264537037037</v>
+        <v>45915.259062500001</v>
       </c>
       <c r="D68" s="2">
-        <v>45919.504305555558</v>
+        <v>45916.545428240737</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
@@ -1829,17 +1841,17 @@
         <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="C69" s="2">
-        <v>45917.038738425923</v>
+        <v>45916.531759259262</v>
       </c>
       <c r="D69" s="2">
-        <v>45918.261030092595</v>
+        <v>45917.797986111109</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
@@ -1847,107 +1859,107 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C70" s="2">
-        <v>45918.257824074077</v>
+        <v>45910.247546296298</v>
       </c>
       <c r="D70" s="2">
-        <v>45919.535219907404</v>
+        <v>45911.529826388891</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C71" s="2">
-        <v>45914.304675925923</v>
+        <v>45917.051562499997</v>
       </c>
       <c r="D71" s="2">
-        <v>45915.505648148152</v>
+        <v>45918.348865740743</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C72" s="2">
-        <v>45916.350173611114</v>
-      </c>
-      <c r="D72" s="2">
-        <v>45917.544189814813</v>
-      </c>
-      <c r="E72" s="2"/>
+        <v>45920.057673611111</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F72">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C73" s="2">
-        <v>45918.558819444443</v>
-      </c>
-      <c r="D73" s="2">
-        <v>45919.759699074071</v>
-      </c>
-      <c r="E73" s="2"/>
+        <v>45920.046643518515</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F73">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C74" s="2">
-        <v>45915.250428240739</v>
+        <v>45918.712372685186</v>
       </c>
       <c r="D74" s="2">
-        <v>45916.492291666669</v>
+        <v>45920.004004629627</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C75" s="2">
-        <v>45913.050844907404</v>
+        <v>45919.267326388886</v>
       </c>
       <c r="D75" s="2">
-        <v>45914.284895833334</v>
+        <v>45920.507592592592</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
@@ -1955,53 +1967,53 @@
         <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C76" s="2">
-        <v>45910.067824074074</v>
+        <v>45918.264537037037</v>
       </c>
       <c r="D76" s="2">
-        <v>45911.284560185188</v>
+        <v>45919.504305555558</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C77" s="2">
-        <v>45914.064189814817</v>
+        <v>45917.038738425923</v>
       </c>
       <c r="D77" s="2">
-        <v>45915.274594907409</v>
+        <v>45918.261030092595</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C78" s="2">
-        <v>45914.060752314814</v>
+        <v>45918.257824074077</v>
       </c>
       <c r="D78" s="2">
-        <v>45915.225474537037</v>
+        <v>45919.535219907404</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
@@ -2009,179 +2021,179 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C79" s="2">
-        <v>45910.356319444443</v>
-      </c>
-      <c r="D79" s="2">
-        <v>45911.500925925924</v>
-      </c>
-      <c r="E79" s="2"/>
+        <v>45920.118576388886</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F79">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C80" s="2">
-        <v>45917.046249999999</v>
+        <v>45918.558819444443</v>
       </c>
       <c r="D80" s="2">
-        <v>45918.227696759262</v>
+        <v>45919.759699074071</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B81" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C81" s="2">
-        <v>45914.011388888888</v>
+        <v>45914.304675925923</v>
       </c>
       <c r="D81" s="2">
-        <v>45915.187569444446</v>
+        <v>45915.505648148152</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B82" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C82" s="2">
-        <v>45915.035682870373</v>
+        <v>45916.350173611114</v>
       </c>
       <c r="D82" s="2">
-        <v>45916.204282407409</v>
+        <v>45917.544189814813</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C83" s="2">
-        <v>45919.064259259256</v>
+        <v>45915.250428240739</v>
       </c>
       <c r="D83" s="2">
-        <v>45920.216261574074</v>
+        <v>45916.492291666669</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B84" t="s">
         <v>44</v>
       </c>
       <c r="C84" s="2">
-        <v>45917.862303240741</v>
+        <v>45913.050844907404</v>
       </c>
       <c r="D84" s="2">
-        <v>45919.004907407405</v>
+        <v>45914.284895833334</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B85" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C85" s="2">
-        <v>45919.362210648149</v>
+        <v>45910.067824074074</v>
       </c>
       <c r="D85" s="2">
-        <v>45920.481516203705</v>
+        <v>45911.284560185188</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C86" s="2">
-        <v>45913.042430555557</v>
+        <v>45920.023310185185</v>
       </c>
       <c r="D86" s="2">
-        <v>45914.200810185182</v>
+        <v>45921.21974537037</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C87" s="2">
-        <v>45914.045497685183</v>
+        <v>45914.064189814817</v>
       </c>
       <c r="D87" s="2">
-        <v>45915.202696759261</v>
+        <v>45915.274594907409</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="C88" s="2">
-        <v>45915.075706018521</v>
+        <v>45914.060752314814</v>
       </c>
       <c r="D88" s="2">
-        <v>45916.188900462963</v>
+        <v>45915.225474537037</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
@@ -2189,17 +2201,17 @@
         <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C89" s="2">
-        <v>45912.041076388887</v>
+        <v>45910.356319444443</v>
       </c>
       <c r="D89" s="2">
-        <v>45913.145925925928</v>
+        <v>45911.500925925924</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
@@ -2207,17 +2219,17 @@
         <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C90" s="2">
-        <v>45913.579629629632</v>
+        <v>45914.011388888888</v>
       </c>
       <c r="D90" s="2">
-        <v>45914.686932870369</v>
+        <v>45915.187569444446</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
@@ -2225,35 +2237,35 @@
         <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C91" s="2">
-        <v>45914.151493055557</v>
+        <v>45915.035682870373</v>
       </c>
       <c r="D91" s="2">
-        <v>45915.287997685184</v>
+        <v>45916.204282407409</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C92" s="2">
-        <v>45911.012094907404</v>
+        <v>45917.046249999999</v>
       </c>
       <c r="D92" s="2">
-        <v>45912.137696759259</v>
+        <v>45918.227696759262</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
@@ -2261,53 +2273,53 @@
         <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C93" s="2">
-        <v>45919.528935185182</v>
-      </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2">
-        <v>45920.649699074071</v>
-      </c>
+        <v>45917.862303240741</v>
+      </c>
+      <c r="D93" s="2">
+        <v>45919.004907407405</v>
+      </c>
+      <c r="E93" s="2"/>
       <c r="F93">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C94" s="2">
-        <v>45919.351388888892</v>
+        <v>45919.064259259256</v>
       </c>
       <c r="D94" s="2">
-        <v>45920.447187500002</v>
+        <v>45920.216261574074</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C95" s="2">
-        <v>45913.064467592594</v>
+        <v>45913.042430555557</v>
       </c>
       <c r="D95" s="2">
-        <v>45914.140983796293</v>
+        <v>45914.200810185182</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.15">
@@ -2315,211 +2327,211 @@
         <v>51</v>
       </c>
       <c r="B96" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C96" s="2">
-        <v>45911.244166666664</v>
+        <v>45919.362210648149</v>
       </c>
       <c r="D96" s="2">
-        <v>45912.265601851854</v>
+        <v>45920.481516203705</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C97" s="2">
-        <v>45911.504976851851</v>
+        <v>45912.041076388887</v>
       </c>
       <c r="D97" s="2">
-        <v>45912.543333333335</v>
+        <v>45913.145925925928</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B98" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C98" s="2">
-        <v>45915.525405092594</v>
+        <v>45914.151493055557</v>
       </c>
       <c r="D98" s="2">
-        <v>45916.54210648148</v>
+        <v>45915.287997685184</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B99" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C99" s="2">
-        <v>45919.499756944446</v>
+        <v>45913.579629629632</v>
       </c>
       <c r="D99" s="2">
-        <v>45920.505324074074</v>
+        <v>45914.686932870369</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C100" s="2">
-        <v>45919.605023148149</v>
-      </c>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2">
-        <v>45920.649699074071</v>
-      </c>
+        <v>45915.075706018521</v>
+      </c>
+      <c r="D100" s="2">
+        <v>45916.188900462963</v>
+      </c>
+      <c r="E100" s="2"/>
       <c r="F100">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B101" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="C101" s="2">
-        <v>45919.589224537034</v>
-      </c>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2">
-        <v>45920.649699074071</v>
-      </c>
+        <v>45914.045497685183</v>
+      </c>
+      <c r="D101" s="2">
+        <v>45915.202696759261</v>
+      </c>
+      <c r="E101" s="2"/>
       <c r="F101">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B102" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C102" s="2">
-        <v>45919.472337962965</v>
-      </c>
-      <c r="D102" s="2">
-        <v>45920.537222222221</v>
-      </c>
-      <c r="E102" s="2"/>
+        <v>45920.226956018516</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F102">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C103" s="2">
-        <v>45913.021006944444</v>
+        <v>45911.012094907404</v>
       </c>
       <c r="D103" s="2">
-        <v>45914.078969907408</v>
+        <v>45912.137696759259</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="C104" s="2">
-        <v>45915.475578703707</v>
-      </c>
-      <c r="D104" s="2">
-        <v>45916.538958333331</v>
-      </c>
-      <c r="E104" s="2"/>
+        <v>45920.218981481485</v>
+      </c>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2">
+        <v>45921.339629629627</v>
+      </c>
       <c r="F104">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B105" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C105" s="2">
-        <v>45911.994386574072</v>
+        <v>45919.351388888892</v>
       </c>
       <c r="D105" s="2">
-        <v>45913.008622685185</v>
+        <v>45920.447187500002</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C106" s="2">
-        <v>45918.199444444443</v>
+        <v>45913.064467592594</v>
       </c>
       <c r="D106" s="2">
-        <v>45919.209988425922</v>
+        <v>45914.140983796293</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C107" s="2">
-        <v>45912.043020833335</v>
+        <v>45913.021006944444</v>
       </c>
       <c r="D107" s="2">
-        <v>45913.113923611112</v>
+        <v>45914.078969907408</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107">
@@ -2528,16 +2540,16 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C108" s="2">
-        <v>45911.684641203705</v>
+        <v>45920.069849537038</v>
       </c>
       <c r="D108" s="2">
-        <v>45912.726527777777</v>
+        <v>45921.099664351852</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108">
@@ -2546,16 +2558,16 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C109" s="2">
-        <v>45919.067708333336</v>
+        <v>45919.472337962965</v>
       </c>
       <c r="D109" s="2">
-        <v>45920.088587962964</v>
+        <v>45920.537222222221</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109">
@@ -2564,16 +2576,16 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B110" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C110" s="2">
-        <v>45917.244652777779</v>
+        <v>45919.499756944446</v>
       </c>
       <c r="D110" s="2">
-        <v>45918.285451388889</v>
+        <v>45920.505324074074</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110">
@@ -2582,16 +2594,16 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B111" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C111" s="2">
-        <v>45915.055277777778</v>
+        <v>45915.525405092594</v>
       </c>
       <c r="D111" s="2">
-        <v>45916.095949074072</v>
+        <v>45916.54210648148</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111">
@@ -2600,16 +2612,16 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B112" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="C112" s="2">
-        <v>45915.483831018515</v>
+        <v>45911.244166666664</v>
       </c>
       <c r="D112" s="2">
-        <v>45916.511701388888</v>
+        <v>45912.265601851854</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112">
@@ -2618,16 +2630,16 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B113" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C113" s="2">
-        <v>45914.036979166667</v>
+        <v>45911.504976851851</v>
       </c>
       <c r="D113" s="2">
-        <v>45915.079004629632</v>
+        <v>45912.543333333335</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113">
@@ -2636,16 +2648,16 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C114" s="2">
-        <v>45919.036516203705</v>
+        <v>45911.994386574072</v>
       </c>
       <c r="D114" s="2">
-        <v>45920.041701388887</v>
+        <v>45913.008622685185</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114">
@@ -2654,16 +2666,16 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C115" s="2">
-        <v>45910.196134259262</v>
+        <v>45918.199444444443</v>
       </c>
       <c r="D115" s="2">
-        <v>45911.248784722222</v>
+        <v>45919.209988425922</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115">
@@ -2672,196 +2684,196 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C116" s="2">
-        <v>45919.566770833335</v>
+        <v>45915.475578703707</v>
       </c>
       <c r="D116" s="2">
-        <v>45920.544930555552</v>
+        <v>45916.538958333331</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C117" s="2">
-        <v>45912.242094907408</v>
+        <v>45915.055277777778</v>
       </c>
       <c r="D117" s="2">
-        <v>45913.231030092589</v>
+        <v>45916.095949074072</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B118" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C118" s="2">
-        <v>45913.530856481484</v>
+        <v>45917.244652777779</v>
       </c>
       <c r="D118" s="2">
-        <v>45914.507928240739</v>
+        <v>45918.285451388889</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C119" s="2">
-        <v>45914.043333333335</v>
+        <v>45911.684641203705</v>
       </c>
       <c r="D119" s="2">
-        <v>45915.064780092594</v>
+        <v>45912.726527777777</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C120" s="2">
-        <v>45914.019074074073</v>
+        <v>45912.043020833335</v>
       </c>
       <c r="D120" s="2">
-        <v>45915.000347222223</v>
+        <v>45913.113923611112</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B121" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C121" s="2">
-        <v>45917.562847222223</v>
+        <v>45919.067708333336</v>
       </c>
       <c r="D121" s="2">
-        <v>45918.543981481482</v>
+        <v>45920.088587962964</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C122" s="2">
-        <v>45915.540833333333</v>
+        <v>45915.483831018515</v>
       </c>
       <c r="D122" s="2">
-        <v>45916.513043981482</v>
+        <v>45916.511701388888</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B123" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C123" s="2">
-        <v>45915.55263888889</v>
+        <v>45910.196134259262</v>
       </c>
       <c r="D123" s="2">
-        <v>45916.542962962965</v>
+        <v>45911.248784722222</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B124" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C124" s="2">
-        <v>45919.638368055559</v>
-      </c>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2">
-        <v>45920.649699074071</v>
-      </c>
+        <v>45914.036979166667</v>
+      </c>
+      <c r="D124" s="2">
+        <v>45915.079004629632</v>
+      </c>
+      <c r="E124" s="2"/>
       <c r="F124">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B125" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C125" s="2">
-        <v>45910.510555555556</v>
+        <v>45919.036516203705</v>
       </c>
       <c r="D125" s="2">
-        <v>45911.524016203701</v>
+        <v>45920.041701388887</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B126" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C126" s="2">
-        <v>45913.030231481483</v>
+        <v>45915.55263888889</v>
       </c>
       <c r="D126" s="2">
-        <v>45914.003888888888</v>
+        <v>45916.542962962965</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126">
@@ -2870,16 +2882,16 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C127" s="2">
-        <v>45917.543113425927</v>
+        <v>45914.043333333335</v>
       </c>
       <c r="D127" s="2">
-        <v>45918.545127314814</v>
+        <v>45915.064780092594</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127">
@@ -2888,16 +2900,16 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C128" s="2">
-        <v>45910.584328703706</v>
+        <v>45915.540833333333</v>
       </c>
       <c r="D128" s="2">
-        <v>45911.616053240738</v>
+        <v>45916.513043981482</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128">
@@ -2906,16 +2918,16 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C129" s="2">
-        <v>45915.020277777781</v>
+        <v>45914.019074074073</v>
       </c>
       <c r="D129" s="2">
-        <v>45916.002210648148</v>
+        <v>45915.000347222223</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129">
@@ -2924,16 +2936,16 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C130" s="2">
-        <v>45918.378263888888</v>
+        <v>45917.562847222223</v>
       </c>
       <c r="D130" s="2">
-        <v>45919.401689814818</v>
+        <v>45918.543981481482</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130">
@@ -2942,16 +2954,16 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B131" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C131" s="2">
-        <v>45917.243622685186</v>
+        <v>45910.510555555556</v>
       </c>
       <c r="D131" s="2">
-        <v>45918.209560185183</v>
+        <v>45911.524016203701</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131">
@@ -2960,16 +2972,16 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B132" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="C132" s="2">
-        <v>45915.572175925925</v>
+        <v>45919.566770833335</v>
       </c>
       <c r="D132" s="2">
-        <v>45916.543171296296</v>
+        <v>45920.544930555552</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132">
@@ -2978,16 +2990,16 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B133" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C133" s="2">
-        <v>45913.701620370368</v>
+        <v>45912.242094907408</v>
       </c>
       <c r="D133" s="2">
-        <v>45914.694907407407</v>
+        <v>45913.231030092589</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133">
@@ -2996,16 +3008,16 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B134" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C134" s="2">
-        <v>45915.220127314817</v>
+        <v>45913.530856481484</v>
       </c>
       <c r="D134" s="2">
-        <v>45916.216979166667</v>
+        <v>45914.507928240739</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134">
@@ -3017,13 +3029,13 @@
         <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C135" s="2">
-        <v>45910.041087962964</v>
+        <v>45920.249756944446</v>
       </c>
       <c r="D135" s="2">
-        <v>45911.026550925926</v>
+        <v>45921.209710648145</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135">
@@ -3035,13 +3047,13 @@
         <v>6</v>
       </c>
       <c r="B136" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C136" s="2">
-        <v>45919.033101851855</v>
+        <v>45920.033518518518</v>
       </c>
       <c r="D136" s="2">
-        <v>45920.037638888891</v>
+        <v>45921.002650462964</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136">
@@ -3053,13 +3065,13 @@
         <v>6</v>
       </c>
       <c r="B137" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C137" s="2">
-        <v>45913.029675925929</v>
+        <v>45913.030231481483</v>
       </c>
       <c r="D137" s="2">
-        <v>45914.000960648147</v>
+        <v>45914.003888888888</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137">
@@ -3071,13 +3083,13 @@
         <v>6</v>
       </c>
       <c r="B138" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C138" s="2">
-        <v>45919.028819444444</v>
+        <v>45915.220127314817</v>
       </c>
       <c r="D138" s="2">
-        <v>45920.000590277778</v>
+        <v>45916.216979166667</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138">
@@ -3089,13 +3101,13 @@
         <v>6</v>
       </c>
       <c r="B139" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C139" s="2">
-        <v>45918.039143518516</v>
+        <v>45918.378263888888</v>
       </c>
       <c r="D139" s="2">
-        <v>45919.000752314816</v>
+        <v>45919.401689814818</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139">
@@ -3104,16 +3116,16 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B140" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C140" s="2">
-        <v>45916.019108796296</v>
+        <v>45917.543113425927</v>
       </c>
       <c r="D140" s="2">
-        <v>45917.00277777778</v>
+        <v>45918.545127314814</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140">
@@ -3122,16 +3134,16 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B141" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C141" s="2">
-        <v>45910.02920138889</v>
+        <v>45918.039143518516</v>
       </c>
       <c r="D141" s="2">
-        <v>45911.005185185182</v>
+        <v>45919.000752314816</v>
       </c>
       <c r="E141" s="2"/>
       <c r="F141">
@@ -3140,16 +3152,16 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B142" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C142" s="2">
-        <v>45911.034571759257</v>
+        <v>45915.020277777781</v>
       </c>
       <c r="D142" s="2">
-        <v>45912.001400462963</v>
+        <v>45916.002210648148</v>
       </c>
       <c r="E142" s="2"/>
       <c r="F142">
@@ -3158,16 +3170,16 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B143" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C143" s="2">
-        <v>45914.0625</v>
+        <v>45917.243622685186</v>
       </c>
       <c r="D143" s="2">
-        <v>45915.059525462966</v>
+        <v>45918.209560185183</v>
       </c>
       <c r="E143" s="2"/>
       <c r="F143">
@@ -3176,16 +3188,16 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B144" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C144" s="2">
-        <v>45919.277962962966</v>
+        <v>45910.584328703706</v>
       </c>
       <c r="D144" s="2">
-        <v>45920.264999999999</v>
+        <v>45911.616053240738</v>
       </c>
       <c r="E144" s="2"/>
       <c r="F144">
@@ -3194,16 +3206,16 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B145" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C145" s="2">
-        <v>45911.556932870371</v>
+        <v>45915.572175925925</v>
       </c>
       <c r="D145" s="2">
-        <v>45912.543055555558</v>
+        <v>45916.543171296296</v>
       </c>
       <c r="E145" s="2"/>
       <c r="F145">
@@ -3212,16 +3224,16 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C146" s="2">
-        <v>45916.579988425925</v>
+        <v>45913.701620370368</v>
       </c>
       <c r="D146" s="2">
-        <v>45917.561284722222</v>
+        <v>45914.694907407407</v>
       </c>
       <c r="E146" s="2"/>
       <c r="F146">
@@ -3230,16 +3242,16 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B147" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C147" s="2">
-        <v>45912.03328703704</v>
+        <v>45910.041087962964</v>
       </c>
       <c r="D147" s="2">
-        <v>45913.003379629627</v>
+        <v>45911.026550925926</v>
       </c>
       <c r="E147" s="2"/>
       <c r="F147">
@@ -3248,16 +3260,16 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B148" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C148" s="2">
-        <v>45913.032546296294</v>
+        <v>45919.033101851855</v>
       </c>
       <c r="D148" s="2">
-        <v>45914.002326388887</v>
+        <v>45920.037638888891</v>
       </c>
       <c r="E148" s="2"/>
       <c r="F148">
@@ -3266,19 +3278,217 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B149" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C149" s="2">
-        <v>45919.031469907408</v>
+        <v>45913.029675925929</v>
       </c>
       <c r="D149" s="2">
-        <v>45920.003437500003</v>
+        <v>45914.000960648147</v>
       </c>
       <c r="E149" s="2"/>
       <c r="F149">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A150" t="s">
+        <v>6</v>
+      </c>
+      <c r="B150" t="s">
+        <v>35</v>
+      </c>
+      <c r="C150" s="2">
+        <v>45919.028819444444</v>
+      </c>
+      <c r="D150" s="2">
+        <v>45920.000590277778</v>
+      </c>
+      <c r="E150" s="2"/>
+      <c r="F150">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A151" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" t="s">
+        <v>45</v>
+      </c>
+      <c r="C151" s="2">
+        <v>45913.032546296294</v>
+      </c>
+      <c r="D151" s="2">
+        <v>45914.002326388887</v>
+      </c>
+      <c r="E151" s="2"/>
+      <c r="F151">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A152" t="s">
+        <v>8</v>
+      </c>
+      <c r="B152" t="s">
+        <v>49</v>
+      </c>
+      <c r="C152" s="2">
+        <v>45912.03328703704</v>
+      </c>
+      <c r="D152" s="2">
+        <v>45913.003379629627</v>
+      </c>
+      <c r="E152" s="2"/>
+      <c r="F152">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A153" t="s">
+        <v>8</v>
+      </c>
+      <c r="B153" t="s">
+        <v>36</v>
+      </c>
+      <c r="C153" s="2">
+        <v>45919.031469907408</v>
+      </c>
+      <c r="D153" s="2">
+        <v>45920.003437500003</v>
+      </c>
+      <c r="E153" s="2"/>
+      <c r="F153">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A154" t="s">
+        <v>8</v>
+      </c>
+      <c r="B154" t="s">
+        <v>13</v>
+      </c>
+      <c r="C154" s="2">
+        <v>45911.556932870371</v>
+      </c>
+      <c r="D154" s="2">
+        <v>45912.543055555558</v>
+      </c>
+      <c r="E154" s="2"/>
+      <c r="F154">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A155" t="s">
+        <v>8</v>
+      </c>
+      <c r="B155" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155" s="2">
+        <v>45916.019108796296</v>
+      </c>
+      <c r="D155" s="2">
+        <v>45917.00277777778</v>
+      </c>
+      <c r="E155" s="2"/>
+      <c r="F155">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A156" t="s">
+        <v>8</v>
+      </c>
+      <c r="B156" t="s">
+        <v>30</v>
+      </c>
+      <c r="C156" s="2">
+        <v>45910.02920138889</v>
+      </c>
+      <c r="D156" s="2">
+        <v>45911.005185185182</v>
+      </c>
+      <c r="E156" s="2"/>
+      <c r="F156">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A157" t="s">
+        <v>8</v>
+      </c>
+      <c r="B157" t="s">
+        <v>30</v>
+      </c>
+      <c r="C157" s="2">
+        <v>45911.034571759257</v>
+      </c>
+      <c r="D157" s="2">
+        <v>45912.001400462963</v>
+      </c>
+      <c r="E157" s="2"/>
+      <c r="F157">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A158" t="s">
+        <v>8</v>
+      </c>
+      <c r="B158" t="s">
+        <v>30</v>
+      </c>
+      <c r="C158" s="2">
+        <v>45914.0625</v>
+      </c>
+      <c r="D158" s="2">
+        <v>45915.059525462966</v>
+      </c>
+      <c r="E158" s="2"/>
+      <c r="F158">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A159" t="s">
+        <v>8</v>
+      </c>
+      <c r="B159" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159" s="2">
+        <v>45919.277962962966</v>
+      </c>
+      <c r="D159" s="2">
+        <v>45920.264999999999</v>
+      </c>
+      <c r="E159" s="2"/>
+      <c r="F159">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A160" t="s">
+        <v>8</v>
+      </c>
+      <c r="B160" t="s">
+        <v>5</v>
+      </c>
+      <c r="C160" s="2">
+        <v>45916.579988425925</v>
+      </c>
+      <c r="D160" s="2">
+        <v>45917.561284722222</v>
+      </c>
+      <c r="E160" s="2"/>
+      <c r="F160">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-26 12:08:43.30
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -124,9 +124,6 @@
     <t>A02号直流</t>
   </si>
   <si>
-    <t>最近一次充电结束时间</t>
-  </si>
-  <si>
     <t>截止一直未充电时间</t>
   </si>
   <si>
@@ -134,6 +131,10 @@
   </si>
   <si>
     <t>006B号直流</t>
+  </si>
+  <si>
+    <t>一次充电结束时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -143,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +164,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -199,6 +207,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -507,33 +518,33 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="24.25" defaultRowHeight="13.5"/>
   <cols>
     <col min="3" max="4" width="24.25" style="2"/>
     <col min="5" max="5" width="24.25" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -550,7 +561,7 @@
         <v>262.35166666656733</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -567,7 +578,7 @@
         <v>141.64277777768439</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -584,7 +595,7 @@
         <v>69.697777777793817</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -601,7 +612,7 @@
         <v>66.216944444342516</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -618,7 +629,7 @@
         <v>46.147777777689043</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -635,7 +646,7 @@
         <v>45.429444444424007</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -652,7 +663,7 @@
         <v>45.299999999930151</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -669,7 +680,7 @@
         <v>45.193333333299961</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -686,7 +697,7 @@
         <v>39.853888888901565</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -703,7 +714,7 @@
         <v>33.051666666695382</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -720,7 +731,7 @@
         <v>32.911111111112405</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -737,7 +748,7 @@
         <v>28.936388888920192</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -754,7 +765,7 @@
         <v>28.793333333276678</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -771,7 +782,7 @@
         <v>28.66833333321847</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -788,7 +799,7 @@
         <v>28.534166666620877</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -805,7 +816,7 @@
         <v>22.708055555471219</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -822,7 +833,7 @@
         <v>21.635277777677402</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -839,7 +850,7 @@
         <v>21.613055555499159</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -856,7 +867,7 @@
         <v>21.503055555454921</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -873,7 +884,7 @@
         <v>21.492222222208511</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -890,7 +901,7 @@
         <v>21.464444444398396</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -907,7 +918,7 @@
         <v>21.365833333285991</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -924,12 +935,12 @@
         <v>21.27972222212702</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2">
         <v>45925.550555555557</v>
@@ -941,7 +952,7 @@
         <v>21.226666666567326</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -958,7 +969,7 @@
         <v>21.13722222216893</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -975,7 +986,7 @@
         <v>20.821111111028586</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -992,7 +1003,7 @@
         <v>20.739166666637175</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1020,7 @@
         <v>19.988055555440951</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1026,7 +1037,7 @@
         <v>17.633611111028586</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1043,7 +1054,7 @@
         <v>16.527222222124692</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1060,7 +1071,7 @@
         <v>15.509444444440305</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1077,7 +1088,7 @@
         <v>15.403888888831716</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Auto commit at 2025-09-26 12:26:08.39
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -10,14 +10,14 @@
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$A$1:$E$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$A$1:$F$73</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>电站名称</t>
   </si>
@@ -133,7 +133,11 @@
     <t>006B号直流</t>
   </si>
   <si>
-    <t>一次充电结束时间</t>
+    <t>上一次充电结束时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>下一次充电开始时间</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -515,19 +519,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.25" defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="4" width="24.25" style="2"/>
-    <col min="5" max="5" width="24.25" style="6"/>
+    <col min="3" max="5" width="24.25" style="2"/>
+    <col min="6" max="6" width="24.25" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -537,14 +541,17 @@
       <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -554,14 +561,14 @@
       <c r="C2" s="2">
         <v>45915.503680555557</v>
       </c>
-      <c r="D2" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="E2" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F2" s="6">
         <v>262.35166666656733</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -571,14 +578,14 @@
       <c r="C3" s="2">
         <v>45920.533217592594</v>
       </c>
-      <c r="D3" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="E3" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F3" s="6">
         <v>141.64277777768439</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -588,14 +595,14 @@
       <c r="C4" s="2">
         <v>45923.530925925923</v>
       </c>
-      <c r="D4" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="E4" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F4" s="6">
         <v>69.697777777793817</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -605,14 +612,14 @@
       <c r="C5" s="2">
         <v>45923.67596064815</v>
       </c>
-      <c r="D5" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="E5" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F5" s="6">
         <v>66.216944444342516</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -622,14 +629,14 @@
       <c r="C6" s="2">
         <v>45924.512175925927</v>
       </c>
-      <c r="D6" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="E6" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F6" s="6">
         <v>46.147777777689043</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -639,14 +646,14 @@
       <c r="C7" s="2">
         <v>45924.54210648148</v>
       </c>
-      <c r="D7" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="E7" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F7" s="6">
         <v>45.429444444424007</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -656,14 +663,14 @@
       <c r="C8" s="2">
         <v>45924.547500000001</v>
       </c>
-      <c r="D8" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="E8" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F8" s="6">
         <v>45.299999999930151</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -673,14 +680,14 @@
       <c r="C9" s="2">
         <v>45924.551944444444</v>
       </c>
-      <c r="D9" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="E9" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F9" s="6">
         <v>45.193333333299961</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -690,14 +697,14 @@
       <c r="C10" s="2">
         <v>45924.774421296293</v>
       </c>
-      <c r="D10" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="E10" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F10" s="6">
         <v>39.853888888901565</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -707,14 +714,14 @@
       <c r="C11" s="2">
         <v>45925.057847222219</v>
       </c>
-      <c r="D11" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="E11" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F11" s="6">
         <v>33.051666666695382</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -724,14 +731,14 @@
       <c r="C12" s="2">
         <v>45925.063703703701</v>
       </c>
-      <c r="D12" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="E12" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F12" s="6">
         <v>32.911111111112405</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -741,14 +748,14 @@
       <c r="C13" s="2">
         <v>45925.229317129626</v>
       </c>
-      <c r="D13" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="E13" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F13" s="6">
         <v>28.936388888920192</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -758,14 +765,14 @@
       <c r="C14" s="2">
         <v>45925.235277777778</v>
       </c>
-      <c r="D14" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="E14" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F14" s="6">
         <v>28.793333333276678</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -775,14 +782,14 @@
       <c r="C15" s="2">
         <v>45925.240486111114</v>
       </c>
-      <c r="D15" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="E15" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F15" s="6">
         <v>28.66833333321847</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -792,14 +799,14 @@
       <c r="C16" s="2">
         <v>45925.246076388888</v>
       </c>
-      <c r="D16" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="E16" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F16" s="6">
         <v>28.534166666620877</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -809,14 +816,14 @@
       <c r="C17" s="2">
         <v>45925.48883101852</v>
       </c>
-      <c r="D17" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="E17" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F17" s="6">
         <v>22.708055555471219</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -826,14 +833,14 @@
       <c r="C18" s="2">
         <v>45925.533530092594</v>
       </c>
-      <c r="D18" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="E18" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F18" s="6">
         <v>21.635277777677402</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -843,14 +850,14 @@
       <c r="C19" s="2">
         <v>45925.534456018519</v>
       </c>
-      <c r="D19" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="E19" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F19" s="6">
         <v>21.613055555499159</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -860,14 +867,14 @@
       <c r="C20" s="2">
         <v>45925.539039351854</v>
       </c>
-      <c r="D20" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E20" s="6">
+      <c r="E20" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F20" s="6">
         <v>21.503055555454921</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -877,14 +884,14 @@
       <c r="C21" s="2">
         <v>45925.539490740739</v>
       </c>
-      <c r="D21" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E21" s="6">
+      <c r="E21" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F21" s="6">
         <v>21.492222222208511</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -894,14 +901,14 @@
       <c r="C22" s="2">
         <v>45925.540648148148</v>
       </c>
-      <c r="D22" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E22" s="6">
+      <c r="E22" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F22" s="6">
         <v>21.464444444398396</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -911,14 +918,14 @@
       <c r="C23" s="2">
         <v>45925.544756944444</v>
       </c>
-      <c r="D23" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E23" s="6">
+      <c r="E23" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F23" s="6">
         <v>21.365833333285991</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -928,14 +935,14 @@
       <c r="C24" s="2">
         <v>45925.548344907409</v>
       </c>
-      <c r="D24" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E24" s="6">
+      <c r="E24" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F24" s="6">
         <v>21.27972222212702</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -945,14 +952,14 @@
       <c r="C25" s="2">
         <v>45925.550555555557</v>
       </c>
-      <c r="D25" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E25" s="6">
+      <c r="E25" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F25" s="6">
         <v>21.226666666567326</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -962,14 +969,14 @@
       <c r="C26" s="2">
         <v>45925.554282407407</v>
       </c>
-      <c r="D26" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E26" s="6">
+      <c r="E26" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F26" s="6">
         <v>21.13722222216893</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -979,14 +986,14 @@
       <c r="C27" s="2">
         <v>45925.567453703705</v>
       </c>
-      <c r="D27" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E27" s="6">
+      <c r="E27" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F27" s="6">
         <v>20.821111111028586</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -996,14 +1003,14 @@
       <c r="C28" s="2">
         <v>45925.570868055554</v>
       </c>
-      <c r="D28" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E28" s="6">
+      <c r="E28" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F28" s="6">
         <v>20.739166666637175</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1013,14 +1020,14 @@
       <c r="C29" s="2">
         <v>45925.602164351854</v>
       </c>
-      <c r="D29" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E29" s="6">
+      <c r="E29" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F29" s="6">
         <v>19.988055555440951</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1030,14 +1037,14 @@
       <c r="C30" s="2">
         <v>45925.700266203705</v>
       </c>
-      <c r="D30" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E30" s="6">
+      <c r="E30" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F30" s="6">
         <v>17.633611111028586</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1047,14 +1054,14 @@
       <c r="C31" s="2">
         <v>45925.746365740742</v>
       </c>
-      <c r="D31" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E31" s="6">
+      <c r="E31" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F31" s="6">
         <v>16.527222222124692</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1064,14 +1071,14 @@
       <c r="C32" s="2">
         <v>45925.788773148146</v>
       </c>
-      <c r="D32" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E32" s="6">
+      <c r="E32" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F32" s="6">
         <v>15.509444444440305</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1081,14 +1088,14 @@
       <c r="C33" s="2">
         <v>45925.793171296296</v>
       </c>
-      <c r="D33" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E33" s="6">
+      <c r="E33" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F33" s="6">
         <v>15.403888888831716</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1098,10 +1105,10 @@
       <c r="C34" s="2">
         <v>45925.860277777778</v>
       </c>
-      <c r="D34" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="E34" s="6">
+      <c r="E34" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="F34" s="6">
         <v>13.793333333276678</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-09-26 12:39:00.25
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -10,14 +10,14 @@
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$A$1:$F$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$A$1:$E$73</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>电站名称</t>
   </si>
@@ -134,10 +134,6 @@
   </si>
   <si>
     <t>上一次充电结束时间</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>下一次充电开始时间</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -519,19 +515,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.25" defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="5" width="24.25" style="2"/>
-    <col min="6" max="6" width="24.25" style="6"/>
+    <col min="3" max="4" width="24.25" style="2"/>
+    <col min="5" max="5" width="24.25" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -541,17 +537,14 @@
       <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -561,14 +554,14 @@
       <c r="C2" s="2">
         <v>45915.503680555557</v>
       </c>
-      <c r="E2" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="D2" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E2" s="6">
         <v>262.35166666656733</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -578,14 +571,14 @@
       <c r="C3" s="2">
         <v>45920.533217592594</v>
       </c>
-      <c r="E3" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="D3" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E3" s="6">
         <v>141.64277777768439</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -595,14 +588,14 @@
       <c r="C4" s="2">
         <v>45923.530925925923</v>
       </c>
-      <c r="E4" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="D4" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E4" s="6">
         <v>69.697777777793817</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -612,14 +605,14 @@
       <c r="C5" s="2">
         <v>45923.67596064815</v>
       </c>
-      <c r="E5" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="D5" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E5" s="6">
         <v>66.216944444342516</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -629,14 +622,14 @@
       <c r="C6" s="2">
         <v>45924.512175925927</v>
       </c>
-      <c r="E6" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="D6" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E6" s="6">
         <v>46.147777777689043</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -646,14 +639,14 @@
       <c r="C7" s="2">
         <v>45924.54210648148</v>
       </c>
-      <c r="E7" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="D7" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E7" s="6">
         <v>45.429444444424007</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -663,14 +656,14 @@
       <c r="C8" s="2">
         <v>45924.547500000001</v>
       </c>
-      <c r="E8" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="D8" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E8" s="6">
         <v>45.299999999930151</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -680,14 +673,14 @@
       <c r="C9" s="2">
         <v>45924.551944444444</v>
       </c>
-      <c r="E9" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="D9" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E9" s="6">
         <v>45.193333333299961</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -697,14 +690,14 @@
       <c r="C10" s="2">
         <v>45924.774421296293</v>
       </c>
-      <c r="E10" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="D10" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E10" s="6">
         <v>39.853888888901565</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -714,14 +707,14 @@
       <c r="C11" s="2">
         <v>45925.057847222219</v>
       </c>
-      <c r="E11" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="D11" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E11" s="6">
         <v>33.051666666695382</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -731,14 +724,14 @@
       <c r="C12" s="2">
         <v>45925.063703703701</v>
       </c>
-      <c r="E12" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="D12" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E12" s="6">
         <v>32.911111111112405</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -748,14 +741,14 @@
       <c r="C13" s="2">
         <v>45925.229317129626</v>
       </c>
-      <c r="E13" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F13" s="6">
+      <c r="D13" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E13" s="6">
         <v>28.936388888920192</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -765,14 +758,14 @@
       <c r="C14" s="2">
         <v>45925.235277777778</v>
       </c>
-      <c r="E14" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="D14" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E14" s="6">
         <v>28.793333333276678</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -782,14 +775,14 @@
       <c r="C15" s="2">
         <v>45925.240486111114</v>
       </c>
-      <c r="E15" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="D15" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E15" s="6">
         <v>28.66833333321847</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -799,14 +792,14 @@
       <c r="C16" s="2">
         <v>45925.246076388888</v>
       </c>
-      <c r="E16" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="D16" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E16" s="6">
         <v>28.534166666620877</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -816,14 +809,14 @@
       <c r="C17" s="2">
         <v>45925.48883101852</v>
       </c>
-      <c r="E17" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F17" s="6">
+      <c r="D17" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E17" s="6">
         <v>22.708055555471219</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -833,14 +826,14 @@
       <c r="C18" s="2">
         <v>45925.533530092594</v>
       </c>
-      <c r="E18" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F18" s="6">
+      <c r="D18" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E18" s="6">
         <v>21.635277777677402</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -850,14 +843,14 @@
       <c r="C19" s="2">
         <v>45925.534456018519</v>
       </c>
-      <c r="E19" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="D19" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E19" s="6">
         <v>21.613055555499159</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -867,14 +860,14 @@
       <c r="C20" s="2">
         <v>45925.539039351854</v>
       </c>
-      <c r="E20" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F20" s="6">
+      <c r="D20" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E20" s="6">
         <v>21.503055555454921</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -884,14 +877,14 @@
       <c r="C21" s="2">
         <v>45925.539490740739</v>
       </c>
-      <c r="E21" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F21" s="6">
+      <c r="D21" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E21" s="6">
         <v>21.492222222208511</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -901,14 +894,14 @@
       <c r="C22" s="2">
         <v>45925.540648148148</v>
       </c>
-      <c r="E22" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F22" s="6">
+      <c r="D22" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E22" s="6">
         <v>21.464444444398396</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -918,14 +911,14 @@
       <c r="C23" s="2">
         <v>45925.544756944444</v>
       </c>
-      <c r="E23" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F23" s="6">
+      <c r="D23" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E23" s="6">
         <v>21.365833333285991</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -935,14 +928,14 @@
       <c r="C24" s="2">
         <v>45925.548344907409</v>
       </c>
-      <c r="E24" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F24" s="6">
+      <c r="D24" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E24" s="6">
         <v>21.27972222212702</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -952,14 +945,14 @@
       <c r="C25" s="2">
         <v>45925.550555555557</v>
       </c>
-      <c r="E25" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="D25" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E25" s="6">
         <v>21.226666666567326</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -969,14 +962,14 @@
       <c r="C26" s="2">
         <v>45925.554282407407</v>
       </c>
-      <c r="E26" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F26" s="6">
+      <c r="D26" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E26" s="6">
         <v>21.13722222216893</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -986,14 +979,14 @@
       <c r="C27" s="2">
         <v>45925.567453703705</v>
       </c>
-      <c r="E27" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="D27" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E27" s="6">
         <v>20.821111111028586</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1003,14 +996,14 @@
       <c r="C28" s="2">
         <v>45925.570868055554</v>
       </c>
-      <c r="E28" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F28" s="6">
+      <c r="D28" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E28" s="6">
         <v>20.739166666637175</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1020,14 +1013,14 @@
       <c r="C29" s="2">
         <v>45925.602164351854</v>
       </c>
-      <c r="E29" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F29" s="6">
+      <c r="D29" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E29" s="6">
         <v>19.988055555440951</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1037,14 +1030,14 @@
       <c r="C30" s="2">
         <v>45925.700266203705</v>
       </c>
-      <c r="E30" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F30" s="6">
+      <c r="D30" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E30" s="6">
         <v>17.633611111028586</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1054,14 +1047,14 @@
       <c r="C31" s="2">
         <v>45925.746365740742</v>
       </c>
-      <c r="E31" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F31" s="6">
+      <c r="D31" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E31" s="6">
         <v>16.527222222124692</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1071,14 +1064,14 @@
       <c r="C32" s="2">
         <v>45925.788773148146</v>
       </c>
-      <c r="E32" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F32" s="6">
+      <c r="D32" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E32" s="6">
         <v>15.509444444440305</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1088,14 +1081,14 @@
       <c r="C33" s="2">
         <v>45925.793171296296</v>
       </c>
-      <c r="E33" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F33" s="6">
+      <c r="D33" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E33" s="6">
         <v>15.403888888831716</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1105,10 +1098,10 @@
       <c r="C34" s="2">
         <v>45925.860277777778</v>
       </c>
-      <c r="E34" s="2">
-        <v>45926.434999999998</v>
-      </c>
-      <c r="F34" s="6">
+      <c r="D34" s="2">
+        <v>45926.434999999998</v>
+      </c>
+      <c r="E34" s="6">
         <v>13.793333333276678</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit at 2025-10-17  8:31:07.37
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -286,7 +286,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,8 +627,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -642,229 +641,261 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="D2" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="D3" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
+      <c r="D4" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
+      <c r="D5" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
+      <c r="D6" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
+      <c r="D9" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
+      <c r="D13" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
+      <c r="D14" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
+      <c r="D15" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
+      <c r="D16" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <v>45927.457337962966</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
@@ -873,11 +904,13 @@
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>45935.0465625</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
+      <c r="D18" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
@@ -886,11 +919,13 @@
       <c r="B19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>45943.020914351851</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
+      <c r="D19" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
@@ -899,11 +934,13 @@
       <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>45944.674907407411</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
+      <c r="D20" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
@@ -912,11 +949,13 @@
       <c r="B21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>45945.536215277774</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
+      <c r="D21" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
@@ -925,11 +964,13 @@
       <c r="B22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>45945.603726851848</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+      <c r="D22" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
@@ -938,11 +979,13 @@
       <c r="B23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <v>45946.045289351852</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
+      <c r="D23" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
@@ -951,11 +994,13 @@
       <c r="B24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>45946.1093287037</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
+      <c r="D24" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
@@ -964,11 +1009,13 @@
       <c r="B25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="9">
         <v>45946.16909722222</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
+      <c r="D25" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
@@ -977,11 +1024,13 @@
       <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <v>45946.185879629629</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
+      <c r="D26" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
@@ -990,11 +1039,13 @@
       <c r="B27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <v>45946.228773148148</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
+      <c r="D27" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
@@ -1003,11 +1054,13 @@
       <c r="B28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="9">
         <v>45946.245138888888</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
+      <c r="D28" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
@@ -1016,11 +1069,13 @@
       <c r="B29" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <v>45946.255624999998</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
+      <c r="D29" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
@@ -1029,11 +1084,13 @@
       <c r="B30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>45946.297500000001</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
+      <c r="D30" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
@@ -1042,11 +1099,13 @@
       <c r="B31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="9">
         <v>45946.298530092594</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11"/>
+      <c r="D31" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
@@ -1055,11 +1114,13 @@
       <c r="B32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="9">
         <v>45946.326631944445</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="11"/>
+      <c r="D32" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
@@ -1068,11 +1129,13 @@
       <c r="B33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <v>45946.35597222222</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
+      <c r="D33" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
@@ -1081,11 +1144,13 @@
       <c r="B34" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <v>45946.411979166667</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
+      <c r="D34" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
@@ -1094,11 +1159,13 @@
       <c r="B35" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="9">
         <v>45946.441458333335</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
+      <c r="D35" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
@@ -1107,11 +1174,13 @@
       <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <v>45946.510474537034</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
+      <c r="D36" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
@@ -1120,11 +1189,13 @@
       <c r="B37" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="9">
         <v>45946.545810185184</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
+      <c r="D37" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
@@ -1133,11 +1204,13 @@
       <c r="B38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="9">
         <v>45946.547372685185</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
+      <c r="D38" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
@@ -1146,11 +1219,13 @@
       <c r="B39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="9">
         <v>45946.549641203703</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
+      <c r="D39" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
@@ -1159,11 +1234,13 @@
       <c r="B40" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="9">
         <v>45946.551319444443</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
+      <c r="D40" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
@@ -1172,122 +1249,126 @@
       <c r="B41" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="9">
         <v>45946.554664351854</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
+      <c r="D41" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42" s="15">
         <v>45946.557071759256</v>
       </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="17"/>
+      <c r="D42" s="9">
+        <v>45947.342986111114</v>
+      </c>
+      <c r="E42" s="16"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="11"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="11"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="11"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="11"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="11"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="11"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="11"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="10"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="11"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="10"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="11"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="11"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="11"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Auto commit at 2026-01-22  8:14:11.81
</commit_message>
<xml_diff>
--- a/data/wcdsc.xlsx
+++ b/data/wcdsc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>电站名称</t>
   </si>
@@ -43,76 +43,85 @@
     <t>长沙市开福区高岭香江国际城充电站建设项目</t>
   </si>
   <si>
-    <t>9176699400500205</t>
-  </si>
-  <si>
     <t>9176699400501205</t>
   </si>
   <si>
-    <t>9176699400501304</t>
-  </si>
-  <si>
-    <t>9176699400500105</t>
-  </si>
-  <si>
     <t>9176699400500501</t>
   </si>
   <si>
-    <t>飞狐四方坪南区充电站</t>
-  </si>
-  <si>
-    <t>9176699368200406</t>
-  </si>
-  <si>
-    <t>9176699400500302</t>
-  </si>
-  <si>
     <t>9176699400500502</t>
   </si>
   <si>
-    <t>9176699420300105</t>
-  </si>
-  <si>
-    <t>211号直流</t>
-  </si>
-  <si>
-    <t>304号直流</t>
-  </si>
-  <si>
     <t>106号直流</t>
   </si>
   <si>
     <t>108号直流</t>
   </si>
   <si>
-    <t>9176699400500704</t>
-  </si>
-  <si>
-    <t>9176699400500104</t>
-  </si>
-  <si>
-    <t>9176699400500202</t>
-  </si>
-  <si>
-    <t>9176699368200404</t>
-  </si>
-  <si>
-    <t>9176699400500203</t>
-  </si>
-  <si>
-    <t>9176699368200101</t>
-  </si>
-  <si>
-    <t>9176699400500401</t>
-  </si>
-  <si>
-    <t>9176699400500805</t>
-  </si>
-  <si>
     <t>9176699400501303</t>
   </si>
   <si>
-    <t>9176699400500603</t>
+    <t>105号直流</t>
+  </si>
+  <si>
+    <t>204号直流</t>
+  </si>
+  <si>
+    <t>206号直流</t>
+  </si>
+  <si>
+    <t>110号直流</t>
+  </si>
+  <si>
+    <t>207号直流</t>
+  </si>
+  <si>
+    <t>111号直流</t>
+  </si>
+  <si>
+    <t>9176699355900102</t>
+  </si>
+  <si>
+    <t>9176699400500403</t>
+  </si>
+  <si>
+    <t>9176699400501305</t>
+  </si>
+  <si>
+    <t>9176699442101001</t>
+  </si>
+  <si>
+    <t>9176699400500605</t>
+  </si>
+  <si>
+    <t>9176699400500204</t>
+  </si>
+  <si>
+    <t>9176699425700301</t>
+  </si>
+  <si>
+    <t>9176699400500301</t>
+  </si>
+  <si>
+    <t>9176699400500102</t>
+  </si>
+  <si>
+    <t>9176699400500604</t>
+  </si>
+  <si>
+    <t>9176699400500304</t>
+  </si>
+  <si>
+    <t>9176699400500504</t>
+  </si>
+  <si>
+    <t>9176699400500303</t>
+  </si>
+  <si>
+    <t>9176699442100302</t>
+  </si>
+  <si>
+    <t>9176699400500201</t>
   </si>
 </sst>
 </file>
@@ -523,7 +532,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -557,13 +566,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" s="9">
-        <v>46042.457071759258</v>
+        <v>46043.552719907406</v>
       </c>
       <c r="D2" s="9">
-        <v>46043.307129629633</v>
+        <v>46044.328784722224</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -572,13 +581,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" s="9">
-        <v>46042.458136574074</v>
+        <v>46043.554050925923</v>
       </c>
       <c r="D3" s="9">
-        <v>46043.307129629633</v>
+        <v>46044.328784722224</v>
       </c>
       <c r="E3" s="10"/>
     </row>
@@ -587,13 +596,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C4" s="9">
-        <v>46042.642581018517</v>
+        <v>46043.624456018515</v>
       </c>
       <c r="D4" s="9">
-        <v>46043.307129629633</v>
+        <v>46044.328784722224</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -602,73 +611,73 @@
         <v>7</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" s="9">
-        <v>46042.68377314815</v>
+        <v>46043.649282407408</v>
       </c>
       <c r="D5" s="9">
-        <v>46043.307129629633</v>
+        <v>46044.328784722224</v>
       </c>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6" s="9">
-        <v>46042.248333333337</v>
+        <v>46043.666828703703</v>
       </c>
       <c r="D6" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.328784722224</v>
       </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="9">
-        <v>46042.248935185184</v>
+        <v>46043.706435185188</v>
       </c>
       <c r="D7" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.328784722224</v>
       </c>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C8" s="9">
-        <v>46042.56349537037</v>
+        <v>46043.70853009259</v>
       </c>
       <c r="D8" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.328784722224</v>
       </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="9">
-        <v>46042.568437499998</v>
+        <v>46043.7112037037</v>
       </c>
       <c r="D9" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.328784722224</v>
       </c>
       <c r="E9" s="10"/>
     </row>
@@ -677,13 +686,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" s="9">
-        <v>46042.578611111108</v>
+        <v>46043.112453703703</v>
       </c>
       <c r="D10" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E10" s="10"/>
     </row>
@@ -692,58 +701,58 @@
         <v>5</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C11" s="9">
-        <v>46042.582569444443</v>
+        <v>46043.377685185187</v>
       </c>
       <c r="D11" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" s="9">
-        <v>46042.583460648151</v>
+        <v>46043.565451388888</v>
       </c>
       <c r="D12" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13" s="9">
-        <v>46042.585023148145</v>
+        <v>46043.573854166665</v>
       </c>
       <c r="D13" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" s="9">
-        <v>46042.585578703707</v>
+        <v>46043.576226851852</v>
       </c>
       <c r="D14" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E14" s="10"/>
     </row>
@@ -752,28 +761,28 @@
         <v>5</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="9">
-        <v>46042.591284722221</v>
+        <v>46043.576481481483</v>
       </c>
       <c r="D15" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C16" s="9">
-        <v>46042.591446759259</v>
+        <v>46043.576921296299</v>
       </c>
       <c r="D16" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -782,13 +791,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C17" s="9">
-        <v>46042.59516203704</v>
+        <v>46043.579606481479</v>
       </c>
       <c r="D17" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E17" s="10"/>
     </row>
@@ -797,28 +806,28 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C18" s="9">
-        <v>46042.600057870368</v>
+        <v>46043.5859375</v>
       </c>
       <c r="D18" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C19" s="9">
-        <v>46042.608796296299</v>
+        <v>46043.590740740743</v>
       </c>
       <c r="D19" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E19" s="10"/>
     </row>
@@ -830,10 +839,10 @@
         <v>30</v>
       </c>
       <c r="C20" s="9">
-        <v>46042.61645833333</v>
+        <v>46043.592974537038</v>
       </c>
       <c r="D20" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E20" s="10"/>
     </row>
@@ -842,28 +851,28 @@
         <v>5</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C21" s="9">
-        <v>46042.664502314816</v>
+        <v>46043.593657407408</v>
       </c>
       <c r="D21" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C22" s="9">
-        <v>46042.687280092592</v>
+        <v>46043.595810185187</v>
       </c>
       <c r="D22" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E22" s="10"/>
     </row>
@@ -872,13 +881,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="9">
-        <v>46042.74459490741</v>
+        <v>46043.604733796295</v>
       </c>
       <c r="D23" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E23" s="10"/>
     </row>
@@ -890,39 +899,71 @@
         <v>31</v>
       </c>
       <c r="C24" s="9">
-        <v>46042.7580787037</v>
+        <v>46043.625358796293</v>
       </c>
       <c r="D24" s="9">
-        <v>46043.297743055555</v>
+        <v>46044.310810185183</v>
       </c>
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="9">
+        <v>46043.634027777778</v>
+      </c>
+      <c r="D25" s="9">
+        <v>46044.310810185183</v>
+      </c>
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="9">
+        <v>46043.651747685188</v>
+      </c>
+      <c r="D26" s="9">
+        <v>46044.310810185183</v>
+      </c>
       <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+      <c r="A27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="9">
+        <v>46043.722638888888</v>
+      </c>
+      <c r="D27" s="9">
+        <v>46044.310810185183</v>
+      </c>
       <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
+      <c r="A28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="9">
+        <v>46043.73709490741</v>
+      </c>
+      <c r="D28" s="9">
+        <v>46044.310810185183</v>
+      </c>
       <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>